<commit_message>
Tehtud logi faili, leitud viga õpilaste faili loomisel
</commit_message>
<xml_diff>
--- a/õpetajateFail.xlsx
+++ b/õpetajateFail.xlsx
@@ -373,7 +373,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kayla 252, Jessica 278, Isabella 427, Madison 204, Madison 324, Alexis 370, Abigail 269, Alyssa 4, Lauren 8, Lauren 60, Abigail 490, Olivia 137, Jessica 46, Lauren 96, Emily 144, Brianna 197, Jessica 425, Isabella 485, Brianna 47, Emily 505, Brianna 148, Kayla 497, Grace 320, Alexis 443, Emily 405, Grace 280, Emily 135</t>
+          <t>Alyssa 4, Lauren 8, Kayla 5, Madison 14</t>
         </is>
       </c>
     </row>
@@ -385,7 +385,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Olivia 259, Isabella 426, Emily 229, Taylor 222, Alyssa 435, Ashley 50, Elizabeth 449, Alyssa 306, Elizabeth 476, Lauren 12, Jessica 423, Sarah 210, Ashley 453, Emily 91, Olivia 234, Taylor 215, Abigail 255, Jessica 44, Samantha 150, Grace 351, Samantha 327, Jessica 32, Abigail 125, Lauren 494, Emily 439, Hannah 314, Olivia 53</t>
+          <t>Lauren 12, Lauren 11</t>
         </is>
       </c>
     </row>
@@ -397,7 +397,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jessica 278, Lauren 8, Jessica 46, Brianna 197, Samantha 150, Emily 135, Alyssa 4</t>
+          <t>Lauren 8, Alyssa 4</t>
         </is>
       </c>
     </row>
@@ -409,7 +409,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emma 118, Lauren 363, Elizabeth 516, Alexis 365, Alexis 104, Madison 204, Jessica 206, Lauren 367, Madison 352, Isabella 244, Elizabeth 472, Emily 144, Jessica 23, Elizabeth 486, Jessica 374, Taylor 158, Abigail 406, Elizabeth 262, Ashley 195, Ashley 458, Olivia 451, Elizabeth 364, Abigail 291, Brianna 513, Madison 149, Ashley 283, Alexis 261, Jessica 293, Elizabeth 10, Alyssa 421</t>
+          <t>Elizabeth 10, Emma 9</t>
         </is>
       </c>
     </row>
@@ -421,7 +421,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Emma 118, Lauren 363, Elizabeth 516, Alexis 365, Alexis 104, Madison 204, Jessica 206, Lauren 367, Madison 352, Isabella 244, Elizabeth 472, Emily 144, Jessica 23, Elizabeth 486, Jessica 374, Taylor 158, Abigail 406, Elizabeth 262, Ashley 195, Ashley 458, Olivia 451, Elizabeth 364, Abigail 291, Brianna 513, Madison 149, Ashley 283, Alexis 261, Jessica 293, Elizabeth 10, Alyssa 421</t>
+          <t>Elizabeth 10, Emma 9</t>
         </is>
       </c>
     </row>
@@ -433,7 +433,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Emma 118, Lauren 363, Elizabeth 516, Alexis 365, Alexis 104, Madison 204, Jessica 206, Lauren 367, Madison 352, Isabella 244, Elizabeth 472, Emily 144, Jessica 23, Elizabeth 486, Jessica 374, Taylor 158, Abigail 406, Elizabeth 262, Ashley 195, Ashley 458, Olivia 451, Elizabeth 364, Abigail 291, Brianna 513, Madison 149, Ashley 283, Alexis 261, Jessica 293, Elizabeth 10, Alyssa 421</t>
+          <t>Elizabeth 10, Emma 9</t>
         </is>
       </c>
     </row>
@@ -443,11 +443,7 @@
           <t>Planimeetria alused</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Alyssa 493, Abigail 212, Jessica 383, Olivia 274, Madison 352, Isabella 244, Alyssa 233, Taylor 288, Sarah 501, Hannah 165, Elizabeth 284, Madison 162, Elizabeth 399, Ashley 195, Alyssa 304, Grace 263, Madison 243, Taylor 215, Brianna 513, Grace 159, Grace 321, Abigail 71, Alexis 470, Grace 120, Emma 185, Lauren 494, Hannah 314, Brianna 362, Alexis 468, Lauren 56</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -455,11 +451,7 @@
           <t>3D-modelleerimine 3. periood</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Elizabeth 174, Hannah 218, Abigail 109, Olivia 53, Ashley 140, Lauren 346, Isabella 63, Grace 253, Olivia 451</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -467,11 +459,7 @@
           <t>3D-modelleerimine 5. periood</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Grace 253, Grace 122, Elizabeth 157, Jessica 147, Abigail 105, Abigail 71, Samantha 27, Madison 519, Samantha 20, Grace 463, Taylor 176</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -481,7 +469,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Alyssa 493, Emma 98, Kayla 252, Abigail 108, Alyssa 508, Ashley 123, Taylor 151, Alyssa 4, Lauren 60, Emma 238, Alyssa 19, Emma 216, Alexis 343, Brianna 197, Madison 444, Emily 152, Ashley 326, Lauren 249, Emma 350, Alexis 294, Grace 280, Lauren 170, Elizabeth 328, Jessica 44</t>
+          <t>Alyssa 4, Kayla 5, Madison 14</t>
         </is>
       </c>
     </row>
@@ -493,7 +481,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Isabella 183, Kayla 188, Hannah 218, Elizabeth 227, Emily 91, Alexis 340, Hannah 266, Olivia 124, Samantha 20, Brianna 47, Grace 320, Alexis 294, Madison 196, Samantha 18, Grace 213, Emily 507, Brianna 492, Taylor 145, Alyssa 128, Kayla 268, Alyssa 421, Sarah 86, Brianna 251, Jessica 303</t>
+          <t>Samantha 18</t>
         </is>
       </c>
     </row>
@@ -505,7 +493,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Emma 28, Isabella 426, Ashley 348, Alexis 365, Lauren 90, Madison 324, Alyssa 435, Olivia 1, Madison 173, Taylor 254, Olivia 416, Alexis 381, Olivia 137, Sarah 74, Alyssa 19, Emma 216, Ashley 286, Sarah 501, Jessica 425, Alyssa 432, Ashley 246, Alyssa 339, Ashley 481, Grace 292</t>
+          <t>Olivia 1</t>
         </is>
       </c>
     </row>
@@ -517,7 +505,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Emma 28, Madison 368, Lauren 232, Jessica 206, Abigail 131, Ashley 50, Alexis 335, Isabella 244, Ashley 193, Samantha 211, Isabella 160, Emma 208, Alexis 498, Kayla 188</t>
+          <t>Kayla 5, Isabella 3, Madison 14, Taylor 17, Alyssa 4, Samantha 18</t>
         </is>
       </c>
     </row>
@@ -529,7 +517,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Madison 368, Elizabeth 67</t>
+          <t>Sarah 2, Kayla 15, Lauren 12</t>
         </is>
       </c>
     </row>
@@ -541,7 +529,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Madison 368, Isabella 426, Kayla 139, Taylor 192, Madison 324, Alyssa 4, Isabella 241, Taylor 288, Emma 238, Lauren 85, Sarah 74, Elizabeth 422, Emily 228, Alexis 343, Ashley 140, Ashley 481</t>
+          <t>Alyssa 4</t>
         </is>
       </c>
     </row>
@@ -553,7 +541,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Kayla 252, Alyssa 508, Abigail 212, Grace 465, Ashley 198, Alexis 335, Emily 146, Samantha 211, Isabella 160, Madison 24, Lauren 8, Brianna 88, Ashley 478, Alyssa 308, Jessica 46, Hannah 202, Brianna 361, Elizabeth 262, Lauren 207, Emma 454, Ashley 326, Samantha 73, Samantha 20, Olivia 134, Taylor 26, Olivia 234, Samantha 276, Lauren 372, Elizabeth 328, Brianna 388, Brianna 492, Grace 159, Hannah 182, Grace 411, Isabella 353, Grace 463</t>
+          <t>Lauren 8, Kayla 15</t>
         </is>
       </c>
     </row>
@@ -565,7 +553,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Alexis 365, Grace 465, Taylor 115, Brianna 433, Ashley 50, Elizabeth 449, Emma 208, Isabella 241, Grace 285, Taylor 106, Olivia 237, Alyssa 133, Kayla 469, Grace 48, Lauren 136, Olivia 496, Lauren 356, Lauren 372, Isabella 3, Alyssa 421</t>
+          <t>Isabella 3</t>
         </is>
       </c>
     </row>
@@ -577,7 +565,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Grace 99, Emily 146, Isabella 354, Samantha 211, Lauren 8, Olivia 416, Abigail 408, Taylor 509, Samantha 429, Hannah 397, Hannah 467, Brianna 47, Sarah 114, Emily 403, Madison 196, Brianna 388, Kayla 268, Isabella 329, Samantha 483, Olivia 169</t>
+          <t>Lauren 8, Lauren 11</t>
         </is>
       </c>
     </row>
@@ -587,11 +575,7 @@
           <t>Labortöid füüsikas 10. ja 11. klassile</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Kayla 252, Emma 28, Kayla 139, Lauren 232, Brianna 433, Grace 99, Lauren 33, Abigail 131, Hannah 59, Olivia 274, Taylor 121, Madison 24</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -601,7 +585,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Madison 368, Isabella 342, Elizabeth 67, Elizabeth 174, Alyssa 359, Madison 126, Kayla 13, Samantha 429, Hannah 218, Alyssa 432, Taylor 130, Ashley 246, Hannah 266, Taylor 523, Emma 454, Samantha 73, Samantha 20, Grace 253, Alexis 69, Olivia 451, Olivia 234, Lauren 459, Elizabeth 157, Jessica 293, Jessica 44, Ashley 389, Sarah 86, Brianna 251, Brianna 419, Olivia 21, Samantha 178, Jessica 147, Ashley 392, Sarah 512, Grace 247, Taylor 110, Olivia 167, Kayla 5, Olivia 376, Grace 428, Grace 256, Taylor 176, Lauren 236, Abigail 109, Madison 464</t>
+          <t>Kayla 13</t>
         </is>
       </c>
     </row>
@@ -611,11 +595,7 @@
           <t>Joonestamine 4. periood</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Elizabeth 174, Emma 142, Grace 99, Alyssa 132, Alyssa 366, Isabella 63, Elizabeth 472, Emma 216, Samantha 27, Emma 58, Jessica 425, Olivia 237, Ashley 140, Brianna 438, Lauren 430, Ashley 326, Hannah 467, Grace 122, Alyssa 304, Olivia 496, Lauren 170, Kayla 7, Jessica 189, Brianna 388, Emma 77, Kayla 272, Samantha 178, Abigail 71, Alexis 470, Sarah 424, Grace 463, Isabella 375, Jessica 147, Lauren 346, Emily 439, Alyssa 491, Olivia 53, Emma 387, Samantha 462, Grace 431, Madison 519, Abigail 105, Alexis 104, Ashley 198, Brianna 88</t>
-        </is>
-      </c>
+      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -625,7 +605,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Emma 28, Abigail 212, Emma 142, Brianna 433, Alyssa 435, Isabella 183, Alexis 335, Isabella 241, Alexis 171, Samantha 402, Hannah 218, Elizabeth 422, Taylor 106, Lauren 457, Samantha 27, Ashley 412, Jessica 219, Isabella 295, Grace 253, Taylor 215, Grace 282, Olivia 376, Isabella 275, Isabella 375</t>
+          <t>Hannah 16</t>
         </is>
       </c>
     </row>
@@ -637,7 +617,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Olivia 259, Jessica 278, Brianna 153, Lauren 33, Abigail 131, Emily 146, Elizabeth 476, Samantha 487, Alyssa 233, Hannah 194, Samantha 271, Sarah 74, Brianna 197, Olivia 237, Taylor 130, Hannah 266, Kayla 235, Olivia 40, Emma 72, Lauren 249, Brianna 148, Lauren 489, Hannah 287, Alexis 261</t>
+          <t>Kayla 7, Kayla 13</t>
         </is>
       </c>
     </row>
@@ -649,7 +629,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Kayla 252, Elizabeth 67, Samantha 302, Jessica 191, Emma 142, Jessica 383, Ashley 198, Samantha 211, Emily 37, Lauren 360, Alexis 381, Lauren 49, Jessica 506, Kayla 15, Alexis 316, Emily 390, Jessica 521, Alexis 45, Olivia 237, Isabella 485, Hannah 266, Ashley 81, Grace 292, Grace 267, Samantha 20</t>
+          <t>Kayla 15</t>
         </is>
       </c>
     </row>
@@ -661,7 +641,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Isabella 426, Isabella 342, Isabella 427, Jessica 191, Elizabeth 436, Ashley 50, Emily 37, Samantha 143, Alexis 381, Ashley 453, Olivia 237, Ashley 246, Isabella 485, Alyssa 133, Brianna 456, Emma 290, Olivia 234, Brianna 148, Elizabeth 157, Abigail 255, Hannah 287, Emily 507</t>
+          <t>Kayla 7</t>
         </is>
       </c>
     </row>
@@ -673,7 +653,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Alyssa 493, Elizabeth 516, Ashley 123, Ashley 50, Olivia 103, Brianna 221, Taylor 121, Emma 208, Alyssa 233, Isabella 241, Olivia 102, Emily 390, Ashley 286, Lauren 207, Grace 263, Olivia 451, Kayla 379, Elizabeth 157, Sarah 114, Lauren 356, Ashley 389, Abigail 517, Grace 351, Olivia 318, Abigail 296, Samantha 386, Grace 321, Elizabeth 307, Samantha 250</t>
+          <t>Emma 9</t>
         </is>
       </c>
     </row>
@@ -685,7 +665,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Sarah 518, Emma 118, Jessica 437, Elizabeth 436, Madison 324, Jessica 206, Alexis 370, Isabella 244, Taylor 288, Alexis 471, Alexis 62, Brianna 203, Grace 199, Emma 401, Kayla 15, Alexis 316, Olivia 345, Taylor 158, Elizabeth 262, Elizabeth 289, Emma 454, Elizabeth 284, Ashley 481, Brianna 47, Grace 320, Brianna 513, Emily 403, Elizabeth 328, Jessica 189, Emma 77, Samantha 327, Lauren 258, Isabella 329, Samantha 483, Ashley 220, Olivia 214, Olivia 376, Alexis 470, Samantha 250, Brianna 418, Abigail 125, Hannah 314, Emma 300, Olivia 53, Hannah 281, Olivia 477, Madison 415, Abigail 341, Brianna 179, Abigail 177</t>
+          <t>Kayla 15, Kayla 5</t>
         </is>
       </c>
     </row>
@@ -697,7 +677,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Alexis 104, Elizabeth 436, Alexis 378, Lauren 367, Lauren 475, Isabella 354, Elizabeth 391, Taylor 254, Alyssa 306, Samantha 487, Emily 445, Abigail 408, Alyssa 39, Kayla 15, Samantha 27, Emily 336, Elizabeth 227, Taylor 158, Abigail 406, Abigail 279, Madison 444, Madison 155, Lauren 207, Emily 152, Sarah 434</t>
+          <t>Kayla 15, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -709,7 +689,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Emma 28, Abigail 108, Jessica 191, Abigail 413, Lauren 248, Isabella 183, Kayla 407, Taylor 6, Jessica 423, Lauren 457, Olivia 345, Jessica 374, Ashley 117, Emily 91, Alexis 340, Grace 267, Taylor 26, Brianna 492, Elizabeth 10, Lauren 358, Hannah 317, Abigail 296, Elizabeth 79, Grace 83, Sarah 424, Taylor 394, Isabella 375, Emma 404</t>
+          <t>Taylor 6, Elizabeth 10</t>
         </is>
       </c>
     </row>
@@ -721,7 +701,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Madison 204, Taylor 115, Ashley 50, Ashley 193, Taylor 121, Alyssa 359, Emily 37, Grace 100, Alexis 381, Ashley 453, Olivia 41, Abigail 279, Isabella 485, Madison 155, Grace 267, Olivia 124, Grace 48, Brianna 299, Samantha 68, Hannah 181, Taylor 26, Alyssa 304, Lauren 372, Samantha 150, Emily 97, Olivia 169, Samantha 386, Samantha 178, Sarah 424, Isabella 375, Jessica 311, Hannah 332, Alyssa 491, Ashley 84, Jessica 70, Grace 431, Olivia 127, Elizabeth 116, Samantha 398, Grace 465, Lauren 337, Abigail 406, Olivia 21, Brianna 201, Samantha 302, Taylor 110, Lauren 170, Emily 333, Ashley 392, Grace 22</t>
+          <t>Hannah 16, Isabella 3</t>
         </is>
       </c>
     </row>
@@ -731,11 +711,7 @@
           <t>Astronoomia</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Jessica 461, Sarah 331, Alyssa 493, Abigail 108, Elizabeth 67, Taylor 151, Brianna 172, Lauren 60, Ashley 240, Lauren 85, Hannah 194, Alexis 381, Abigail 408, Lauren 96, Emma 216, Alyssa 273, Samantha 429, Brianna 197, Ashley 412, Lauren 207, Alyssa 339, Lauren 310, Kayla 469, Madison 162, Grace 253, Brianna 47, Brianna 180, Lauren 459, Kayla 379, Alexis 294</t>
-        </is>
-      </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -743,11 +719,7 @@
           <t>Astrofüüsika 2. periood</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Emma 25, Olivia 259, Brianna 153, Emily 334, Grace 99, Lauren 33, Madison 54, Ashley 123, Samantha 211, Abigail 338, Emily 37, Emma 238, Alexis 471, Hannah 194, Brianna 201, Samantha 402, Olivia 102, Emma 401, Alyssa 273, Hannah 202, Elizabeth 385, Ashley 453, Emily 479, Brianna 456, Ashley 81, Emma 290, Jessica 219, Alexis 355, Kayla 466, Elizabeth 328, Grace 213, Olivia 138, Brianna 388, Sarah 442, Abigail 231</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -757,7 +729,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Alexis 35, Abigail 108, Taylor 192, Alexis 104, Lauren 248, Alyssa 132, Kayla 407, Elizabeth 476, Lauren 360, Lauren 49, Hannah 397, Taylor 130, Hannah 266, Alyssa 304, Emma 72, Lauren 29, Taylor 215, Grace 320, Alexis 294, Madison 149, Hannah 287, Grace 22, Abigail 503, Sarah 86, Abigail 296, Samantha 483, Ashley 220, Elizabeth 43, Sarah 424, Isabella 95, Brianna 373, Kayla 5, Lauren 236, Samantha 484, Abigail 341</t>
+          <t>Kayla 5, Emma 9</t>
         </is>
       </c>
     </row>
@@ -769,7 +741,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Elizabeth 67, Jessica 278, Jessica 191, Madison 204, Elizabeth 436, Emma 142, Brianna 153, Jessica 206, Isabella 183, Alexis 370, Olivia 103, Taylor 151, Taylor 121, Alyssa 4, Alyssa 359, Elizabeth 449, Alyssa 233, Grace 199, Abigail 408, Sarah 210</t>
+          <t>Alyssa 4, Lauren 11</t>
         </is>
       </c>
     </row>
@@ -779,11 +751,7 @@
           <t>Loogika 2. periood</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Emma 98, Emily 229, Ashley 78, Jessica 206, Ashley 198, Alexis 335, Brianna 221, Isabella 63, Ashley 240, Lauren 360, Sarah 210, Taylor 509, Hannah 323, Hannah 397, Samantha 480, Olivia 40, Jessica 265, Kayla 379, Olivia 239, Abigail 517, Samantha 327, Kayla 268, Olivia 214, Brianna 92, Brianna 200, Abigail 450, Hannah 129, Jessica 230, Emily 349, Olivia 264, Ashley 168</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -793,7 +761,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sarah 331, Madison 204, Brianna 153, Lauren 33, Alexis 378, Lauren 475, Abigail 490, Jessica 423, Hannah 194, Sarah 2, Samantha 402, Elizabeth 262, Ashley 246, Alyssa 133, Alexis 355, Ashley 441, Lauren 459, Alyssa 440, Alexis 261, Abigail 344, Ashley 414, Grace 120, Emma 404, Emma 55, Elizabeth 141, Hannah 314, Lauren 337, Alexis 80, Isabella 187, Taylor 192, Brianna 513</t>
+          <t>Sarah 2</t>
         </is>
       </c>
     </row>
@@ -803,11 +771,7 @@
           <t>Programmeerimine keeles Java 1</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Hannah 314, Emily 405, Emily 135, Brianna 47, Isabella 485</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -825,7 +789,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Lauren 52, Alexis 365, Olivia 504, Isabella 244, Brianna 172, Olivia 416, Brianna 203, Sarah 74, Lauren 96, Elizabeth 422, Taylor 106, Jessica 23, Lauren 457, Grace 396, Brianna 361, Kayla 469, Olivia 134, Emily 505, Emily 405, Abigail 255, Samantha 327, Grace 282, Olivia 214, Jessica 32, Ashley 510, Elizabeth 473, Abigail 109, Madison 301, Lauren 494, Sarah 277</t>
+          <t>Kayla 5</t>
         </is>
       </c>
     </row>
@@ -837,7 +801,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Madison 368, Abigail 108, Alexis 365, Isabella 427, Emma 142, Hannah 59, Olivia 103, Taylor 151, Elizabeth 391, Alyssa 366, Isabella 63, Emma 238, Brianna 88, Alexis 171, Lauren 49, Olivia 102, Alyssa 19, Alyssa 39, Lauren 457, Madison 225, Kayla 51, Emily 390, Jessica 425, Ashley 246, Lauren 430, Ashley 195, Olivia 502, Brianna 180, Taylor 215, Abigail 291, Kayla 369, Alexis 443, Emma 350, Alexis 294, Isabella 474, Grace 428, Elizabeth 307, Sarah 420, Ashley 510, Emma 305, Elizabeth 473, Emma 185, Olivia 186, Sarah 512, Olivia 270, Alexis 80, Kayla 75, Madison 322, Brianna 438, Sarah 156</t>
+          <t>Elizabeth 10, Alyssa 4</t>
         </is>
       </c>
     </row>
@@ -849,7 +813,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Elizabeth 67, Alyssa 508, Alyssa 435, Isabella 183, Emily 87, Isabella 160, Abigail 338, Madison 173, Samantha 143, Lauren 12, Alyssa 308, Madison 126, Lauren 452, Elizabeth 472, Samantha 429, Hannah 218, Elizabeth 385, Grace 396, Alexis 343, Ashley 286, Alyssa 432, Alexis 340, Alyssa 339, Hannah 467, Samantha 480, Ashley 458, Madison 243, Lauren 459, Emily 405, Ashley 283, Abigail 255, Jessica 293, Kayla 272, Grace 282, Isabella 353, Taylor 394, Madison 301, Jessica 230, Jessica 175, Emma 387, Lauren 11, Kayla 409, Sarah 315, Jessica 163, Abigail 82, Sarah 107, Emma 9, Elizabeth 166, Olivia 167, Olivia 1</t>
+          <t>Lauren 12, Lauren 11, Emma 9, Sarah 2, Olivia 1</t>
         </is>
       </c>
     </row>
@@ -859,11 +823,7 @@
           <t>Arvutite riistvara ja lisaseadmed</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Emily 229, Emily 334, Abigail 131, Alexis 370, Madison 173, Taylor 288, Emma 401, Alyssa 273, Alexis 316, Emma 454, Isabella 161, Alexis 69, Taylor 26, Brianna 180, Alyssa 380, Hannah 119</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -871,11 +831,7 @@
           <t>Loodusteadused, tehnoloogia ja ühiskond</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Lauren 90, Elizabeth 436, Emily 146, Emily 87, Samantha 211, Isabella 160, Taylor 254, Elizabeth 476, Lauren 60, Emily 445, Emma 238, Lauren 452, Sarah 377, Olivia 137, Emily 144, Emily 228, Elizabeth 385, Jessica 521, Hannah 165, Emily 152, Taylor 215, Samantha 298, Brianna 205, Grace 280, Brianna 419</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -885,7 +841,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Brianna 61, Alexis 35, Emily 334, Ashley 193, Alexis 471, Alyssa 308, Madison 126, Lauren 49, Samantha 429, Taylor 158, Alyssa 432, Taylor 130, Isabella 485, Madison 155, Emma 290, Jessica 219, Alexis 69, Madison 243, Olivia 234, Elizabeth 364, Isabella 347, Ashley 283, Sarah 156, Samantha 483, Olivia 21, Alyssa 245, Taylor 394</t>
+          <t>Hannah 16, Olivia 1</t>
         </is>
       </c>
     </row>
@@ -897,7 +853,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Brianna 61, Ashley 78, Jessica 66, Lauren 248, Emily 330, Taylor 6, Alyssa 233, Grace 100, Kayla 188, Emma 499, Abigail 490, Sarah 400, Lauren 452, Brianna 201, Ashley 460, Kayla 51, Olivia 41, Hannah 165</t>
+          <t>Taylor 6</t>
         </is>
       </c>
     </row>
@@ -909,7 +865,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Brianna 61, Ashley 78, Jessica 66, Lauren 248, Emily 330, Taylor 6, Alyssa 233, Grace 100, Kayla 188, Emma 499, Abigail 490, Sarah 400, Lauren 452, Brianna 201, Ashley 460, Kayla 51, Olivia 41, Hannah 165</t>
+          <t>Taylor 6</t>
         </is>
       </c>
     </row>
@@ -921,7 +877,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Brianna 61, Ashley 78, Jessica 66, Lauren 248, Emily 330, Taylor 6, Alyssa 233, Grace 100, Kayla 188, Emma 499, Abigail 490, Sarah 400, Lauren 452, Brianna 201, Ashley 460, Kayla 51, Olivia 41, Hannah 165</t>
+          <t>Taylor 6</t>
         </is>
       </c>
     </row>
@@ -931,11 +887,7 @@
           <t>Kirjandus ja film</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Sarah 331, Elizabeth 516, Lauren 90, Emily 330, Grace 100, Olivia 416, Kayla 188, Alexis 62, Samantha 143, Alyssa 308, Sarah 400, Alexis 171, Elizabeth 472, Alyssa 19, Alexis 316, Emily 390, Olivia 41, Kayla 235, Isabella 161, Abigail 291, Kayla 369, Emma 350, Sarah 114, Emily 403, Madison 149, Abigail 255, Lauren 170, Sarah 156, Emma 77, Kayla 272, Hannah 357, Grace 282, Kayla 495, Olivia 169</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -945,7 +897,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Brianna 61, Lauren 363, Ashley 348, Samantha 302, Isabella 395, Emma 142, Olivia 504, Hannah 59, Elizabeth 476, Brianna 203, Alexis 381, Samantha 271, Jessica 506, Jessica 23, Elizabeth 486, Jessica 521, Elizabeth 289, Ashley 412, Olivia 502, Lauren 249, Isabella 347, Alexis 524, Grace 511</t>
+          <t>Emma 9</t>
         </is>
       </c>
     </row>
@@ -957,7 +909,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Emma 118, Taylor 192, Lauren 232, Madison 24, Alyssa 366, Alexis 498, Taylor 226, Lauren 85, Lauren 12, Lauren 452, Sarah 2, Sarah 74, Madison 319, Elizabeth 422, Sarah 31, Alexis 343, Brianna 361, Elizabeth 262, Ashley 140, Emily 65</t>
+          <t>Lauren 12, Sarah 2, Hannah 16</t>
         </is>
       </c>
     </row>
@@ -969,7 +921,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Jessica 437, Kayla 139, Taylor 222, Alyssa 435, Olivia 103, Brianna 172, Isabella 160, Brianna 88, Emma 499, Grace 199, Emma 58, Alexis 45, Ashley 481, Hannah 467, Brianna 180, Hannah 119, Alexis 294, Isabella 474, Lauren 93, Alexis 261</t>
+          <t>Lauren 11</t>
         </is>
       </c>
     </row>
@@ -981,7 +933,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Sarah 518, Emma 98, Abigail 212, Emma 142, Isabella 183, Lauren 8, Alyssa 308, Jessica 46, Emma 401, Alyssa 19, Kayla 13, Elizabeth 385, Samantha 27, Emily 390, Olivia 124, Samantha 20</t>
+          <t>Lauren 8, Kayla 13, Isabella 3, Kayla 7</t>
         </is>
       </c>
     </row>
@@ -1001,7 +953,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Emma 25, Isabella 342, Jessica 278, Taylor 192, Abigail 269, Abigail 338, Madison 173, Emily 37, Alexis 498, Lauren 360, Taylor 509, Grace 396, Ashley 286, Abigail 279, Taylor 130, Madison 444</t>
+          <t>Madison 14, Taylor 17, Kayla 5</t>
         </is>
       </c>
     </row>
@@ -1019,11 +971,7 @@
           <t>Lähis-Ida 20. sajandi teisest poolest tänapäevani</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Lauren 52, Samantha 302, Lauren 90, Madison 324, Brianna 221, Alyssa 359, Emma 238, Brianna 88, Lauren 49, Emily 228, Lauren 457, Olivia 345, Madison 225, Alexis 45, Alyssa 432, Jessica 219, Kayla 235, Alexis 355, Emma 72, Grace 280, Grace 213, Taylor 145, Hannah 357, Olivia 214, Grace 321, Brianna 42, Grace 428, Emma 55, Jessica 230, Lauren 346, Alexis 371, Emma 217, Brianna 362, Grace 515, Alexis 468, Olivia 127</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1033,7 +981,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Madison 368, Alexis 35, Emily 334, Jessica 383, Madison 54, Olivia 103, Isabella 241, Olivia 416, Samantha 143, Madison 126, Sarah 2, Hannah 218, Hannah 397, Sarah 501, Jessica 520, Elizabeth 289, Olivia 237, Isabella 485, Emily 65, Ashley 481, Olivia 40, Lauren 29, Lauren 249, Grace 320, Emma 257, Hannah 119, Samantha 298, Emily 403, Lauren 356, Sarah 156, Kayla 272, Brianna 492</t>
+          <t>Sarah 2</t>
         </is>
       </c>
     </row>
@@ -1045,7 +993,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Isabella 395, Grace 465, Alexis 378, Olivia 1, Alyssa 366, Lauren 309, Brianna 203, Grace 285, Grace 199, Sarah 377, Olivia 102, Hannah 202, Olivia 384, Emily 336, Elizabeth 227, Emily 479, Ashley 117, Sarah 434, Elizabeth 399, Grace 263</t>
+          <t>Olivia 1</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1005,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Isabella 395, Grace 465, Alexis 378, Olivia 1, Alyssa 366, Lauren 309, Brianna 203, Grace 285, Grace 199, Sarah 377, Olivia 102, Hannah 202, Olivia 384, Emily 336, Elizabeth 227, Emily 479, Ashley 117, Sarah 434, Elizabeth 399, Grace 263</t>
+          <t>Olivia 1</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1017,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Isabella 395, Grace 465, Alexis 378, Olivia 1, Alyssa 366, Lauren 309, Brianna 203, Grace 285, Grace 199, Sarah 377, Olivia 102, Hannah 202, Olivia 384, Emily 336, Elizabeth 227, Emily 479, Ashley 117, Sarah 434, Elizabeth 399, Grace 263</t>
+          <t>Olivia 1</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1029,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Jessica 437, Elizabeth 174, Hannah 522, Olivia 504, Alyssa 132, Emily 87, Taylor 254, Emma 208, Isabella 63, Alexis 471, Alexis 62, Ashley 478, Samantha 271, Madison 319, Hannah 323, Sarah 31, Madison 155, Lauren 430, Grace 48, Samantha 68, Olivia 502, Jessica 265, Emily 505, Kayla 466, Samantha 18</t>
+          <t>Samantha 18</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1041,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Jessica 437, Elizabeth 174, Hannah 522, Olivia 504, Alyssa 132, Emily 87, Taylor 254, Emma 208, Isabella 63, Alexis 471, Alexis 62, Ashley 478, Samantha 271, Madison 319, Hannah 323, Sarah 31, Madison 155, Lauren 430, Grace 48, Samantha 68, Olivia 502, Jessica 265, Emily 505, Kayla 466, Samantha 18</t>
+          <t>Samantha 18</t>
         </is>
       </c>
     </row>
@@ -1105,7 +1053,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Jessica 437, Elizabeth 174, Hannah 522, Olivia 504, Alyssa 132, Emily 87, Taylor 254, Emma 208, Isabella 63, Alexis 471, Alexis 62, Ashley 478, Samantha 271, Madison 319, Hannah 323, Sarah 31, Madison 155, Lauren 430, Grace 48, Samantha 68, Olivia 502, Jessica 265, Emily 505, Kayla 466, Samantha 18</t>
+          <t>Samantha 18</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1065,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alyssa 508, Jessica 191, Abigail 413, Ashley 198, Ashley 123, Alexis 370, Alexis 335, Emily 146, Lauren 475, Isabella 354, Ashley 193, Alyssa 4, Elizabeth 391, Samantha 487, Jessica 506, Kayla 15, Emma 58, Brianna 361</t>
+          <t>Alyssa 4, Kayla 15, Hannah 16</t>
         </is>
       </c>
     </row>
@@ -1127,11 +1075,7 @@
           <t>Ajakirjanduse alused</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Sarah 331, Kayla 139, Emily 330, Abigail 131, Ashley 193, Kayla 188, Ashley 460, Elizabeth 472, Elizabeth 422, Jessica 23, Olivia 345, Taylor 158, Hannah 165, Alyssa 133, Madison 444, Madison 155, Lauren 430, Kayla 469, Elizabeth 284, Isabella 161, Lauren 459, Lauren 136, Olivia 496, Abigail 255, Olivia 239, Alexis 261, Jessica 293, Jessica 44, Jessica 189, Alyssa 128, Kayla 410</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1141,7 +1085,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Emma 118, Samantha 302, Emily 229, Ashley 78, Taylor 115, Olivia 504, Emily 87, Abigail 338, Emma 208, Emily 445, Taylor 288, Ashley 240, Grace 285, Jessica 423, Sarah 377, Taylor 106, Lauren 457, Ashley 453, Emma 58, Emily 390, Abigail 406, Ashley 81, Lauren 310, Emily 505, Brianna 148, Lauren 489, Lauren 93, Samantha 18, Emily 507, Lauren 258</t>
+          <t>Hannah 16, Samantha 18</t>
         </is>
       </c>
     </row>
@@ -1151,11 +1095,7 @@
           <t>Filosoofia 2</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Emma 208, Emily 445, Taylor 106, Emma 58, Lauren 93, Emily 507, Lauren 310</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1165,7 +1105,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Sarah 518, Madison 368, Lauren 363, Brianna 433, Jessica 383, Samantha 143, Samantha 271, Madison 319, Emma 401, Jessica 506, Alyssa 39, Olivia 384, Madison 225, Jessica 520, Ashley 412, Sarah 434, Taylor 17, Isabella 295</t>
+          <t>Kayla 7, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1117,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Sarah 518, Madison 368, Lauren 363, Brianna 433, Jessica 383, Samantha 143, Samantha 271, Madison 319, Emma 401, Jessica 506, Alyssa 39, Olivia 384, Madison 225, Jessica 520, Ashley 412, Sarah 434, Taylor 17, Isabella 295</t>
+          <t>Kayla 7, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1129,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Alyssa 493, Emma 98, Lauren 33, Ashley 123, Ashley 50, Lauren 367, Lauren 475, Isabella 244, Isabella 354, Lauren 12, Sarah 400, Lauren 96, Taylor 509, Jessica 374, Abigail 279, Alexis 340, Hannah 467, Brianna 180, Elizabeth 364, Lauren 249, Emma 257, Hannah 119, Kayla 379, Isabella 474, Kayla 272, Emily 97</t>
+          <t>Lauren 12, Taylor 6</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1141,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Lauren 52, Brianna 61, Isabella 427, Isabella 395, Hannah 522, Abigail 269, Alyssa 306, Lauren 60, Samantha 487, Alexis 62, Abigail 490, Madison 126, Hannah 194, Sarah 2, Brianna 201, Samantha 429, Hannah 323, Olivia 41</t>
+          <t>Sarah 2, Isabella 3, Elizabeth 10, Madison 14</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1153,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Jessica 461, Jessica 437, Elizabeth 516, Abigail 413, Emily 334, Alexis 378, Olivia 274, Madison 352, Brianna 221, Brianna 172, Elizabeth 391, Isabella 241, Alexis 498, Alexis 471, Lauren 309, Emma 499</t>
+          <t>Kayla 13</t>
         </is>
       </c>
     </row>
@@ -1223,11 +1163,7 @@
           <t>Fotograafia 1</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Alexis 35, Abigail 413, Brianna 153, Lauren 475, Isabella 160, Emily 445, Taylor 226, Alyssa 308, Lauren 49, Lauren 96, Jessica 506, Sarah 501, Jessica 425, Jessica 520, Ashley 481, Kayla 235, Alexis 355, Samantha 20, Olivia 134, Hannah 181, Samantha 480, Madison 243, Lauren 459, Kayla 497</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1235,11 +1171,7 @@
           <t>Inimene ja ühiskond 3. periood</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Taylor 192, Jessica 383, Taylor 121, Abigail 338, Elizabeth 391, Samantha 487, Madison 126, Jessica 423, Olivia 137, Emily 91, Ashley 81, Emily 65, Brianna 299, Emma 72, Kayla 369, Grace 320, Emma 77, Kayla 272, Ashley 389, Lauren 258, Grace 159, Kayla 495, Samantha 488, Ashley 392, Jessica 230, Brianna 373, Jessica 163, Abigail 82, Lauren 56, Taylor 94, Emma 64, Lauren 337, Lauren 11, Ashley 198, Olivia 270, Hannah 194</t>
-        </is>
-      </c>
+      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1249,7 +1181,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Emma 25, Taylor 222, Madison 24, Lauren 12, Elizabeth 289, Kayla 379, Lauren 93, Jessica 189, Jessica 32, Isabella 95, Emma 404, Abigail 125, Lauren 494, Alexis 371, Alyssa 491, Olivia 53, Elizabeth 313, Hannah 281, Madison 415, Taylor 110, Brianna 179, Lauren 223, Elizabeth 116, Emma 9, Madison 417, Emily 349, Lauren 236, Olivia 318, Sarah 277, Elizabeth 307, Alyssa 440, Lauren 372, Samantha 382, Ashley 441, Abigail 209, Samantha 462</t>
+          <t>Lauren 12</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1193,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Jessica 278, Lauren 90, Abigail 269, Kayla 407, Alyssa 359, Madison 225, Ashley 140, Brianna 438, Kayla 469, Madison 162, Grace 122, Alyssa 304, Olivia 40, Lauren 29, Lauren 136, Samantha 276, Olivia 239, Grace 213, Isabella 3, Alyssa 128, Lauren 358, Kayla 410, Hannah 317, Brianna 251, Brianna 419, Alyssa 245, Taylor 394, Sarah 442, Isabella 242, Brianna 200</t>
+          <t>Isabella 3</t>
         </is>
       </c>
     </row>
@@ -1273,7 +1205,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Kayla 252, Isabella 426, Jessica 437, Abigail 413, Isabella 395, Brianna 153, Alexis 378, Lauren 475, Brianna 221, Abigail 338, Elizabeth 391, Taylor 254, Elizabeth 476, Lauren 12, Sarah 400, Jessica 46, Jessica 506, Kayla 15, Alexis 316, Sarah 31, Lauren 457, Samantha 27, Emily 390, Brianna 361, Emily 91, Abigail 279, Hannah 266, Madison 444, Lauren 207, Emily 65</t>
+          <t>Lauren 12, Kayla 15, Lauren 11, Elizabeth 10</t>
         </is>
       </c>
     </row>
@@ -1283,11 +1215,7 @@
           <t>Turundus</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Jessica 461, Lauren 52, Olivia 259, Ashley 348, Lauren 232, Lauren 33, Hannah 59, Brianna 221, Ashley 240, Brianna 88, Alyssa 39, Emily 390, Alyssa 432, Taylor 130, Emily 97, Abigail 503, Ashley 220, Jessica 303, Abigail 71, Emma 305, Grace 411, Alexis 470, Madison 301, Jessica 311, Elizabeth 141, Lauren 346</t>
-        </is>
-      </c>
+      <c r="E79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1297,7 +1225,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Sarah 518, Sarah 331, Olivia 274, Elizabeth 449, Elizabeth 476, Lauren 85, Sarah 74, Kayla 13, Grace 396, Alexis 45, Elizabeth 284, Taylor 17, Samantha 73, Emma 257, Samantha 298, Lauren 489, Lauren 356, Abigail 517, Olivia 21, Grace 428, Samantha 250, Grace 120, Abigail 109, Jessica 147</t>
+          <t>Kayla 13, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1237,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Emma 25, Isabella 426, Emma 118, Jessica 437, Abigail 108, Alyssa 508, Lauren 248, Isabella 395, Taylor 222, Elizabeth 449, Grace 100, Taylor 226, Lauren 85, Lauren 12, Grace 199, Abigail 408, Hannah 202, Kayla 15, Elizabeth 486, Alexis 343</t>
+          <t>Lauren 12, Kayla 15, Lauren 11, Elizabeth 10, Isabella 3</t>
         </is>
       </c>
     </row>
@@ -1319,11 +1247,7 @@
           <t>Kujutav geomeetria</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Emma 98, Kayla 252, Hannah 59, Isabella 354, Madison 173, Taylor 288, Ashley 478, Sarah 400, Taylor 509, Alyssa 273, Ashley 453, Jessica 374, Abigail 406, Elizabeth 289, Madison 444, Ashley 81, Kayla 235, Madison 162, Grace 253, Ashley 195, Hannah 181, Olivia 502</t>
-        </is>
-      </c>
+      <c r="E82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1331,11 +1255,7 @@
           <t>Loominguline joonistamine 2</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Samantha 302, Alexis 381</t>
-        </is>
-      </c>
+      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1345,7 +1265,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Ashley 348, Emily 229, Jessica 66, Taylor 115, Jessica 206, Madison 24, Lauren 309, Grace 285, Sarah 210, Kayla 13, Hannah 323, Abigail 279, Taylor 523, Elizabeth 284, Samantha 73, Isabella 161, Ashley 458, Emma 72, Brianna 180, Lauren 249, Abigail 291, Emily 403, Hannah 287, Grace 159, Grace 511, Hannah 317, Olivia 169, Samantha 488, Grace 83, Isabella 353, Abigail 231, Brianna 200, Alexis 36, Isabella 260, Sarah 57</t>
+          <t>Kayla 13, Taylor 6, Madison 14</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1277,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Emma 28, Jessica 278, Taylor 115, Grace 99, Ashley 123, Alexis 370, Elizabeth 391, Alyssa 359, Lauren 60, Jessica 423, Sarah 210, Lauren 96, Kayla 13, Alyssa 273, Samantha 429, Hannah 397, Lauren 457, Grace 396, Brianna 361, Sarah 501, Abigail 279, Elizabeth 284, Samantha 73, Brianna 299, Hannah 181, Samantha 480, Olivia 234, Lauren 459, Alyssa 440, Alyssa 380, Emily 403, Ashley 297, Lauren 372, Kayla 7, Sarah 86, Samantha 224</t>
+          <t>Kayla 13, Lauren 11, Kayla 7</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1289,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Lauren 232, Lauren 90, Emily 334, Alyssa 435, Brianna 221, Lauren 8, Elizabeth 476, Samantha 487, Hannah 194, Abigail 408, Emma 401, Jessica 520, Brianna 438, Taylor 523, Emma 454</t>
+          <t>Lauren 8, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1301,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Abigail 212, Brianna 433, Brianna 153, Abigail 269, Isabella 160, Abigail 338, Emily 445, Samantha 143, Sarah 2, Olivia 137, Samantha 402, Taylor 130, Ashley 246, Ashley 412, Alyssa 339, Lauren 310, Jessica 219, Grace 122, Alyssa 128, Abigail 517, Hannah 317, Brianna 251, Brianna 42, Abigail 109</t>
+          <t>Sarah 2, Madison 14</t>
         </is>
       </c>
     </row>
@@ -1393,7 +1313,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Alyssa 493, Ashley 50, Emily 146, Olivia 103, Taylor 226, Hannah 218, Alexis 340, Emma 290, Emily 65, Emily 152, Kayla 469, Hannah 467, Hannah 119, Isabella 474, Abigail 255, Hannah 287, Samantha 150, Hannah 357, Samantha 327, Grace 282, Kayla 495, Olivia 169, Samantha 386, Ashley 414, Emma 305, Elizabeth 473, Emma 185, Ashley 392, Hannah 129, Lauren 346, Emma 448, Emily 349, Kayla 5, Olivia 186, Ashley 168, Lauren 101, Taylor 500, Kayla 409, Olivia 264, Brianna 492, Taylor 176, Isabella 347, Brianna 92, Brianna 172, Kayla 410, Brianna 47, Alexis 294, Jessica 311, Elizabeth 164, Brianna 205, Abigail 82, Alyssa 245, Emma 72, Sarah 518, Madison 444, Isabella 161, Grace 463, Sarah 420, Kayla 272, Emily 135, Lauren 489, Olivia 138, Kayla 497, Grace 159, Brianna 197, Abigail 344, Sarah 114, Emma 216, Brianna 419, Hannah 332, Kayla 75, Elizabeth 157, Emily 405, Abigail 108, Isabella 375, Madison 455, Sarah 482, Alyssa 19, Elizabeth 385, Lauren 258</t>
+          <t>Kayla 5</t>
         </is>
       </c>
     </row>
@@ -1403,11 +1323,7 @@
           <t>Riigikaitse 2</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Taylor 226, Hannah 218, Samantha 150, Olivia 169, Samantha 386, Hannah 119, Emma 185, Brianna 47, Alexis 294, Ashley 414, Ashley 392, Lauren 346, Hannah 467, Elizabeth 157, Emily 349, Kayla 272, Sarah 420, Abigail 344, Emily 152, Olivia 138, Emily 135</t>
-        </is>
-      </c>
+      <c r="E89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1417,7 +1333,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Lauren 52, Emily 229, Abigail 413, Lauren 33, Isabella 183, Hannah 59, Olivia 274, Kayla 407, Taylor 121, Madison 173, Alyssa 306, Alexis 498, Brianna 88, Alyssa 308, Jessica 46, Taylor 106, Olivia 345, Emma 58, Madison 225, Ashley 286, Emily 91, Jessica 425, Alyssa 432, Brianna 456, Lauren 207</t>
+          <t>Isabella 3, Hannah 16</t>
         </is>
       </c>
     </row>
@@ -1427,11 +1343,7 @@
           <t>Ajakirjanduse praktika</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Emily 229, Emily 330, Ashley 460, Jessica 23, Sarah 501, Taylor 523, Samantha 73, Abigail 255, Grace 511, Hannah 317, Alexis 36, Samantha 488, Brianna 492, Jessica 189, Brianna 200, Isabella 161, Lauren 309, Emma 257, Elizabeth 284, Madison 126, Sarah 210, Kayla 13, Lauren 136, Lauren 356, Olivia 345, Isabella 353, Samantha 143, Emily 403, Alyssa 128</t>
-        </is>
-      </c>
+      <c r="E91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1441,7 +1353,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Jessica 461, Alexis 35, Isabella 342, Elizabeth 67, Elizabeth 174, Jessica 278, Lauren 90, Elizabeth 436, Hannah 522, Taylor 222, Madison 54, Alexis 370, Alyssa 359, Taylor 6, Samantha 487, Isabella 241, Taylor 288, Abigail 490, Grace 199, Brianna 201, Hannah 323, Hannah 397, Olivia 384, Emily 336, Taylor 158, Olivia 41, Brianna 197, Hannah 165, Alexis 340, Ashley 140</t>
+          <t>Taylor 6, Kayla 13</t>
         </is>
       </c>
     </row>
@@ -1453,7 +1365,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Emma 98, Ashley 348, Kayla 139, Taylor 192, Jessica 191, Alexis 104, Emily 334, Olivia 103, Abigail 269, Kayla 407, Taylor 121, Madison 24, Lauren 8, Lauren 60, Alexis 471, Brianna 88, Alyssa 308, Grace 285</t>
+          <t>Lauren 8, Sarah 2</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1377,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Alyssa 493, Emma 118, Ashley 78, Taylor 115, Alyssa 435, Jessica 383, Grace 99, Ashley 123, Alyssa 132, Olivia 1, Emily 87, Alyssa 366, Grace 100, Olivia 416, Emma 499, Samantha 271</t>
+          <t>Olivia 1, Emma 9, Hannah 16, Kayla 7</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1389,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Alyssa 493, Lauren 52, Lauren 363, Elizabeth 174, Abigail 413, Hannah 522, Emily 330, Olivia 504, Brianna 221, Kayla 407, Madison 24, Lauren 8, Taylor 6, Isabella 241, Ashley 478, Taylor 226, Grace 285, Abigail 490, Sarah 377, Emma 216</t>
+          <t>Lauren 8, Taylor 6, Samantha 18, Madison 14, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1401,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Sarah 518, Isabella 426, Alexis 35, Hannah 522, Abigail 131, Olivia 1, Emily 146, Taylor 151, Emily 87, Taylor 121, Lauren 309, Sarah 377, Lauren 49, Ashley 460, Kayla 51, Ashley 286</t>
+          <t>Olivia 1, Samantha 18, Kayla 7</t>
         </is>
       </c>
     </row>
@@ -1499,11 +1411,7 @@
           <t>Tänavakunst</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Sarah 331, Kayla 252, Isabella 342, Emily 229, Jessica 191, Alexis 104, Lauren 90, Brianna 433, Grace 99, Alyssa 132, Samantha 211, Alyssa 306, Alexis 498, Ashley 240, Lauren 309, Emma 499, Abigail 408, Lauren 96, Taylor 509, Emily 144</t>
-        </is>
-      </c>
+      <c r="E97" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Järjekorra lisamine kursustele ja discordi bot
</commit_message>
<xml_diff>
--- a/õpetajateFail.xlsx
+++ b/õpetajateFail.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:O97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,6 +364,11 @@
           <t>Õpilased</t>
         </is>
       </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Järjekord</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -373,7 +378,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Alyssa 4, Lauren 8, Kayla 5, Madison 14</t>
+          <t>Jessica 278, Madison 204, Alexis 370, Abigail 269, Olivia 137, Lauren 96, Madison 324, Isabella 427, Lauren 60, Alyssa 4, Jessica 46, Kayla 252, Abigail 490, Lauren 8, Emily 144, Olivia 318, Samantha 488, Brianna 148, Madison 14, Isabella 485, Alexis 443, Jessica 425, Grace 280, Emily 505, Madison 464, Abigail 109, Isabella 95</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Kayla 497, Grace 320, Kayla 5, Emily 405, Isabella 275, Olivia 270, Emily 135, Olivia 186, Brianna 197, Brianna 47</t>
         </is>
       </c>
     </row>
@@ -385,7 +395,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lauren 12, Lauren 11</t>
+          <t>Jessica 423, Alyssa 435, Sarah 210, Alyssa 306, Elizabeth 476, Olivia 259, Ashley 453, Emily 229, Taylor 222, Ashley 50, Lauren 12, Elizabeth 449, Isabella 426, Samantha 327, Olivia 53, Emily 91, Sarah 315, Abigail 255, Olivia 234, Abigail 125, Jessica 44, Emily 439, Lauren 11, Madison 184, Madison 417, Samantha 150, Olivia 264</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Jessica 32, Grace 351, Lauren 494, Taylor 215, Taylor 176, Hannah 314, Madison 519, Kayla 75, Abigail 338, Emma 118</t>
         </is>
       </c>
     </row>
@@ -397,9 +412,10 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lauren 8, Alyssa 4</t>
-        </is>
-      </c>
+          <t>Jessica 278, Jessica 46, Lauren 8, Madison 417, Samantha 150, Alyssa 4</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -409,7 +425,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Elizabeth 10, Emma 9</t>
+          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Emily 349, Brianna 200, Brianna 513, Alyssa 421, Olivia 376, Madison 455, Elizabeth 10, Elizabeth 262, Taylor 158, Grace 256</t>
         </is>
       </c>
     </row>
@@ -421,9 +442,10 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Elizabeth 10, Emma 9</t>
-        </is>
-      </c>
+          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -433,9 +455,10 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Elizabeth 10, Emma 9</t>
-        </is>
-      </c>
+          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -443,7 +466,16 @@
           <t>Planimeetria alused</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Alyssa 493, Alyssa 233, Madison 352, Olivia 274, Jessica 383, Abigail 212, Isabella 244, Taylor 288, Elizabeth 399, Ashley 195, Madison 162, Grace 321, Grace 120, Elizabeth 284, Grace 263, Hannah 165, Grace 159, Brianna 513, Brianna 362, Sarah 501, Alexis 468, Abigail 71, Lauren 494, Lauren 56, Samantha 398, Madison 243, Alexis 470, Emma 185, Alyssa 304, Taylor 215</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Hannah 314, Brianna 61, Emma 64, Hannah 317, Ashley 326, Jessica 423, Emily 34, Taylor 288, Lauren 101, Lauren 248</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -451,7 +483,12 @@
           <t>3D-modelleerimine 3. periood</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Hannah 218, Elizabeth 174, Grace 515, Ashley 140, Lauren 346, Emma 58, Olivia 451, Grace 253, Isabella 63</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -459,7 +496,12 @@
           <t>3D-modelleerimine 5. periood</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Jessica 147, Grace 122, Grace 253, Elizabeth 157, Abigail 71, Samantha 27, Madison 519, Samantha 20</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -469,7 +511,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Alyssa 4, Kayla 5, Madison 14</t>
+          <t>Ashley 123, Alyssa 493, Taylor 151, Emma 216, Emma 238, Alyssa 508, Emma 98, Lauren 60, Alyssa 4, Abigail 108, Alyssa 19, Kayla 252, Madison 14, Alexis 343, Olivia 384, Emily 152, Sarah 315, Elizabeth 473, Lauren 249, Grace 280, Jessica 70, Brianna 179, Taylor 145, Jessica 44</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Emma 350, Elizabeth 328, Alexis 294, Jessica 374, Ashley 326, Hannah 165, Emma 217, Samantha 150, Jessica 32, Sarah 86</t>
         </is>
       </c>
     </row>
@@ -481,7 +528,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
+          <t>Kayla 188, Hannah 218, Isabella 183, Emily 507, Emily 91, Grace 89, Ashley 412, Brianna 373, Taylor 145, Brianna 42, Sarah 482, Alexis 294, Brianna 492, Samantha 20, Alexis 112, Madison 196, Alyssa 128, Samantha 18, Hannah 266, Brianna 251, Sarah 86, Grace 320, Emily 349, Alyssa 421</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Olivia 376, Olivia 124, Emily 333, Alexis 340, Kayla 268, Sarah 107, Hannah 393, Brianna 47, Taylor 176, Elizabeth 227</t>
         </is>
       </c>
     </row>
@@ -493,7 +545,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
+          <t>Alyssa 435, Olivia 416, Olivia 137, Alexis 381, Sarah 74, Emma 216, Taylor 254, Madison 324, Lauren 90, Emma 28, Madison 173, Alyssa 19, Olivia 1, Alexis 365, Ashley 348, Isabella 426, Samantha 327, Ashley 286, Grace 83, Jessica 311, Jessica 325, Grace 292, Grace 267, Jessica 425</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Elizabeth 473, Grace 321, Olivia 40, Emma 217, Lauren 101, Madison 196, Olivia 167, Ashley 246, Grace 351, Ashley 481</t>
         </is>
       </c>
     </row>
@@ -505,7 +562,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kayla 5, Isabella 3, Madison 14, Taylor 17, Alyssa 4, Samantha 18</t>
+          <t>Kayla 188, Jessica 206, Samantha 211, Lauren 232, Lauren 49, Alexis 498, Abigail 131, Ashley 50, Isabella 244, Madison 368, Emma 208, Lauren 360, Emma 28, Lauren 452</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Ashley 193, Alexis 335, Isabella 160, Elizabeth 385, Elizabeth 399, Madison 14, Taylor 17, Brianna 456, Ashley 392, Alexis 443</t>
         </is>
       </c>
     </row>
@@ -517,7 +579,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Sarah 2, Kayla 15, Lauren 12</t>
+          <t>Sarah 2, Kayla 15, Brianna 172, Olivia 103, Sarah 210, Alyssa 306, Alexis 498, Kayla 139, Madison 368, Elizabeth 67, Ashley 193, Samantha 302, Brianna 361, Grace 267, Emily 34, Sarah 156, Isabella 474, Olivia 496, Olivia 127, Samantha 462, Jessica 521</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Madison 417, Samantha 18, Lauren 310, Abigail 296, Alyssa 491, Jessica 175, Brianna 513, Emma 58, Isabella 347, Emily 479</t>
         </is>
       </c>
     </row>
@@ -529,7 +596,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Alyssa 4</t>
+          <t>Lauren 85, Emily 228, Sarah 74, Madison 324, Emma 238, Alyssa 4, Kayla 139, Madison 368, Isabella 241, Elizabeth 422, Taylor 192, Isabella 426, Taylor 288, Grace 22, Jessica 325, Alexis 343</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Alexis 443, Sarah 315, Jessica 44, Olivia 451, Emma 350, Abigail 341, Abigail 514, Hannah 182, Olivia 127, Kayla 497</t>
         </is>
       </c>
     </row>
@@ -541,7 +613,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Lauren 8, Kayla 15</t>
+          <t>Emily 146, Ashley 198, Samantha 211, Madison 24, Hannah 202, Grace 465, Alyssa 308, Alyssa 508, Abigail 212, Jessica 46, Kayla 252, Brianna 88, Alexis 335, Isabella 160, Ashley 478, Lauren 8, Emma 454, Jessica 147, Lauren 207, Brianna 361, Taylor 110, Samantha 276, Olivia 234, Elizabeth 328, Olivia 134, Grace 463, Brianna 492, Ashley 326, Samantha 20, Hannah 182, Lauren 372, Samantha 447, Grace 159, Elizabeth 166, Sarah 57, Olivia 154</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Samantha 73, Abigail 231, Isabella 353, Isabella 275, Taylor 26, Brianna 388, Elizabeth 262, Alexis 80, Emma 55, Madison 519</t>
         </is>
       </c>
     </row>
@@ -553,7 +630,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Isabella 3</t>
+          <t>Taylor 115, Brianna 433, Grace 465, Taylor 106, Ashley 50, Emma 208, Elizabeth 449, Alexis 365, Grace 285, Isabella 241, Grace 48, Kayla 410, Elizabeth 164, Jessica 70, Lauren 136, Alexis 371, Isabella 3, Samantha 483, Olivia 496, Madison 184</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Abigail 105, Lauren 372, Lauren 223, Samantha 447, Alyssa 133, Samantha 224, Alyssa 491, Jessica 175, Elizabeth 43, Alyssa 421</t>
         </is>
       </c>
     </row>
@@ -565,7 +647,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Lauren 8, Lauren 11</t>
+          <t>Emily 146, Samantha 211, Olivia 416, Grace 99, Taylor 509, Hannah 397, Abigail 408, Samantha 429, Isabella 354, Lauren 8, Kayla 409, Hannah 467, Sarah 114, Abigail 514, Lauren 11, Hannah 182, Ashley 414, Olivia 169, Lauren 101, Madison 196</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Isabella 260, Madison 149, Samantha 386, Emily 403, Isabella 353, Brianna 388, Kayla 268, Kayla 466, Ashley 458, Brianna 47</t>
         </is>
       </c>
     </row>
@@ -575,7 +662,16 @@
           <t>Labortöid füüsikas 10. ja 11. klassile</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Hannah 59, Brianna 433, Madison 24, Lauren 232, Taylor 121, Grace 99, Taylor 106, Sarah 74, Olivia 274, Abigail 131, Kayla 139, Alyssa 39</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Emma 28, Kayla 252, Elizabeth 422, Lauren 33, Alexis 171, Kayla 409, Samantha 488, Taylor 523, Emma 64, Grace 292</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -585,7 +681,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Kayla 13</t>
+          <t>Isabella 342, Hannah 218, Madison 126, Madison 368, Elizabeth 67, Elizabeth 174, Samantha 429, Alyssa 359, Kayla 13, Emma 454, Taylor 523, Jessica 147, Ashley 392, Taylor 110, Jessica 293, Olivia 234, Jessica 44, Olivia 451, Lauren 459, Sarah 512, Taylor 130, Samantha 20, Grace 247, Hannah 266, Brianna 251, Alexis 69, Olivia 167, Sarah 86, Ashley 246, Samantha 73, Alyssa 432, Brianna 419, Ashley 389, Grace 253, Elizabeth 157, Samantha 178, Olivia 21, Grace 428, Brianna 388, Emma 76, Elizabeth 473, Sarah 424, Grace 515, Grace 256, Olivia 376</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Emma 257, Elizabeth 227, Grace 159, Taylor 176, Abigail 71, Ashley 458, Olivia 154, Alexis 524, Abigail 131, Taylor 151</t>
         </is>
       </c>
     </row>
@@ -595,7 +696,16 @@
           <t>Joonestamine 4. periood</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Alyssa 132, Samantha 27, Emma 142, Grace 99, Emma 216, Alyssa 366, Elizabeth 472, Elizabeth 174, Isabella 63, Isabella 375, Olivia 53, Lauren 430, Jessica 147, Emma 387, Jessica 425, Hannah 467, Kayla 272, Grace 463, Emily 439, Olivia 496, Ashley 326, Grace 122, Samantha 462, Jessica 189, Lauren 346, Alyssa 491, Emma 58, Kayla 7, Abigail 71, Brianna 438, Emma 77, Brianna 388, Lauren 170, Sarah 424, Grace 431, Alexis 470, Olivia 237, Alyssa 304, Samantha 178, Ashley 140, Madison 519, Madison 301, Abigail 177, Kayla 369, Brianna 88</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Hannah 181, Brianna 197, Taylor 226, Emma 142, Elizabeth 262, Ashley 198, Sarah 501, Alexis 171, Grace 411, Grace 263</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -605,7 +715,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Hannah 16</t>
+          <t>Samantha 27, Alyssa 435, Brianna 433, Hannah 218, Isabella 183, Emma 142, Taylor 106, Lauren 457, Samantha 402, Abigail 212, Emma 28, Alexis 335, Isabella 241, Elizabeth 422, Alexis 171, Isabella 375, Isabella 295, Ashley 412, Alexis 36, Alexis 112, Olivia 477, Emma 404, Grace 282, Elizabeth 116</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Olivia 376, Jessica 219, Kayla 51, Isabella 275, Sarah 277, Grace 111, Lauren 494, Grace 253, Hannah 16, Abigail 113</t>
         </is>
       </c>
     </row>
@@ -617,7 +732,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Kayla 7, Kayla 13</t>
+          <t>Jessica 278, Emily 146, Hannah 194, Alyssa 233, Elizabeth 476, Olivia 259, Sarah 74, Brianna 153, Samantha 487, Abigail 131, Samantha 271, Lauren 33, Alexis 261, Lauren 489, Grace 83, Brianna 148, Hannah 357, Lauren 249, Samantha 382, Taylor 145, Brianna 42, Kayla 235, Emily 439, Taylor 130</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Olivia 40, Abigail 105, Ashley 414, Emma 217, Lauren 101, Hannah 266, Grace 159, Samantha 484, Hannah 287, Grace 511</t>
         </is>
       </c>
     </row>
@@ -629,7 +749,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Kayla 15</t>
+          <t>Emily 37, Kayla 15, Ashley 198, Samantha 211, Lauren 49, Alexis 381, Emma 142, Jessica 506, Jessica 383, Alexis 316, Lauren 360, Jessica 191, Elizabeth 67, Kayla 252, Samantha 302, Lauren 489, Olivia 318, Brianna 148, Ashley 81, Olivia 384, Elizabeth 307, Isabella 485, Grace 292, Grace 30, Grace 267</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Samantha 276, Jessica 70, Ashley 220, Hannah 332, Sarah 442, Emily 505, Alexis 36, Alexis 45, Grace 463, Abigail 105</t>
         </is>
       </c>
     </row>
@@ -641,7 +766,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Kayla 7</t>
+          <t>Emily 37, Elizabeth 436, Isabella 342, Alexis 381, Samantha 143, Ashley 453, Isabella 427, Ashley 50, Jessica 191, Isabella 426, Samantha 327, Olivia 318, Olivia 53, Emily 507, Grace 83, Brianna 148, Brianna 456, Isabella 485, Grace 30, Abigail 255, Hannah 357, Olivia 234</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Brianna 492, Emma 290, Brianna 190, Alyssa 133, Ashley 246, Hannah 287, Grace 511, Kayla 7, Elizabeth 79, Olivia 270</t>
         </is>
       </c>
     </row>
@@ -653,7 +783,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Emma 9</t>
+          <t>Ashley 123, Alyssa 493, Olivia 103, Brianna 221, Elizabeth 516, Taylor 121, Olivia 102, Alyssa 233, Ashley 50, Emma 208, Isabella 241, Olivia 318, Ashley 286, Abigail 517, Emma 448, Lauren 207, Hannah 129, Elizabeth 307, Jessica 70, Samantha 382, Alexis 371, Sarah 114, Olivia 451, Madison 225, Grace 321, Emma 9, Madison 184, Grace 263, Kayla 379</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Samantha 250, Emily 390, Abigail 296, Olivia 167, Samantha 386, Elizabeth 116, Grace 351, Lauren 356, Jessica 230, Ashley 389</t>
         </is>
       </c>
     </row>
@@ -665,7 +800,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Kayla 15, Kayla 5</t>
+          <t>Alexis 370, Kayla 15, Jessica 206, Elizabeth 436, Brianna 203, Sarah 518, Alexis 62, Madison 324, Grace 199, Alexis 316, Isabella 244, Emma 401, Jessica 437, Emma 118, Olivia 345, Taylor 288, Alexis 471, Samantha 327, Olivia 53, Emma 454, Elizabeth 289, Emma 300, Isabella 329, Brianna 179, Ashley 220, Abigail 125, Abigail 341, Elizabeth 328, Samantha 483, Elizabeth 284, Samantha 250, Olivia 477, Lauren 258, Jessica 189, Grace 320, Brianna 513, Ashley 481, Olivia 376, Emily 403, Brianna 418, Madison 415, Emma 77, Abigail 177, Elizabeth 262, Olivia 214, Taylor 158, Alexis 470, Hannah 281, Brianna 47, Hannah 314</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Brianna 179, Kayla 75, Brianna 190, Madison 415, Hannah 202, Kayla 369, Taylor 145, Brianna 92, Elizabeth 307, Sarah 501</t>
         </is>
       </c>
     </row>
@@ -677,7 +817,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Kayla 15, Taylor 17</t>
+          <t>Alexis 104, Kayla 15, Samantha 27, Elizabeth 436, Alyssa 306, Taylor 254, Samantha 487, Emily 445, Abigail 408, Lauren 367, Elizabeth 391, Alyssa 39, Isabella 354, Alexis 378, Lauren 475, Sarah 434, Emily 336, Isabella 295, Emily 507, Lauren 207, Taylor 17, Isabella 329, Elizabeth 307, Brianna 373, Emily 152</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Samantha 276, Elizabeth 473, Ashley 297, Alyssa 128, Samantha 150, Jessica 189, Olivia 376, Madison 155, Isabella 353, Brianna 418</t>
         </is>
       </c>
     </row>
@@ -689,7 +834,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Taylor 6, Elizabeth 10</t>
+          <t>Jessica 423, Isabella 183, Kayla 407, Taylor 6, Abigail 413, Lauren 457, Jessica 191, Emma 28, Lauren 248, Olivia 345, Abigail 108, Isabella 375, Kayla 409, Grace 83, Emily 91, Grace 267, Emily 34, Hannah 317, Alexis 36, Jessica 374, Brianna 492, Taylor 394, Lauren 101, Isabella 260, Elizabeth 166, Abigail 296, Lauren 358, Emma 404</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Elizabeth 10, Elizabeth 79, Taylor 26, Ashley 117, Sarah 277, Alexis 340, Sarah 424, Madison 415, Emily 152, Kayla 369</t>
         </is>
       </c>
     </row>
@@ -701,7 +851,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hannah 16, Isabella 3</t>
+          <t>Emily 37, Taylor 115, Madison 204, Alexis 381, Grace 100, Taylor 121, Ashley 453, Ashley 50, Ashley 193, Alyssa 359, Isabella 375, Grace 48, Jessica 311, Isabella 485, Grace 267, Jessica 70, Hannah 332, Hannah 181, Lauren 372, Olivia 127, Olivia 169, Samantha 150, Samantha 386, Samantha 68, Alyssa 491, Elizabeth 116, Madison 155, Ashley 84, Emily 97, Olivia 124, Taylor 26, Brianna 299, Sarah 424, Samantha 398, Grace 431, Alyssa 304, Samantha 178, Abigail 279, Olivia 41, Lauren 337, Ashley 392, Grace 463, Isabella 3, Grace 465, Hannah 16, Brianna 201, Samantha 276, Samantha 302, Olivia 21, Grace 111</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Alexis 316, Lauren 452, Hannah 165, Jessica 230, Emily 507, Elizabeth 227, Alyssa 39, Olivia 259, Emma 185, Olivia 237</t>
         </is>
       </c>
     </row>
@@ -711,7 +866,16 @@
           <t>Astronoomia</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Alyssa 493, Brianna 172, Lauren 85, Taylor 151, Hannah 194, Alexis 381, Lauren 96, Emma 216, Lauren 60, Abigail 408, Elizabeth 67, Abigail 108, Jessica 461, Ashley 240, Samantha 429, Sarah 331, Alyssa 273, Taylor 94, Emily 507, Lauren 207, Emma 387, Ashley 412, Brianna 180, Madison 162, Alyssa 245, Lauren 459, Alexis 294, Kayla 379, Alyssa 128, Samantha 447</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Lauren 310, Sarah 57, Olivia 138, Kayla 469, Brianna 419, Grace 253, Grace 431, Alexis 470, Brianna 197, Brianna 47</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -719,7 +883,16 @@
           <t>Astrofüüsika 2. periood</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Emily 37, Ashley 123, Madison 54, Samantha 211, Hannah 202, Hannah 194, Abigail 338, Olivia 102, Grace 99, Olivia 259, Emma 238, Brianna 153, Samantha 402, Ashley 453, Emma 25, Brianna 201, Emma 401, Lauren 33, Alyssa 273, Elizabeth 385, Alexis 471, Emily 334, Taylor 94, Emma 64, Ashley 81, Brianna 456, Jessica 446, Sarah 442, Elizabeth 328, Emily 439, Emma 290, Madison 417, Samantha 484, Brianna 190, Jessica 219</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Abigail 231, Emily 479, Olivia 138, Brianna 388, Alexis 80, Alexis 355, Kayla 466, Kayla 75, Grace 213, Brianna 179</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -729,7 +902,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Kayla 5, Emma 9</t>
+          <t>Alyssa 132, Alexis 104, Lauren 49, Kayla 407, Elizabeth 476, Alexis 35, Hannah 397, Lauren 360, Lauren 248, Abigail 108, Taylor 192, Grace 22, Brianna 373, Ashley 220, Abigail 341, Emma 9, Abigail 503, Samantha 483, Alexis 294, Lauren 29, Taylor 130, Isabella 95, Hannah 266, Madison 149, Abigail 296, Sarah 86, Grace 320, Hannah 287, Kayla 5, Elizabeth 43, Emma 72, Sarah 424, Alyssa 304, Taylor 215, Lauren 236</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Elizabeth 307, Hannah 16, Kayla 272, Lauren 457, Alexis 171, Elizabeth 449, Lauren 309, Brianna 221, Grace 120, Emma 238</t>
         </is>
       </c>
     </row>
@@ -741,7 +919,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Alyssa 4, Lauren 11</t>
+          <t>Jessica 278, Madison 204, Alexis 370, Samantha 27, Jessica 206, Elizabeth 436, Isabella 183, Olivia 103, Sarah 210, Taylor 151, Emma 142, Taylor 121, Alyssa 233, Brianna 153, Alyssa 4, Grace 199, Abigail 408, Jessica 191, Elizabeth 67, Elizabeth 449</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Alyssa 359, Alyssa 273, Elizabeth 385, Emily 336, Elizabeth 399, Brianna 456, Elizabeth 307, Isabella 485, Abigail 125, Olivia 502</t>
         </is>
       </c>
     </row>
@@ -751,7 +934,16 @@
           <t>Loogika 2. periood</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Jessica 206, Ashley 198, Brianna 221, Sarah 210, Hannah 323, Taylor 509, Emma 98, Emily 229, Hannah 397, Lauren 360, Ashley 78, Ashley 240, Alexis 335, Isabella 63, Samantha 327, Abigail 517, Samantha 480, Hannah 129, Olivia 239, Sarah 482, Abigail 450, Olivia 40, Kayla 379, Jessica 163, Olivia 264, Emily 349, Jessica 265, Brianna 200, Jessica 230, Brianna 92, Olivia 214</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Kayla 268, Ashley 168, Lauren 337, Olivia 318, Olivia 234, Brianna 92, Elizabeth 307, Samantha 483, Hannah 287, Abigail 231</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -761,7 +953,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sarah 2</t>
+          <t>Sarah 2, Madison 204, Jessica 423, Hannah 194, Brianna 153, Samantha 402, Alexis 378, Sarah 331, Abigail 490, Lauren 33, Lauren 475, Alexis 261, Lauren 337, Grace 120, Lauren 459, Ashley 414, Alyssa 133, Emma 404, Abigail 344, Ashley 246, Elizabeth 141, Alyssa 440, Elizabeth 262, Alexis 80, Alexis 355, Ashley 168, Emma 55, Hannah 314, Ashley 441, Isabella 187, Madison 415</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Emily 144, Sarah 107, Hannah 467, Lauren 232, Olivia 137, Alyssa 245, Abigail 82, Abigail 291, Samantha 402, Jessica 437</t>
         </is>
       </c>
     </row>
@@ -771,7 +968,12 @@
           <t>Programmeerimine keeles Java 1</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Olivia 318, Sarah 315, Isabella 485</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -780,6 +982,7 @@
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -789,7 +992,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Kayla 5</t>
+          <t>Olivia 504, Brianna 172, Olivia 416, Brianna 203, Grace 396, Jessica 23, Taylor 106, Sarah 74, Lauren 96, Lauren 457, Isabella 244, Alexis 365, Lauren 52, Elizabeth 422, Samantha 327, Olivia 384, Brianna 361, Abigail 255, Elizabeth 473, Emily 505, Abigail 109, Olivia 134, Sarah 512, Samantha 484, Jessica 32, Grace 282, Kayla 5, Emily 405, Kayla 469, Sarah 277</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Olivia 214, Lauren 494, Samantha 398, Lauren 236, Madison 301, Ashley 510, Jessica 44, Grace 463, Olivia 318, Brianna 201</t>
         </is>
       </c>
     </row>
@@ -801,7 +1009,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Elizabeth 10, Alyssa 4</t>
+          <t>Hannah 59, Lauren 49, Olivia 103, Taylor 151, Emma 142, Olivia 102, Lauren 457, Emma 238, Isabella 427, Alyssa 366, Elizabeth 391, Alyssa 39, Madison 368, Abigail 108, Alyssa 19, Alexis 365, Brianna 88, Alexis 171, Isabella 63, Lauren 430, Ashley 195, Elizabeth 307, Alexis 443, Jessica 425, Elizabeth 473, Abigail 291, Olivia 502, Brianna 180, Emma 350, Madison 225, Alexis 294, Sarah 512, Isabella 474, Emily 390, Ashley 246, Kayla 369, Emma 305, Kayla 51, Madison 322, Olivia 270, Grace 428, Alexis 80, Sarah 420, Olivia 186, Emma 185, Kayla 75, Taylor 215, Ashley 510, Jessica 44, Emily 152</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Brianna 388, Hannah 181, Alexis 45, Elizabeth 262, Abigail 450, Hannah 281, Abigail 279, Brianna 42, Sarah 312, Alyssa 366</t>
         </is>
       </c>
     </row>
@@ -813,7 +1026,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Lauren 12, Lauren 11, Emma 9, Sarah 2, Olivia 1</t>
+          <t>Alyssa 435, Hannah 218, Isabella 183, Abigail 338, Alyssa 308, Grace 396, Samantha 143, Madison 126, Alyssa 508, Lauren 12, Elizabeth 472, Elizabeth 67, Madison 173, Lauren 452, Samantha 429, Isabella 160, Elizabeth 385, Emily 87, Kayla 409, Ashley 286, Alexis 343, Emma 387, Samantha 480, Sarah 315, Hannah 467, Abigail 255, Jessica 293, Emma 9, Lauren 459, Kayla 272, Lauren 11, Taylor 394, Jessica 163, Ashley 283, Elizabeth 166, Olivia 167, Jessica 175, Grace 282, Emily 405, Isabella 353, Jessica 230, Alyssa 432, Abigail 82, Alexis 340, Madison 243, Ashley 458, Sarah 107, Alyssa 339, Madison 301, Olivia 318</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Brianna 362, Ashley 198, Elizabeth 472, Taylor 288, Lauren 309, Grace 263, Taylor 509, Grace 515, Jessica 374, Emma 387</t>
         </is>
       </c>
     </row>
@@ -823,7 +1041,16 @@
           <t>Arvutite riistvara ja lisaseadmed</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Alexis 370, Abigail 131, Emily 229, Alexis 316, Emma 401, Madison 173, Alyssa 273, Taylor 288, Emily 334, Emma 454, Emma 448, Emma 387, Grace 89, Brianna 180, Brianna 42, Ashley 297</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Madison 464, Sarah 512, Grace 463, Alyssa 380, Grace 263, Lauren 372, Grace 247, Elizabeth 166, Alexis 69, Jessica 189</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -831,7 +1058,16 @@
           <t>Loodusteadused, tehnoloogia ja ühiskond</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Emily 146, Elizabeth 436, Samantha 211, Olivia 137, Emily 228, Elizabeth 476, Taylor 254, Emma 238, Lauren 60, Emily 445, Lauren 90, Sarah 377, Lauren 452, Isabella 160, Elizabeth 385, Emily 87, Emily 144, Jessica 311, Emily 152, Grace 280, Hannah 165, Emma 217, Jessica 521, Emma 305, Sarah 312</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Elizabeth 79, Samantha 298, Grace 515, Brianna 419, Brianna 205, Taylor 215, Lauren 85, Samantha 68, Brianna 362, Emily 135</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -841,7 +1077,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Hannah 16, Olivia 1</t>
+          <t>Lauren 49, Alyssa 308, Madison 126, Brianna 61, Alexis 35, Samantha 429, Ashley 193, Alexis 471, Emily 334, Ashley 392, Isabella 485, Elizabeth 364, Taylor 110, Sarah 156, Olivia 234, Alyssa 245, Abigail 514, Samantha 483, Taylor 130, Emma 290, Taylor 394, Ashley 283, Alexis 69, Jessica 219, Madison 155, Isabella 347, Isabella 275</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Alexis 468, Alyssa 432, Abigail 177, Taylor 158, Hannah 16, Madison 243, Olivia 21, Kayla 75, Brianna 190, Lauren 337</t>
         </is>
       </c>
     </row>
@@ -853,7 +1094,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
+          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Abigail 503, Isabella 474, Lauren 93, Hannah 165, Isabella 95, Alexis 69, Alyssa 133, Samantha 386, Emma 305, Abigail 209</t>
         </is>
       </c>
     </row>
@@ -865,9 +1111,10 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
-        </is>
-      </c>
+          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -877,9 +1124,10 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
-        </is>
-      </c>
+          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -887,7 +1135,16 @@
           <t>Kirjandus ja film</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Sarah 400, Kayla 188, Emily 330, Olivia 416, Alyssa 308, Grace 100, Elizabeth 516, Samantha 143, Alexis 62, Alexis 316, Lauren 90, Elizabeth 472, Alyssa 19, Sarah 331, Alexis 171, Emma 387, Abigail 255, Hannah 357, Sarah 156, Abigail 291, Sarah 114, Alyssa 245, Hannah 332, Emma 350, Olivia 38, Kayla 235, Kayla 272, Olivia 169, Emily 390, Madison 149, Kayla 495, Samantha 386, Grace 282, Kayla 369</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Isabella 161, Emily 403, Madison 415, Emma 77, Abigail 82, Lauren 170, Grace 431, Sarah 107, Madison 519, Olivia 41</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -897,7 +1154,12 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Emma 9</t>
+          <t>Lauren 363, Olivia 504, Elizabeth 486, Hannah 59, Brianna 203, Alexis 381, Isabella 395, Emma 142, Jessica 23, Elizabeth 476, Jessica 506, Brianna 61, Samantha 271, Samantha 302, Ashley 348, Olivia 53, Elizabeth 289, Ashley 412, Lauren 249, Abigail 125, Olivia 502, Emma 9, Emma 217</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Jessica 521, Lauren 346, Grace 511, Sarah 57, Emma 305, Elizabeth 141, Isabella 347, Madison 322, Elizabeth 313, Alexis 524</t>
         </is>
       </c>
     </row>
@@ -909,7 +1171,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Lauren 12, Sarah 2, Hannah 16</t>
+          <t>Sarah 2, Madison 24, Lauren 232, Lauren 85, Sarah 74, Alexis 498, Sarah 31, Alyssa 366, Lauren 12, Madison 319, Emma 118, Lauren 452, Taylor 226, Elizabeth 422, Taylor 192, Lauren 337, Grace 22, Jessica 311, Jessica 325, Alexis 343</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Brianna 361, Emily 65, Abigail 341, Alyssa 380, Ashley 326, Samantha 250, Madison 196, Ashley 283, Olivia 477, Lauren 310</t>
         </is>
       </c>
     </row>
@@ -921,7 +1188,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Lauren 11</t>
+          <t>Alyssa 435, Brianna 172, Olivia 103, Taylor 222, Grace 199, Emma 499, Kayla 139, Jessica 437, Brianna 88, Isabella 160, Alexis 261, Emma 300, Sarah 315, Hannah 467, Samantha 382, Ashley 220, Brianna 180, Abigail 503, Alexis 294, Alexis 45</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Grace 463, Isabella 474, Lauren 11, Lauren 93, Alexis 112, Lauren 258, Ashley 481, Emma 58, Madison 455, Grace 515</t>
         </is>
       </c>
     </row>
@@ -933,7 +1205,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Lauren 8, Kayla 13, Isabella 3, Kayla 7</t>
+          <t>Samantha 27, Isabella 183, Alyssa 308, Emma 142, Sarah 518, Emma 98, Abigail 212, Jessica 46, Emma 401, Alyssa 19, Kayla 13, Elizabeth 385, Lauren 8, Brianna 148, Grace 30, Hannah 317</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Sarah 114, Alexis 36, Isabella 3, Samantha 20, Taylor 394, Olivia 169, Samantha 250, Emily 390, Olivia 154, Kayla 7</t>
         </is>
       </c>
     </row>
@@ -944,6 +1221,7 @@
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -953,7 +1231,12 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Madison 14, Taylor 17, Kayla 5</t>
+          <t>Jessica 278, Emily 37, Isabella 342, Abigail 269, Abigail 338, Grace 396, Alexis 498, Taylor 509, Emma 25, Lauren 360, Madison 173, Taylor 192, Ashley 286, Abigail 517, Madison 14, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Samantha 480, Ashley 81, Brianna 456, Grace 267, Sarah 442, Alyssa 380, Abigail 450, Olivia 496, Taylor 130, Samantha 462</t>
         </is>
       </c>
     </row>
@@ -964,6 +1247,7 @@
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -971,7 +1255,16 @@
           <t>Lähis-Ida 20. sajandi teisest poolest tänapäevani</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Lauren 49, Brianna 221, Emily 228, Lauren 457, Madison 324, Emma 238, Lauren 90, Olivia 345, Brianna 88, Samantha 302, Alyssa 359, Lauren 52, Hannah 357, Grace 280, Taylor 145, Alexis 371, Brianna 42, Madison 225, Grace 321, Kayla 235, Alexis 45, Olivia 127, Emma 217, Lauren 346, Jessica 219, Brianna 362, Jessica 230, Alexis 468, Grace 515, Alyssa 432, Grace 428, Olivia 214, Emma 72, Alexis 355, Emma 55, Grace 213</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Brianna 179, Madison 301, Ashley 392, Abigail 177, Elizabeth 307, Grace 267, Samantha 483, Olivia 134, Lauren 475, Elizabeth 449</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -981,7 +1274,12 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sarah 2</t>
+          <t>Sarah 2, Madison 54, Hannah 218, Olivia 103, Olivia 416, Samantha 143, Madison 126, Alexis 35, Jessica 383, Hannah 397, Madison 368, Isabella 241, Emily 334, Isabella 375, Grace 22, Jessica 520, Elizabeth 289, Grace 83, Elizabeth 164, Isabella 485, Emily 65, Sarah 156, Lauren 249, Jessica 70, Abigail 514, Kayla 272, Lauren 29, Brianna 492, Olivia 40, Lauren 101, Abigail 296, Grace 320</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Ashley 481, Emily 403, Lauren 356, Sarah 501, Samantha 298, Emma 257, Emily 333, Kayla 268, Hannah 119, Olivia 237</t>
         </is>
       </c>
     </row>
@@ -993,7 +1291,12 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
+          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Grace 89, Olivia 384, Elizabeth 307, Brianna 179, Grace 120, Sarah 482, Grace 263, Lauren 258, Emma 404, Hannah 287</t>
         </is>
       </c>
     </row>
@@ -1005,9 +1308,10 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
-        </is>
-      </c>
+          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1017,9 +1321,10 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
-        </is>
-      </c>
+          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1029,7 +1334,12 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
+          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Samantha 224, Samantha 68, Jessica 265, Alyssa 491, Grace 511, Abigail 231, Madison 155, Isabella 353, Ashley 84, Abigail 177</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1351,10 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
-        </is>
-      </c>
+          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1053,9 +1364,10 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
-        </is>
-      </c>
+          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1065,7 +1377,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alyssa 4, Kayla 15, Hannah 16</t>
+          <t>Alexis 370, Kayla 15, Ashley 123, Emily 146, Ashley 198, Jessica 506, Abigail 413, Alyssa 508, Samantha 487, Alyssa 4, Elizabeth 391, Jessica 191, Isabella 354, Ashley 193, Alexis 335, Lauren 475, Olivia 318, Emma 454</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Emma 448, Ashley 392, Brianna 361, Emily 34, Elizabeth 473, Emma 350, Abigail 341, Ashley 297, Madison 464, Elizabeth 328</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1392,16 @@
           <t>Ajakirjanduse alused</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Kayla 188, Emily 330, Jessica 23, Ashley 460, Abigail 131, Kayla 139, Elizabeth 472, Olivia 345, Ashley 193, Sarah 331, Elizabeth 422, Alexis 261, Lauren 430, Kayla 410, Abigail 255, Jessica 293, Lauren 136, Alexis 371, Jessica 44, Olivia 38, Lauren 459, Olivia 239, Elizabeth 284, Olivia 496, Hannah 165, Lauren 223, Alyssa 128, Isabella 260, Jessica 189, Brianna 190, Alyssa 133</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Samantha 386, Jessica 175, Isabella 161, Olivia 376, Madison 155, Madison 322, Kayla 469, Madison 444, Madison 415, Taylor 158</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1085,7 +1411,12 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Hannah 16, Samantha 18</t>
+          <t>Taylor 115, Jessica 423, Olivia 504, Abigail 338, Taylor 106, Lauren 457, Ashley 453, Emily 229, Emily 445, Emma 118, Emma 208, Sarah 377, Ashley 78, Ashley 240, Grace 285, Samantha 302, Emily 87, Taylor 288, Lauren 489, Olivia 53, Emily 507, Emma 300, Brianna 148, Ashley 81, Elizabeth 164, Jessica 70, Emily 505, Madison 464, Lauren 93, Taylor 394</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Samantha 462, Emily 390, Samantha 18, Isabella 242, Lauren 258, Lauren 310, Kayla 495, Elizabeth 116, Emma 58, Sarah 312</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1426,12 @@
           <t>Filosoofia 2</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Taylor 106, Emily 445, Emma 208, Emily 507, Lauren 93</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1105,7 +1441,12 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Kayla 7, Taylor 17</t>
+          <t>Lauren 363, Brianna 433, Samantha 143, Sarah 518, Jessica 506, Jessica 383, Alyssa 39, Madison 319, Emma 401, Madison 368, Samantha 271, Sarah 434, Isabella 295, Jessica 520, Jessica 303, Samantha 488, Taylor 17, Ashley 195</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Olivia 384, Ashley 412, Grace 30, Grace 280, Brianna 179, Jessica 446, Madison 225, Samantha 250, Brianna 251, Lauren 346</t>
         </is>
       </c>
     </row>
@@ -1117,9 +1458,10 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Kayla 7, Taylor 17</t>
-        </is>
-      </c>
+          <t>Lauren 363, Brianna 433, Samantha 143, Sarah 518, Jessica 506, Jessica 383, Alyssa 39, Madison 319, Emma 401, Madison 368, Samantha 271, Sarah 434, Isabella 295, Jessica 520, Jessica 303, Samantha 488, Taylor 17, Ashley 195</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1129,7 +1471,12 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Lauren 12, Taylor 6</t>
+          <t>Sarah 400, Ashley 123, Alyssa 493, Lauren 96, Taylor 509, Emma 98, Lauren 367, Ashley 50, Lauren 12, Isabella 244, Isabella 354, Lauren 33, Lauren 475, Kayla 409, Lauren 337, Abigail 517, Elizabeth 364, Hannah 467, Hannah 357, Lauren 249, Samantha 382, Brianna 180, Kayla 272, Jessica 374, Abigail 450, Isabella 474</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Emily 439, Ashley 414, Kayla 379, Madison 417, Jessica 32, Lauren 358, Brianna 362, Olivia 270, Emily 97, Emma 257</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1488,12 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Sarah 2, Isabella 3, Elizabeth 10, Madison 14</t>
+          <t>Sarah 2, Abigail 269, Hannah 194, Isabella 395, Hannah 323, Alyssa 306, Alexis 62, Madison 126, Brianna 61, Samantha 487, Isabella 427, Lauren 60, Brianna 201, Hannah 522, Samantha 429, Lauren 52, Abigail 490, Madison 14</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Hannah 129, Sarah 114, Alyssa 245, Sarah 442, Alexis 36, Isabella 3, Abigail 514, Kayla 235, Sarah 512, Grace 263</t>
         </is>
       </c>
     </row>
@@ -1153,7 +1505,12 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Kayla 13</t>
+          <t>Brianna 172, Brianna 221, Elizabeth 516, Madison 352, Abigail 413, Alexis 498, Olivia 274, Lauren 309, Sarah 31, Elizabeth 391, Emma 499, Jessica 437, Jessica 461, Alexis 378, Isabella 241, Kayla 13</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Alexis 471, Emily 144, Emily 334, Elizabeth 289, Taylor 523, Emily 152, Madison 162, Emily 349, Brianna 513, Grace 515</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1520,16 @@
           <t>Fotograafia 1</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Lauren 49, Alyssa 308, Lauren 96, Jessica 506, Abigail 413, Alexis 35, Brianna 153, Emily 445, Taylor 226, Isabella 160, Lauren 475, Grace 22, Jessica 520, Jessica 325, Samantha 480, Elizabeth 307, Jessica 425, Alexis 371, Hannah 181, Abigail 341, Lauren 459, Kayla 235, Olivia 134, Lauren 93</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Samantha 20, Kayla 497, Ashley 481, Abigail 231, Madison 455, Sarah 501, Olivia 138, Alexis 355, Grace 431, Madison 243</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1171,7 +1537,16 @@
           <t>Inimene ja ühiskond 3. periood</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Jessica 423, Olivia 137, Abigail 338, Taylor 121, Madison 126, Samantha 487, Jessica 383, Elizabeth 391, Taylor 192, Taylor 94, Samantha 488, Emma 64, Emily 91, Ashley 81, Ashley 392, Emily 65, Kayla 272, Jessica 163, Grace 159, Lauren 258, Kayla 495, Grace 320, Jessica 265, Kayla 369, Jessica 230, Ashley 389, Ashley 117, Brianna 299, Emma 77, Abigail 82, Emma 72, Lauren 56, Grace 463, Ashley 198, Sarah 277, Olivia 270</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Kayla 466, Ashley 481, Alyssa 491, Lauren 11, Madison 444, Samantha 211, Samantha 402, Madison 196, Sarah 482, Olivia 237</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1181,7 +1556,12 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Lauren 12</t>
+          <t>Madison 24, Emma 25, Taylor 222, Lauren 12, Elizabeth 289, Isabella 95, Kayla 379, Madison 417, Jessica 189, Jessica 32, Alyssa 491, Isabella 161, Isabella 275, Madison 444, Madison 415, Emma 257, Alexis 355, Lauren 494, Elizabeth 313, Brianna 197, Hannah 281, Elizabeth 227, Olivia 21, Kayla 51, Emma 76, Grace 411, Sarah 424, Grace 111, Hannah 393, Alyssa 440, Alexis 69, Grace 253, Olivia 237, Emily 349, Hannah 194, Ashley 441</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Emily 390, Olivia 38, Sarah 377, Alyssa 493, Elizabeth 364, Jessica 325, Lauren 372, Emily 146, Abigail 209, Jessica 163</t>
         </is>
       </c>
     </row>
@@ -1193,7 +1573,12 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Isabella 3</t>
+          <t>Jessica 278, Abigail 269, Kayla 407, Lauren 90, Alyssa 359, Samantha 276, Hannah 317, Lauren 136, Abigail 125, Madison 162, Alyssa 245, Sarah 442, Madison 225, Olivia 38, Isabella 3, Olivia 239, Sarah 482, Lauren 29, Abigail 450, Olivia 40, Taylor 394, Grace 122, Alyssa 128, Isabella 242, Brianna 251, Lauren 358, Sarah 57, Brianna 200, Grace 515, Kayla 469</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Brianna 419, Brianna 438, Alexis 80, Sarah 107, Alyssa 304, Ashley 140, Grace 213, Lauren 85, Taylor 226, Olivia 234</t>
         </is>
       </c>
     </row>
@@ -1205,7 +1590,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Lauren 12, Kayla 15, Lauren 11, Elizabeth 10</t>
+          <t>Sarah 400, Kayla 15, Samantha 27, Brianna 221, Abigail 338, Isabella 395, Elizabeth 476, Jessica 506, Taylor 254, Abigail 413, Lauren 457, Brianna 153, Sarah 31, Jessica 46, Alexis 316, Elizabeth 391, Lauren 12, Jessica 437, Alexis 378, Kayla 252, Isabella 426, Lauren 475, Alexis 261, Emily 507, Emma 300, Brianna 148, Lauren 207, Emily 91, Brianna 361, Emily 65</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Grace 267, Sarah 315, Emily 34, Hannah 357, Abigail 291, Brianna 179, Madison 225, Grace 321, Isabella 474, Emily 439</t>
         </is>
       </c>
     </row>
@@ -1215,7 +1605,16 @@
           <t>Turundus</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Hannah 59, Lauren 232, Brianna 221, Olivia 259, Alyssa 39, Jessica 461, Ashley 240, Brianna 88, Lauren 52, Lauren 33, Ashley 348, Abigail 503, Taylor 130, Emily 390, Lauren 346, Alyssa 421, Emma 305, Madison 155, Elizabeth 141, Ashley 84, Alyssa 432, Emily 97, Abigail 71, Elizabeth 262, Taylor 158, Ashley 168</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Samantha 398, Alexis 470, Kayla 75, Madison 301, Grace 411, Emma 76, Madison 415, Kayla 369, Alyssa 304, Hannah 317</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1225,7 +1624,12 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Kayla 13, Taylor 17</t>
+          <t>Lauren 85, Grace 396, Elizabeth 476, Sarah 518, Sarah 74, Olivia 274, Elizabeth 449, Sarah 331, Kayla 13, Lauren 489, Abigail 517, Taylor 17, Hannah 332, Grace 120, Abigail 109, Elizabeth 284, Alexis 45, Emily 439, Madison 184, Samantha 250, Olivia 167, Samantha 68, Samantha 73, Lauren 356</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Brianna 362, Alexis 468, Madison 322, Samantha 298, Grace 428, Emma 257, Emily 333, Hannah 281, Taylor 500, Madison 519</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1641,12 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Lauren 12, Kayla 15, Lauren 11, Elizabeth 10, Isabella 3</t>
+          <t>Kayla 15, Elizabeth 486, Hannah 202, Lauren 85, Grace 100, Isabella 395, Alyssa 508, Emma 25, Taylor 222, Grace 199, Abigail 408, Lauren 12, Jessica 437, Emma 118, Lauren 248, Abigail 108, Taylor 226, Elizabeth 449, Isabella 426, Emily 336</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Jessica 325, Alexis 343, Grace 267, Alexis 443, Samantha 276, Jessica 293, Jessica 44, Olivia 239, Lauren 11, Elizabeth 166</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1656,16 @@
           <t>Kujutav geomeetria</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Sarah 400, Hannah 59, Taylor 509, Emma 98, Ashley 453, Madison 173, Isabella 354, Kayla 252, Alyssa 273, Ashley 478, Taylor 288, Elizabeth 289, Emma 300, Isabella 329, Ashley 81, Grace 30, Emily 34, Lauren 136, Abigail 125, Jessica 446, Olivia 502, Madison 162</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Hannah 332, Hannah 181, Kayla 235, Madison 464, Elizabeth 328, Jessica 374, Isabella 95, Lauren 372, Grace 247, Lauren 101</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1255,7 +1673,12 @@
           <t>Loominguline joonistamine 2</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Alexis 381, Samantha 302</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1265,7 +1688,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Kayla 13, Taylor 6, Madison 14</t>
+          <t>Taylor 115, Jessica 206, Madison 24, Sarah 210, Hannah 323, Jessica 66, Lauren 309, Emily 229, Grace 285, Kayla 13, Ashley 348, Kayla 409, Taylor 94, Grace 83, Taylor 523, Hannah 317, Lauren 249, Abigail 291, Brianna 180, Alexis 36, Elizabeth 284, Olivia 127, Olivia 169, Isabella 260, Grace 159, Hannah 287, Grace 511, Sarah 57, Brianna 200, Isabella 161, Samantha 73, Abigail 231, Emily 403, Isabella 353, Madison 322</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Emma 72, Lauren 56, Ashley 458, Abigail 279, Ashley 78, Ashley 392, Alyssa 304, Taylor 222, Alyssa 432, Taylor 6</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1705,12 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Kayla 13, Lauren 11, Kayla 7</t>
+          <t>Jessica 278, Taylor 115, Alexis 370, Jessica 423, Ashley 123, Sarah 210, Grace 396, Grace 99, Lauren 96, Lauren 457, Lauren 60, Hannah 397, Elizabeth 391, Emma 28, Samantha 429, Alyssa 359, Kayla 13, Alyssa 273, Samantha 480, Grace 89, Brianna 361, Elizabeth 164, Olivia 234, Alyssa 245, Hannah 181, Ashley 297, Lauren 459, Elizabeth 284, Alyssa 380, Lauren 11, Lauren 372, Emma 217, Samantha 462, Olivia 477, Sarah 86, Samantha 224</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Jessica 265, Samantha 73, Emily 403, Isabella 353, Kayla 7, Madison 455, Sarah 501, Elizabeth 79, Grace 515, Abigail 71</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1722,12 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Lauren 8, Taylor 17</t>
+          <t>Alyssa 435, Lauren 232, Brianna 221, Hannah 194, Elizabeth 476, Samantha 487, Abigail 408, Lauren 90, Emma 401, Lauren 8, Emily 334, Isabella 295, Emma 454, Jessica 520, Samantha 488</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Kayla 410, Taylor 523, Taylor 17, Ashley 195, Sarah 156, Lauren 136, Sarah 114, Grace 321, Olivia 38, Olivia 239</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1739,12 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Sarah 2, Madison 14</t>
+          <t>Sarah 2, Brianna 433, Abigail 269, Olivia 137, Abigail 338, Samantha 143, Brianna 153, Samantha 402, Emily 445, Abigail 212, Isabella 160, Taylor 94, Abigail 517, Madison 14, Emma 387, Ashley 412, Emily 34, Hannah 317, Jessica 446, Brianna 42, Sarah 482, Abigail 109, Emily 439, Taylor 130</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Grace 122, Alyssa 128, Isabella 260, Lauren 310, Samantha 484, Brianna 251, Ashley 246, Brianna 513, Alyssa 421, Jessica 219</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1756,12 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Kayla 5</t>
+          <t>Emily 146, Alyssa 493, Hannah 218, Olivia 103, Ashley 50, Taylor 226, Samantha 327, Emma 448, Ashley 392, Emily 152, Emily 65, Hannah 467, Abigail 255, Hannah 357, Elizabeth 473, Isabella 474, Emma 290, Ashley 414, Olivia 169, Lauren 101, Samantha 150, Lauren 346, Kayla 495, Samantha 386, Emily 349, Hannah 287, Grace 282, Kayla 5, Emma 305, Elizabeth 10, Kayla 469, Ashley 117, Alexis 340, Ashley 168, Olivia 186, Hannah 119, Ashley 458, Emma 185, Taylor 500, Grace 463, Lauren 310, Brianna 92, Emma 216, Kayla 272, Elizabeth 262, Olivia 138, Emily 135, Brianna 205, Kayla 497, Emily 479, Isabella 347, Sarah 114, Emma 72, Abigail 82, Grace 159, Taylor 176, Sarah 420, Jessica 265, Madison 225, Brianna 419, Brianna 492, Olivia 264, Hannah 266, Brianna 172, Brianna 47, Sarah 518, Alexis 294, Elizabeth 116, Brianna 299, Olivia 154, Elizabeth 385, Samantha 298, Elizabeth 157, Abigail 108, Brianna 513, Madison 455, Samantha 398, Hannah 332, Isabella 375, Kayla 75</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Emily 65, Lauren 337, Jessica 325, Elizabeth 166, Emma 28, Isabella 426, Olivia 376, Ashley 460, Grace 282, Lauren 494</t>
         </is>
       </c>
     </row>
@@ -1323,7 +1771,12 @@
           <t>Riigikaitse 2</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Hannah 218, Taylor 226, Olivia 169, Samantha 150, Samantha 386, Ashley 392, Hannah 119, Ashley 414, Emma 185, Brianna 47, Alexis 294, Lauren 346, Elizabeth 10, Elizabeth 157, Olivia 138, Sarah 420, Elizabeth 262, Elizabeth 116, Emily 135, Emily 349, Hannah 266, Hannah 467, Kayla 272, Emily 152, Ashley 458</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1333,7 +1786,12 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Isabella 3, Hannah 16</t>
+          <t>Hannah 59, Isabella 183, Alyssa 308, Kayla 407, Alyssa 306, Taylor 121, Taylor 106, Abigail 413, Alexis 498, Olivia 274, Emily 229, Jessica 46, Olivia 345, Madison 173, Brianna 88, Lauren 52, Lauren 33, Kayla 409, Ashley 286, Lauren 207, Emily 91, Brianna 456, Jessica 425, Lauren 249, Taylor 145</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Madison 225, Grace 120, Isabella 3, Samantha 483, Alexis 294, Kayla 272, Abigail 450, Olivia 496, Brianna 492, Ashley 326</t>
         </is>
       </c>
     </row>
@@ -1343,7 +1801,16 @@
           <t>Ajakirjanduse praktika</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Emily 330, Jessica 23, Ashley 460, Emily 229, Isabella 375, Taylor 523, Abigail 255, Hannah 317, Jessica 70, Alexis 36, Brianna 190, Grace 511, Samantha 73, Lauren 309, Hannah 165, Alexis 371, Emily 334, Isabella 161, Brianna 200, Brianna 492, Jessica 189, Elizabeth 284, Samantha 143, Emily 403, Kayla 13, Lauren 223, Lauren 136, Olivia 345, Isabella 353, Alyssa 128</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Brianna 88, Lauren 207, Elizabeth 141, Emily 144, Kayla 409, Jessica 461, Emily 479, Emma 499, Ashley 414, Elizabeth 307</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1353,7 +1820,12 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Taylor 6, Kayla 13</t>
+          <t>Jessica 278, Alexis 370, Elizabeth 436, Madison 54, Isabella 342, Hannah 323, Taylor 6, Alexis 35, Samantha 487, Hannah 397, Taylor 222, Grace 199, Brianna 201, Lauren 90, Elizabeth 67, Elizabeth 174, Jessica 461, Hannah 522, Alyssa 359, Isabella 241, Abigail 490, Taylor 288, Emily 336, Olivia 318, Olivia 53, Grace 48, Jessica 147, Grace 89, Ashley 195, Olivia 384</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Isabella 485, Lauren 249, Taylor 145, Alyssa 245, Hannah 181, Ashley 297, Lauren 459, Grace 463, Grace 263, Hannah 165</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1837,12 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Lauren 8, Sarah 2</t>
+          <t>Sarah 2, Alexis 104, Elizabeth 486, Madison 24, Abigail 269, Hannah 202, Olivia 103, Sarah 210, Alyssa 308, Kayla 407, Taylor 121, Sarah 74, Madison 126, Emma 98, Lauren 60, Kayla 139, Alyssa 39, Jessica 191</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Alyssa 19, Samantha 429, Grace 285, Brianna 88, Alexis 171, Ashley 348, Taylor 192, Alexis 471, Lauren 8, Emily 334</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1854,12 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Olivia 1, Emma 9, Hannah 16, Kayla 7</t>
+          <t>Alyssa 132, Taylor 115, Ashley 123, Alyssa 435, Alyssa 493, Olivia 416, Grace 100, Emily 228, Grace 99, Taylor 509, Samantha 402, Jessica 383, Alyssa 366, Emma 499, Emma 118, Ashley 78</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Olivia 345, Olivia 1, Samantha 271, Emily 87, Kayla 409, Samantha 327, Lauren 337, Taylor 94, Jessica 303, Grace 83</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1871,12 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Lauren 8, Taylor 6, Samantha 18, Madison 14, Taylor 17</t>
+          <t>Lauren 363, Olivia 504, Alyssa 493, Emily 330, Madison 24, Brianna 221, Kayla 407, Emma 216, Taylor 6, Abigail 413, Sarah 31, Sarah 377, Elizabeth 174, Hannah 522, Taylor 226, Grace 285, Isabella 241, Lauren 52, Elizabeth 422, Abigail 490</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Ashley 478, Lauren 8, Taylor 94, Jessica 520, Jessica 303, Elizabeth 399, Taylor 523, Emily 91, Madison 14, Taylor 17</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1888,12 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Olivia 1, Samantha 18, Kayla 7</t>
+          <t>Emily 146, Lauren 49, Taylor 151, Taylor 121, Sarah 518, Ashley 460, Alexis 35, Lauren 309, Abigail 131, Sarah 377, Hannah 522, Olivia 1, Emily 87, Isabella 426, Lauren 430, Ashley 286</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Emma 448, Grace 89, Grace 30, Brianna 179, Taylor 145, Hannah 181, Lauren 29, Grace 122, Samantha 462, Samantha 18</t>
         </is>
       </c>
     </row>
@@ -1411,7 +1903,16 @@
           <t>Tänavakunst</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Alyssa 132, Alexis 104, Elizabeth 486, Brianna 433, Samantha 211, Isabella 342, Alyssa 306, Jessica 23, Grace 99, Lauren 96, Alexis 498, Taylor 509, Lauren 309, Emily 229, Hannah 397, Abigail 408, Emma 499, Lauren 90, Jessica 191, Ashley 240</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Kayla 252, Sarah 331, Emily 144, Emily 336, Olivia 318, Samantha 488, Jessica 325, Ashley 81, Brianna 456, Grace 292</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
paremini loetav logi fail
</commit_message>
<xml_diff>
--- a/õpetajateFail.xlsx
+++ b/õpetajateFail.xlsx
@@ -378,14 +378,10 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jessica 278, Madison 204, Alexis 370, Abigail 269, Olivia 137, Lauren 96, Madison 324, Isabella 427, Lauren 60, Alyssa 4, Jessica 46, Kayla 252, Abigail 490, Lauren 8, Emily 144, Olivia 318, Samantha 488, Brianna 148, Madison 14, Isabella 485, Alexis 443, Jessica 425, Grace 280, Emily 505, Madison 464, Abigail 109, Isabella 95</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Kayla 497, Grace 320, Kayla 5, Emily 405, Isabella 275, Olivia 270, Emily 135, Olivia 186, Brianna 197, Brianna 47</t>
-        </is>
-      </c>
+          <t>Lauren 8, Alyssa 4, Kayla 5, Madison 14</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -395,14 +391,10 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Jessica 423, Alyssa 435, Sarah 210, Alyssa 306, Elizabeth 476, Olivia 259, Ashley 453, Emily 229, Taylor 222, Ashley 50, Lauren 12, Elizabeth 449, Isabella 426, Samantha 327, Olivia 53, Emily 91, Sarah 315, Abigail 255, Olivia 234, Abigail 125, Jessica 44, Emily 439, Lauren 11, Madison 184, Madison 417, Samantha 150, Olivia 264</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Jessica 32, Grace 351, Lauren 494, Taylor 215, Taylor 176, Hannah 314, Madison 519, Kayla 75, Abigail 338, Emma 118</t>
-        </is>
-      </c>
+          <t>Lauren 12, Lauren 11</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -412,7 +404,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Jessica 278, Jessica 46, Lauren 8, Madison 417, Samantha 150, Alyssa 4</t>
+          <t>Lauren 8, Alyssa 4</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
@@ -425,14 +417,10 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Emily 349, Brianna 200, Brianna 513, Alyssa 421, Olivia 376, Madison 455, Elizabeth 10, Elizabeth 262, Taylor 158, Grace 256</t>
-        </is>
-      </c>
+          <t>Emma 9, Elizabeth 10</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -442,7 +430,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
+          <t>Emma 9, Elizabeth 10</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
@@ -455,7 +443,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lauren 363, Madison 204, Alexis 104, Elizabeth 486, Jessica 206, Elizabeth 516, Jessica 23, Madison 352, Lauren 367, Isabella 244, Emma 118, Elizabeth 472, Alexis 365, Emily 144, Alexis 261, Isabella 329, Ashley 195, Brianna 373, Elizabeth 364, Jessica 293, Abigail 291, Ashley 220, Olivia 451, Emma 9, Jessica 374, Ashley 283, Madison 149, Elizabeth 166, Samantha 484, Abigail 344</t>
+          <t>Emma 9, Elizabeth 10</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
@@ -466,16 +454,8 @@
           <t>Planimeetria alused</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Alyssa 493, Alyssa 233, Madison 352, Olivia 274, Jessica 383, Abigail 212, Isabella 244, Taylor 288, Elizabeth 399, Ashley 195, Madison 162, Grace 321, Grace 120, Elizabeth 284, Grace 263, Hannah 165, Grace 159, Brianna 513, Brianna 362, Sarah 501, Alexis 468, Abigail 71, Lauren 494, Lauren 56, Samantha 398, Madison 243, Alexis 470, Emma 185, Alyssa 304, Taylor 215</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Hannah 314, Brianna 61, Emma 64, Hannah 317, Ashley 326, Jessica 423, Emily 34, Taylor 288, Lauren 101, Lauren 248</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -483,11 +463,7 @@
           <t>3D-modelleerimine 3. periood</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Hannah 218, Elizabeth 174, Grace 515, Ashley 140, Lauren 346, Emma 58, Olivia 451, Grace 253, Isabella 63</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -496,11 +472,7 @@
           <t>3D-modelleerimine 5. periood</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Jessica 147, Grace 122, Grace 253, Elizabeth 157, Abigail 71, Samantha 27, Madison 519, Samantha 20</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -511,14 +483,10 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ashley 123, Alyssa 493, Taylor 151, Emma 216, Emma 238, Alyssa 508, Emma 98, Lauren 60, Alyssa 4, Abigail 108, Alyssa 19, Kayla 252, Madison 14, Alexis 343, Olivia 384, Emily 152, Sarah 315, Elizabeth 473, Lauren 249, Grace 280, Jessica 70, Brianna 179, Taylor 145, Jessica 44</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Emma 350, Elizabeth 328, Alexis 294, Jessica 374, Ashley 326, Hannah 165, Emma 217, Samantha 150, Jessica 32, Sarah 86</t>
-        </is>
-      </c>
+          <t>Alyssa 4, Kayla 5, Madison 14</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -528,14 +496,10 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Kayla 188, Hannah 218, Isabella 183, Emily 507, Emily 91, Grace 89, Ashley 412, Brianna 373, Taylor 145, Brianna 42, Sarah 482, Alexis 294, Brianna 492, Samantha 20, Alexis 112, Madison 196, Alyssa 128, Samantha 18, Hannah 266, Brianna 251, Sarah 86, Grace 320, Emily 349, Alyssa 421</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>Olivia 376, Olivia 124, Emily 333, Alexis 340, Kayla 268, Sarah 107, Hannah 393, Brianna 47, Taylor 176, Elizabeth 227</t>
-        </is>
-      </c>
+          <t>Samantha 18</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -545,14 +509,10 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Alyssa 435, Olivia 416, Olivia 137, Alexis 381, Sarah 74, Emma 216, Taylor 254, Madison 324, Lauren 90, Emma 28, Madison 173, Alyssa 19, Olivia 1, Alexis 365, Ashley 348, Isabella 426, Samantha 327, Ashley 286, Grace 83, Jessica 311, Jessica 325, Grace 292, Grace 267, Jessica 425</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>Elizabeth 473, Grace 321, Olivia 40, Emma 217, Lauren 101, Madison 196, Olivia 167, Ashley 246, Grace 351, Ashley 481</t>
-        </is>
-      </c>
+          <t>Olivia 1</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -562,14 +522,10 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Kayla 188, Jessica 206, Samantha 211, Lauren 232, Lauren 49, Alexis 498, Abigail 131, Ashley 50, Isabella 244, Madison 368, Emma 208, Lauren 360, Emma 28, Lauren 452</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>Ashley 193, Alexis 335, Isabella 160, Elizabeth 385, Elizabeth 399, Madison 14, Taylor 17, Brianna 456, Ashley 392, Alexis 443</t>
-        </is>
-      </c>
+          <t>Isabella 3, Kayla 5, Madison 14, Taylor 17, Alyssa 4, Samantha 18</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -579,14 +535,10 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Sarah 2, Kayla 15, Brianna 172, Olivia 103, Sarah 210, Alyssa 306, Alexis 498, Kayla 139, Madison 368, Elizabeth 67, Ashley 193, Samantha 302, Brianna 361, Grace 267, Emily 34, Sarah 156, Isabella 474, Olivia 496, Olivia 127, Samantha 462, Jessica 521</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Madison 417, Samantha 18, Lauren 310, Abigail 296, Alyssa 491, Jessica 175, Brianna 513, Emma 58, Isabella 347, Emily 479</t>
-        </is>
-      </c>
+          <t>Sarah 2, Kayla 15, Lauren 12</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -596,14 +548,10 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Lauren 85, Emily 228, Sarah 74, Madison 324, Emma 238, Alyssa 4, Kayla 139, Madison 368, Isabella 241, Elizabeth 422, Taylor 192, Isabella 426, Taylor 288, Grace 22, Jessica 325, Alexis 343</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>Alexis 443, Sarah 315, Jessica 44, Olivia 451, Emma 350, Abigail 341, Abigail 514, Hannah 182, Olivia 127, Kayla 497</t>
-        </is>
-      </c>
+          <t>Alyssa 4</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -613,14 +561,10 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Emily 146, Ashley 198, Samantha 211, Madison 24, Hannah 202, Grace 465, Alyssa 308, Alyssa 508, Abigail 212, Jessica 46, Kayla 252, Brianna 88, Alexis 335, Isabella 160, Ashley 478, Lauren 8, Emma 454, Jessica 147, Lauren 207, Brianna 361, Taylor 110, Samantha 276, Olivia 234, Elizabeth 328, Olivia 134, Grace 463, Brianna 492, Ashley 326, Samantha 20, Hannah 182, Lauren 372, Samantha 447, Grace 159, Elizabeth 166, Sarah 57, Olivia 154</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>Samantha 73, Abigail 231, Isabella 353, Isabella 275, Taylor 26, Brianna 388, Elizabeth 262, Alexis 80, Emma 55, Madison 519</t>
-        </is>
-      </c>
+          <t>Lauren 8, Kayla 15</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -630,14 +574,10 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Taylor 115, Brianna 433, Grace 465, Taylor 106, Ashley 50, Emma 208, Elizabeth 449, Alexis 365, Grace 285, Isabella 241, Grace 48, Kayla 410, Elizabeth 164, Jessica 70, Lauren 136, Alexis 371, Isabella 3, Samantha 483, Olivia 496, Madison 184</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>Abigail 105, Lauren 372, Lauren 223, Samantha 447, Alyssa 133, Samantha 224, Alyssa 491, Jessica 175, Elizabeth 43, Alyssa 421</t>
-        </is>
-      </c>
+          <t>Isabella 3</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -647,14 +587,10 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Emily 146, Samantha 211, Olivia 416, Grace 99, Taylor 509, Hannah 397, Abigail 408, Samantha 429, Isabella 354, Lauren 8, Kayla 409, Hannah 467, Sarah 114, Abigail 514, Lauren 11, Hannah 182, Ashley 414, Olivia 169, Lauren 101, Madison 196</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>Isabella 260, Madison 149, Samantha 386, Emily 403, Isabella 353, Brianna 388, Kayla 268, Kayla 466, Ashley 458, Brianna 47</t>
-        </is>
-      </c>
+          <t>Lauren 8, Lauren 11</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -662,16 +598,8 @@
           <t>Labortöid füüsikas 10. ja 11. klassile</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Hannah 59, Brianna 433, Madison 24, Lauren 232, Taylor 121, Grace 99, Taylor 106, Sarah 74, Olivia 274, Abigail 131, Kayla 139, Alyssa 39</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>Emma 28, Kayla 252, Elizabeth 422, Lauren 33, Alexis 171, Kayla 409, Samantha 488, Taylor 523, Emma 64, Grace 292</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -681,14 +609,10 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Isabella 342, Hannah 218, Madison 126, Madison 368, Elizabeth 67, Elizabeth 174, Samantha 429, Alyssa 359, Kayla 13, Emma 454, Taylor 523, Jessica 147, Ashley 392, Taylor 110, Jessica 293, Olivia 234, Jessica 44, Olivia 451, Lauren 459, Sarah 512, Taylor 130, Samantha 20, Grace 247, Hannah 266, Brianna 251, Alexis 69, Olivia 167, Sarah 86, Ashley 246, Samantha 73, Alyssa 432, Brianna 419, Ashley 389, Grace 253, Elizabeth 157, Samantha 178, Olivia 21, Grace 428, Brianna 388, Emma 76, Elizabeth 473, Sarah 424, Grace 515, Grace 256, Olivia 376</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>Emma 257, Elizabeth 227, Grace 159, Taylor 176, Abigail 71, Ashley 458, Olivia 154, Alexis 524, Abigail 131, Taylor 151</t>
-        </is>
-      </c>
+          <t>Kayla 13</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -696,16 +620,8 @@
           <t>Joonestamine 4. periood</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Alyssa 132, Samantha 27, Emma 142, Grace 99, Emma 216, Alyssa 366, Elizabeth 472, Elizabeth 174, Isabella 63, Isabella 375, Olivia 53, Lauren 430, Jessica 147, Emma 387, Jessica 425, Hannah 467, Kayla 272, Grace 463, Emily 439, Olivia 496, Ashley 326, Grace 122, Samantha 462, Jessica 189, Lauren 346, Alyssa 491, Emma 58, Kayla 7, Abigail 71, Brianna 438, Emma 77, Brianna 388, Lauren 170, Sarah 424, Grace 431, Alexis 470, Olivia 237, Alyssa 304, Samantha 178, Ashley 140, Madison 519, Madison 301, Abigail 177, Kayla 369, Brianna 88</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Hannah 181, Brianna 197, Taylor 226, Emma 142, Elizabeth 262, Ashley 198, Sarah 501, Alexis 171, Grace 411, Grace 263</t>
-        </is>
-      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -715,14 +631,10 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Samantha 27, Alyssa 435, Brianna 433, Hannah 218, Isabella 183, Emma 142, Taylor 106, Lauren 457, Samantha 402, Abigail 212, Emma 28, Alexis 335, Isabella 241, Elizabeth 422, Alexis 171, Isabella 375, Isabella 295, Ashley 412, Alexis 36, Alexis 112, Olivia 477, Emma 404, Grace 282, Elizabeth 116</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Olivia 376, Jessica 219, Kayla 51, Isabella 275, Sarah 277, Grace 111, Lauren 494, Grace 253, Hannah 16, Abigail 113</t>
-        </is>
-      </c>
+          <t>Hannah 16</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -732,14 +644,10 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Jessica 278, Emily 146, Hannah 194, Alyssa 233, Elizabeth 476, Olivia 259, Sarah 74, Brianna 153, Samantha 487, Abigail 131, Samantha 271, Lauren 33, Alexis 261, Lauren 489, Grace 83, Brianna 148, Hannah 357, Lauren 249, Samantha 382, Taylor 145, Brianna 42, Kayla 235, Emily 439, Taylor 130</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Olivia 40, Abigail 105, Ashley 414, Emma 217, Lauren 101, Hannah 266, Grace 159, Samantha 484, Hannah 287, Grace 511</t>
-        </is>
-      </c>
+          <t>Kayla 7, Kayla 13</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -749,14 +657,10 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Emily 37, Kayla 15, Ashley 198, Samantha 211, Lauren 49, Alexis 381, Emma 142, Jessica 506, Jessica 383, Alexis 316, Lauren 360, Jessica 191, Elizabeth 67, Kayla 252, Samantha 302, Lauren 489, Olivia 318, Brianna 148, Ashley 81, Olivia 384, Elizabeth 307, Isabella 485, Grace 292, Grace 30, Grace 267</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>Samantha 276, Jessica 70, Ashley 220, Hannah 332, Sarah 442, Emily 505, Alexis 36, Alexis 45, Grace 463, Abigail 105</t>
-        </is>
-      </c>
+          <t>Kayla 15</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -766,14 +670,10 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Emily 37, Elizabeth 436, Isabella 342, Alexis 381, Samantha 143, Ashley 453, Isabella 427, Ashley 50, Jessica 191, Isabella 426, Samantha 327, Olivia 318, Olivia 53, Emily 507, Grace 83, Brianna 148, Brianna 456, Isabella 485, Grace 30, Abigail 255, Hannah 357, Olivia 234</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>Brianna 492, Emma 290, Brianna 190, Alyssa 133, Ashley 246, Hannah 287, Grace 511, Kayla 7, Elizabeth 79, Olivia 270</t>
-        </is>
-      </c>
+          <t>Kayla 7</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -783,14 +683,10 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Ashley 123, Alyssa 493, Olivia 103, Brianna 221, Elizabeth 516, Taylor 121, Olivia 102, Alyssa 233, Ashley 50, Emma 208, Isabella 241, Olivia 318, Ashley 286, Abigail 517, Emma 448, Lauren 207, Hannah 129, Elizabeth 307, Jessica 70, Samantha 382, Alexis 371, Sarah 114, Olivia 451, Madison 225, Grace 321, Emma 9, Madison 184, Grace 263, Kayla 379</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>Samantha 250, Emily 390, Abigail 296, Olivia 167, Samantha 386, Elizabeth 116, Grace 351, Lauren 356, Jessica 230, Ashley 389</t>
-        </is>
-      </c>
+          <t>Emma 9</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -800,14 +696,10 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Alexis 370, Kayla 15, Jessica 206, Elizabeth 436, Brianna 203, Sarah 518, Alexis 62, Madison 324, Grace 199, Alexis 316, Isabella 244, Emma 401, Jessica 437, Emma 118, Olivia 345, Taylor 288, Alexis 471, Samantha 327, Olivia 53, Emma 454, Elizabeth 289, Emma 300, Isabella 329, Brianna 179, Ashley 220, Abigail 125, Abigail 341, Elizabeth 328, Samantha 483, Elizabeth 284, Samantha 250, Olivia 477, Lauren 258, Jessica 189, Grace 320, Brianna 513, Ashley 481, Olivia 376, Emily 403, Brianna 418, Madison 415, Emma 77, Abigail 177, Elizabeth 262, Olivia 214, Taylor 158, Alexis 470, Hannah 281, Brianna 47, Hannah 314</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>Brianna 179, Kayla 75, Brianna 190, Madison 415, Hannah 202, Kayla 369, Taylor 145, Brianna 92, Elizabeth 307, Sarah 501</t>
-        </is>
-      </c>
+          <t>Kayla 15, Kayla 5</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -817,14 +709,10 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Alexis 104, Kayla 15, Samantha 27, Elizabeth 436, Alyssa 306, Taylor 254, Samantha 487, Emily 445, Abigail 408, Lauren 367, Elizabeth 391, Alyssa 39, Isabella 354, Alexis 378, Lauren 475, Sarah 434, Emily 336, Isabella 295, Emily 507, Lauren 207, Taylor 17, Isabella 329, Elizabeth 307, Brianna 373, Emily 152</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>Samantha 276, Elizabeth 473, Ashley 297, Alyssa 128, Samantha 150, Jessica 189, Olivia 376, Madison 155, Isabella 353, Brianna 418</t>
-        </is>
-      </c>
+          <t>Kayla 15, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -834,14 +722,10 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Jessica 423, Isabella 183, Kayla 407, Taylor 6, Abigail 413, Lauren 457, Jessica 191, Emma 28, Lauren 248, Olivia 345, Abigail 108, Isabella 375, Kayla 409, Grace 83, Emily 91, Grace 267, Emily 34, Hannah 317, Alexis 36, Jessica 374, Brianna 492, Taylor 394, Lauren 101, Isabella 260, Elizabeth 166, Abigail 296, Lauren 358, Emma 404</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>Elizabeth 10, Elizabeth 79, Taylor 26, Ashley 117, Sarah 277, Alexis 340, Sarah 424, Madison 415, Emily 152, Kayla 369</t>
-        </is>
-      </c>
+          <t>Taylor 6, Elizabeth 10</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -851,14 +735,10 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Emily 37, Taylor 115, Madison 204, Alexis 381, Grace 100, Taylor 121, Ashley 453, Ashley 50, Ashley 193, Alyssa 359, Isabella 375, Grace 48, Jessica 311, Isabella 485, Grace 267, Jessica 70, Hannah 332, Hannah 181, Lauren 372, Olivia 127, Olivia 169, Samantha 150, Samantha 386, Samantha 68, Alyssa 491, Elizabeth 116, Madison 155, Ashley 84, Emily 97, Olivia 124, Taylor 26, Brianna 299, Sarah 424, Samantha 398, Grace 431, Alyssa 304, Samantha 178, Abigail 279, Olivia 41, Lauren 337, Ashley 392, Grace 463, Isabella 3, Grace 465, Hannah 16, Brianna 201, Samantha 276, Samantha 302, Olivia 21, Grace 111</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>Alexis 316, Lauren 452, Hannah 165, Jessica 230, Emily 507, Elizabeth 227, Alyssa 39, Olivia 259, Emma 185, Olivia 237</t>
-        </is>
-      </c>
+          <t>Hannah 16, Isabella 3</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -866,16 +746,8 @@
           <t>Astronoomia</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Alyssa 493, Brianna 172, Lauren 85, Taylor 151, Hannah 194, Alexis 381, Lauren 96, Emma 216, Lauren 60, Abigail 408, Elizabeth 67, Abigail 108, Jessica 461, Ashley 240, Samantha 429, Sarah 331, Alyssa 273, Taylor 94, Emily 507, Lauren 207, Emma 387, Ashley 412, Brianna 180, Madison 162, Alyssa 245, Lauren 459, Alexis 294, Kayla 379, Alyssa 128, Samantha 447</t>
-        </is>
-      </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>Lauren 310, Sarah 57, Olivia 138, Kayla 469, Brianna 419, Grace 253, Grace 431, Alexis 470, Brianna 197, Brianna 47</t>
-        </is>
-      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -883,16 +755,8 @@
           <t>Astrofüüsika 2. periood</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Emily 37, Ashley 123, Madison 54, Samantha 211, Hannah 202, Hannah 194, Abigail 338, Olivia 102, Grace 99, Olivia 259, Emma 238, Brianna 153, Samantha 402, Ashley 453, Emma 25, Brianna 201, Emma 401, Lauren 33, Alyssa 273, Elizabeth 385, Alexis 471, Emily 334, Taylor 94, Emma 64, Ashley 81, Brianna 456, Jessica 446, Sarah 442, Elizabeth 328, Emily 439, Emma 290, Madison 417, Samantha 484, Brianna 190, Jessica 219</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>Abigail 231, Emily 479, Olivia 138, Brianna 388, Alexis 80, Alexis 355, Kayla 466, Kayla 75, Grace 213, Brianna 179</t>
-        </is>
-      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -902,14 +766,10 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Alyssa 132, Alexis 104, Lauren 49, Kayla 407, Elizabeth 476, Alexis 35, Hannah 397, Lauren 360, Lauren 248, Abigail 108, Taylor 192, Grace 22, Brianna 373, Ashley 220, Abigail 341, Emma 9, Abigail 503, Samantha 483, Alexis 294, Lauren 29, Taylor 130, Isabella 95, Hannah 266, Madison 149, Abigail 296, Sarah 86, Grace 320, Hannah 287, Kayla 5, Elizabeth 43, Emma 72, Sarah 424, Alyssa 304, Taylor 215, Lauren 236</t>
-        </is>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>Elizabeth 307, Hannah 16, Kayla 272, Lauren 457, Alexis 171, Elizabeth 449, Lauren 309, Brianna 221, Grace 120, Emma 238</t>
-        </is>
-      </c>
+          <t>Kayla 5, Emma 9</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -919,14 +779,10 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Jessica 278, Madison 204, Alexis 370, Samantha 27, Jessica 206, Elizabeth 436, Isabella 183, Olivia 103, Sarah 210, Taylor 151, Emma 142, Taylor 121, Alyssa 233, Brianna 153, Alyssa 4, Grace 199, Abigail 408, Jessica 191, Elizabeth 67, Elizabeth 449</t>
-        </is>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>Alyssa 359, Alyssa 273, Elizabeth 385, Emily 336, Elizabeth 399, Brianna 456, Elizabeth 307, Isabella 485, Abigail 125, Olivia 502</t>
-        </is>
-      </c>
+          <t>Alyssa 4, Lauren 11</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -934,16 +790,8 @@
           <t>Loogika 2. periood</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Jessica 206, Ashley 198, Brianna 221, Sarah 210, Hannah 323, Taylor 509, Emma 98, Emily 229, Hannah 397, Lauren 360, Ashley 78, Ashley 240, Alexis 335, Isabella 63, Samantha 327, Abigail 517, Samantha 480, Hannah 129, Olivia 239, Sarah 482, Abigail 450, Olivia 40, Kayla 379, Jessica 163, Olivia 264, Emily 349, Jessica 265, Brianna 200, Jessica 230, Brianna 92, Olivia 214</t>
-        </is>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>Kayla 268, Ashley 168, Lauren 337, Olivia 318, Olivia 234, Brianna 92, Elizabeth 307, Samantha 483, Hannah 287, Abigail 231</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -953,14 +801,10 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sarah 2, Madison 204, Jessica 423, Hannah 194, Brianna 153, Samantha 402, Alexis 378, Sarah 331, Abigail 490, Lauren 33, Lauren 475, Alexis 261, Lauren 337, Grace 120, Lauren 459, Ashley 414, Alyssa 133, Emma 404, Abigail 344, Ashley 246, Elizabeth 141, Alyssa 440, Elizabeth 262, Alexis 80, Alexis 355, Ashley 168, Emma 55, Hannah 314, Ashley 441, Isabella 187, Madison 415</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>Emily 144, Sarah 107, Hannah 467, Lauren 232, Olivia 137, Alyssa 245, Abigail 82, Abigail 291, Samantha 402, Jessica 437</t>
-        </is>
-      </c>
+          <t>Sarah 2</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -968,11 +812,7 @@
           <t>Programmeerimine keeles Java 1</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>Olivia 318, Sarah 315, Isabella 485</t>
-        </is>
-      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
@@ -992,14 +832,10 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Olivia 504, Brianna 172, Olivia 416, Brianna 203, Grace 396, Jessica 23, Taylor 106, Sarah 74, Lauren 96, Lauren 457, Isabella 244, Alexis 365, Lauren 52, Elizabeth 422, Samantha 327, Olivia 384, Brianna 361, Abigail 255, Elizabeth 473, Emily 505, Abigail 109, Olivia 134, Sarah 512, Samantha 484, Jessica 32, Grace 282, Kayla 5, Emily 405, Kayla 469, Sarah 277</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>Olivia 214, Lauren 494, Samantha 398, Lauren 236, Madison 301, Ashley 510, Jessica 44, Grace 463, Olivia 318, Brianna 201</t>
-        </is>
-      </c>
+          <t>Kayla 5</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1009,14 +845,10 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Hannah 59, Lauren 49, Olivia 103, Taylor 151, Emma 142, Olivia 102, Lauren 457, Emma 238, Isabella 427, Alyssa 366, Elizabeth 391, Alyssa 39, Madison 368, Abigail 108, Alyssa 19, Alexis 365, Brianna 88, Alexis 171, Isabella 63, Lauren 430, Ashley 195, Elizabeth 307, Alexis 443, Jessica 425, Elizabeth 473, Abigail 291, Olivia 502, Brianna 180, Emma 350, Madison 225, Alexis 294, Sarah 512, Isabella 474, Emily 390, Ashley 246, Kayla 369, Emma 305, Kayla 51, Madison 322, Olivia 270, Grace 428, Alexis 80, Sarah 420, Olivia 186, Emma 185, Kayla 75, Taylor 215, Ashley 510, Jessica 44, Emily 152</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>Brianna 388, Hannah 181, Alexis 45, Elizabeth 262, Abigail 450, Hannah 281, Abigail 279, Brianna 42, Sarah 312, Alyssa 366</t>
-        </is>
-      </c>
+          <t>Elizabeth 10, Alyssa 4</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1026,14 +858,10 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Alyssa 435, Hannah 218, Isabella 183, Abigail 338, Alyssa 308, Grace 396, Samantha 143, Madison 126, Alyssa 508, Lauren 12, Elizabeth 472, Elizabeth 67, Madison 173, Lauren 452, Samantha 429, Isabella 160, Elizabeth 385, Emily 87, Kayla 409, Ashley 286, Alexis 343, Emma 387, Samantha 480, Sarah 315, Hannah 467, Abigail 255, Jessica 293, Emma 9, Lauren 459, Kayla 272, Lauren 11, Taylor 394, Jessica 163, Ashley 283, Elizabeth 166, Olivia 167, Jessica 175, Grace 282, Emily 405, Isabella 353, Jessica 230, Alyssa 432, Abigail 82, Alexis 340, Madison 243, Ashley 458, Sarah 107, Alyssa 339, Madison 301, Olivia 318</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>Brianna 362, Ashley 198, Elizabeth 472, Taylor 288, Lauren 309, Grace 263, Taylor 509, Grace 515, Jessica 374, Emma 387</t>
-        </is>
-      </c>
+          <t>Lauren 12, Emma 9, Lauren 11, Sarah 2, Olivia 1</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1041,16 +869,8 @@
           <t>Arvutite riistvara ja lisaseadmed</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Alexis 370, Abigail 131, Emily 229, Alexis 316, Emma 401, Madison 173, Alyssa 273, Taylor 288, Emily 334, Emma 454, Emma 448, Emma 387, Grace 89, Brianna 180, Brianna 42, Ashley 297</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Madison 464, Sarah 512, Grace 463, Alyssa 380, Grace 263, Lauren 372, Grace 247, Elizabeth 166, Alexis 69, Jessica 189</t>
-        </is>
-      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1058,16 +878,8 @@
           <t>Loodusteadused, tehnoloogia ja ühiskond</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Emily 146, Elizabeth 436, Samantha 211, Olivia 137, Emily 228, Elizabeth 476, Taylor 254, Emma 238, Lauren 60, Emily 445, Lauren 90, Sarah 377, Lauren 452, Isabella 160, Elizabeth 385, Emily 87, Emily 144, Jessica 311, Emily 152, Grace 280, Hannah 165, Emma 217, Jessica 521, Emma 305, Sarah 312</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>Elizabeth 79, Samantha 298, Grace 515, Brianna 419, Brianna 205, Taylor 215, Lauren 85, Samantha 68, Brianna 362, Emily 135</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1077,14 +889,10 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Lauren 49, Alyssa 308, Madison 126, Brianna 61, Alexis 35, Samantha 429, Ashley 193, Alexis 471, Emily 334, Ashley 392, Isabella 485, Elizabeth 364, Taylor 110, Sarah 156, Olivia 234, Alyssa 245, Abigail 514, Samantha 483, Taylor 130, Emma 290, Taylor 394, Ashley 283, Alexis 69, Jessica 219, Madison 155, Isabella 347, Isabella 275</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>Alexis 468, Alyssa 432, Abigail 177, Taylor 158, Hannah 16, Madison 243, Olivia 21, Kayla 75, Brianna 190, Lauren 337</t>
-        </is>
-      </c>
+          <t>Hannah 16, Olivia 1</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1094,14 +902,10 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>Abigail 503, Isabella 474, Lauren 93, Hannah 165, Isabella 95, Alexis 69, Alyssa 133, Samantha 386, Emma 305, Abigail 209</t>
-        </is>
-      </c>
+          <t>Taylor 6</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1111,7 +915,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
+          <t>Taylor 6</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -1124,7 +928,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Sarah 400, Kayla 188, Emily 330, Grace 100, Alyssa 233, Jessica 66, Taylor 6, Brianna 61, Ashley 460, Emma 499, Brianna 201, Lauren 248, Ashley 78, Lauren 452, Abigail 490, Hannah 129, Alexis 443, Taylor 110</t>
+          <t>Taylor 6</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -1135,16 +939,8 @@
           <t>Kirjandus ja film</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Sarah 400, Kayla 188, Emily 330, Olivia 416, Alyssa 308, Grace 100, Elizabeth 516, Samantha 143, Alexis 62, Alexis 316, Lauren 90, Elizabeth 472, Alyssa 19, Sarah 331, Alexis 171, Emma 387, Abigail 255, Hannah 357, Sarah 156, Abigail 291, Sarah 114, Alyssa 245, Hannah 332, Emma 350, Olivia 38, Kayla 235, Kayla 272, Olivia 169, Emily 390, Madison 149, Kayla 495, Samantha 386, Grace 282, Kayla 369</t>
-        </is>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Isabella 161, Emily 403, Madison 415, Emma 77, Abigail 82, Lauren 170, Grace 431, Sarah 107, Madison 519, Olivia 41</t>
-        </is>
-      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1154,14 +950,10 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Lauren 363, Olivia 504, Elizabeth 486, Hannah 59, Brianna 203, Alexis 381, Isabella 395, Emma 142, Jessica 23, Elizabeth 476, Jessica 506, Brianna 61, Samantha 271, Samantha 302, Ashley 348, Olivia 53, Elizabeth 289, Ashley 412, Lauren 249, Abigail 125, Olivia 502, Emma 9, Emma 217</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>Jessica 521, Lauren 346, Grace 511, Sarah 57, Emma 305, Elizabeth 141, Isabella 347, Madison 322, Elizabeth 313, Alexis 524</t>
-        </is>
-      </c>
+          <t>Emma 9</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1171,14 +963,10 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Sarah 2, Madison 24, Lauren 232, Lauren 85, Sarah 74, Alexis 498, Sarah 31, Alyssa 366, Lauren 12, Madison 319, Emma 118, Lauren 452, Taylor 226, Elizabeth 422, Taylor 192, Lauren 337, Grace 22, Jessica 311, Jessica 325, Alexis 343</t>
-        </is>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>Brianna 361, Emily 65, Abigail 341, Alyssa 380, Ashley 326, Samantha 250, Madison 196, Ashley 283, Olivia 477, Lauren 310</t>
-        </is>
-      </c>
+          <t>Sarah 2, Lauren 12, Hannah 16</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1188,14 +976,10 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Alyssa 435, Brianna 172, Olivia 103, Taylor 222, Grace 199, Emma 499, Kayla 139, Jessica 437, Brianna 88, Isabella 160, Alexis 261, Emma 300, Sarah 315, Hannah 467, Samantha 382, Ashley 220, Brianna 180, Abigail 503, Alexis 294, Alexis 45</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>Grace 463, Isabella 474, Lauren 11, Lauren 93, Alexis 112, Lauren 258, Ashley 481, Emma 58, Madison 455, Grace 515</t>
-        </is>
-      </c>
+          <t>Lauren 11</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1205,14 +989,10 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Samantha 27, Isabella 183, Alyssa 308, Emma 142, Sarah 518, Emma 98, Abigail 212, Jessica 46, Emma 401, Alyssa 19, Kayla 13, Elizabeth 385, Lauren 8, Brianna 148, Grace 30, Hannah 317</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Sarah 114, Alexis 36, Isabella 3, Samantha 20, Taylor 394, Olivia 169, Samantha 250, Emily 390, Olivia 154, Kayla 7</t>
-        </is>
-      </c>
+          <t>Kayla 13, Lauren 8, Isabella 3, Kayla 7</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1231,14 +1011,10 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Jessica 278, Emily 37, Isabella 342, Abigail 269, Abigail 338, Grace 396, Alexis 498, Taylor 509, Emma 25, Lauren 360, Madison 173, Taylor 192, Ashley 286, Abigail 517, Madison 14, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>Samantha 480, Ashley 81, Brianna 456, Grace 267, Sarah 442, Alyssa 380, Abigail 450, Olivia 496, Taylor 130, Samantha 462</t>
-        </is>
-      </c>
+          <t>Madison 14, Taylor 17, Kayla 5</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1255,16 +1031,8 @@
           <t>Lähis-Ida 20. sajandi teisest poolest tänapäevani</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Lauren 49, Brianna 221, Emily 228, Lauren 457, Madison 324, Emma 238, Lauren 90, Olivia 345, Brianna 88, Samantha 302, Alyssa 359, Lauren 52, Hannah 357, Grace 280, Taylor 145, Alexis 371, Brianna 42, Madison 225, Grace 321, Kayla 235, Alexis 45, Olivia 127, Emma 217, Lauren 346, Jessica 219, Brianna 362, Jessica 230, Alexis 468, Grace 515, Alyssa 432, Grace 428, Olivia 214, Emma 72, Alexis 355, Emma 55, Grace 213</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>Brianna 179, Madison 301, Ashley 392, Abigail 177, Elizabeth 307, Grace 267, Samantha 483, Olivia 134, Lauren 475, Elizabeth 449</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1274,14 +1042,10 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sarah 2, Madison 54, Hannah 218, Olivia 103, Olivia 416, Samantha 143, Madison 126, Alexis 35, Jessica 383, Hannah 397, Madison 368, Isabella 241, Emily 334, Isabella 375, Grace 22, Jessica 520, Elizabeth 289, Grace 83, Elizabeth 164, Isabella 485, Emily 65, Sarah 156, Lauren 249, Jessica 70, Abigail 514, Kayla 272, Lauren 29, Brianna 492, Olivia 40, Lauren 101, Abigail 296, Grace 320</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Ashley 481, Emily 403, Lauren 356, Sarah 501, Samantha 298, Emma 257, Emily 333, Kayla 268, Hannah 119, Olivia 237</t>
-        </is>
-      </c>
+          <t>Sarah 2</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1291,14 +1055,10 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Grace 89, Olivia 384, Elizabeth 307, Brianna 179, Grace 120, Sarah 482, Grace 263, Lauren 258, Emma 404, Hannah 287</t>
-        </is>
-      </c>
+          <t>Olivia 1</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1308,7 +1068,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
+          <t>Olivia 1</t>
         </is>
       </c>
       <c r="O60" t="inlineStr"/>
@@ -1321,7 +1081,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Hannah 202, Grace 465, Brianna 203, Isabella 395, Olivia 102, Lauren 309, Grace 199, Alyssa 366, Sarah 377, Olivia 1, Grace 285, Alexis 378, Sarah 434, Emily 336, Jessica 303, Elizabeth 399, Kayla 410, Emma 300, Jessica 147, Jessica 311</t>
+          <t>Olivia 1</t>
         </is>
       </c>
       <c r="O61" t="inlineStr"/>
@@ -1334,14 +1094,10 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Samantha 224, Samantha 68, Jessica 265, Alyssa 491, Grace 511, Abigail 231, Madison 155, Isabella 353, Ashley 84, Abigail 177</t>
-        </is>
-      </c>
+          <t>Samantha 18</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1351,7 +1107,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
+          <t>Samantha 18</t>
         </is>
       </c>
       <c r="O63" t="inlineStr"/>
@@ -1364,7 +1120,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Alyssa 132, Olivia 504, Hannah 323, Alexis 62, Taylor 254, Sarah 31, Madison 319, Jessica 437, Emma 208, Elizabeth 174, Hannah 522, Samantha 271, Emily 87, Ashley 478, Alexis 471, Isabella 63, Lauren 337, Grace 48, Lauren 430, Samantha 382, Olivia 502, Emily 505, Abigail 105, Lauren 223, Samantha 18</t>
+          <t>Samantha 18</t>
         </is>
       </c>
       <c r="O64" t="inlineStr"/>
@@ -1377,14 +1133,10 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alexis 370, Kayla 15, Ashley 123, Emily 146, Ashley 198, Jessica 506, Abigail 413, Alyssa 508, Samantha 487, Alyssa 4, Elizabeth 391, Jessica 191, Isabella 354, Ashley 193, Alexis 335, Lauren 475, Olivia 318, Emma 454</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>Emma 448, Ashley 392, Brianna 361, Emily 34, Elizabeth 473, Emma 350, Abigail 341, Ashley 297, Madison 464, Elizabeth 328</t>
-        </is>
-      </c>
+          <t>Kayla 15, Alyssa 4, Hannah 16</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1392,16 +1144,8 @@
           <t>Ajakirjanduse alused</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Kayla 188, Emily 330, Jessica 23, Ashley 460, Abigail 131, Kayla 139, Elizabeth 472, Olivia 345, Ashley 193, Sarah 331, Elizabeth 422, Alexis 261, Lauren 430, Kayla 410, Abigail 255, Jessica 293, Lauren 136, Alexis 371, Jessica 44, Olivia 38, Lauren 459, Olivia 239, Elizabeth 284, Olivia 496, Hannah 165, Lauren 223, Alyssa 128, Isabella 260, Jessica 189, Brianna 190, Alyssa 133</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Samantha 386, Jessica 175, Isabella 161, Olivia 376, Madison 155, Madison 322, Kayla 469, Madison 444, Madison 415, Taylor 158</t>
-        </is>
-      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1411,14 +1155,10 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Taylor 115, Jessica 423, Olivia 504, Abigail 338, Taylor 106, Lauren 457, Ashley 453, Emily 229, Emily 445, Emma 118, Emma 208, Sarah 377, Ashley 78, Ashley 240, Grace 285, Samantha 302, Emily 87, Taylor 288, Lauren 489, Olivia 53, Emily 507, Emma 300, Brianna 148, Ashley 81, Elizabeth 164, Jessica 70, Emily 505, Madison 464, Lauren 93, Taylor 394</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>Samantha 462, Emily 390, Samantha 18, Isabella 242, Lauren 258, Lauren 310, Kayla 495, Elizabeth 116, Emma 58, Sarah 312</t>
-        </is>
-      </c>
+          <t>Hannah 16, Samantha 18</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1426,11 +1166,7 @@
           <t>Filosoofia 2</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Taylor 106, Emily 445, Emma 208, Emily 507, Lauren 93</t>
-        </is>
-      </c>
+      <c r="E68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -1441,14 +1177,10 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Lauren 363, Brianna 433, Samantha 143, Sarah 518, Jessica 506, Jessica 383, Alyssa 39, Madison 319, Emma 401, Madison 368, Samantha 271, Sarah 434, Isabella 295, Jessica 520, Jessica 303, Samantha 488, Taylor 17, Ashley 195</t>
-        </is>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Olivia 384, Ashley 412, Grace 30, Grace 280, Brianna 179, Jessica 446, Madison 225, Samantha 250, Brianna 251, Lauren 346</t>
-        </is>
-      </c>
+          <t>Kayla 7, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1458,7 +1190,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Lauren 363, Brianna 433, Samantha 143, Sarah 518, Jessica 506, Jessica 383, Alyssa 39, Madison 319, Emma 401, Madison 368, Samantha 271, Sarah 434, Isabella 295, Jessica 520, Jessica 303, Samantha 488, Taylor 17, Ashley 195</t>
+          <t>Kayla 7, Taylor 17</t>
         </is>
       </c>
       <c r="O70" t="inlineStr"/>
@@ -1471,14 +1203,10 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Sarah 400, Ashley 123, Alyssa 493, Lauren 96, Taylor 509, Emma 98, Lauren 367, Ashley 50, Lauren 12, Isabella 244, Isabella 354, Lauren 33, Lauren 475, Kayla 409, Lauren 337, Abigail 517, Elizabeth 364, Hannah 467, Hannah 357, Lauren 249, Samantha 382, Brianna 180, Kayla 272, Jessica 374, Abigail 450, Isabella 474</t>
-        </is>
-      </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>Emily 439, Ashley 414, Kayla 379, Madison 417, Jessica 32, Lauren 358, Brianna 362, Olivia 270, Emily 97, Emma 257</t>
-        </is>
-      </c>
+          <t>Lauren 12, Taylor 6</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1488,14 +1216,10 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Sarah 2, Abigail 269, Hannah 194, Isabella 395, Hannah 323, Alyssa 306, Alexis 62, Madison 126, Brianna 61, Samantha 487, Isabella 427, Lauren 60, Brianna 201, Hannah 522, Samantha 429, Lauren 52, Abigail 490, Madison 14</t>
-        </is>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>Hannah 129, Sarah 114, Alyssa 245, Sarah 442, Alexis 36, Isabella 3, Abigail 514, Kayla 235, Sarah 512, Grace 263</t>
-        </is>
-      </c>
+          <t>Sarah 2, Isabella 3, Madison 14, Elizabeth 10</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1505,14 +1229,10 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Brianna 172, Brianna 221, Elizabeth 516, Madison 352, Abigail 413, Alexis 498, Olivia 274, Lauren 309, Sarah 31, Elizabeth 391, Emma 499, Jessica 437, Jessica 461, Alexis 378, Isabella 241, Kayla 13</t>
-        </is>
-      </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>Alexis 471, Emily 144, Emily 334, Elizabeth 289, Taylor 523, Emily 152, Madison 162, Emily 349, Brianna 513, Grace 515</t>
-        </is>
-      </c>
+          <t>Kayla 13</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1520,16 +1240,8 @@
           <t>Fotograafia 1</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Lauren 49, Alyssa 308, Lauren 96, Jessica 506, Abigail 413, Alexis 35, Brianna 153, Emily 445, Taylor 226, Isabella 160, Lauren 475, Grace 22, Jessica 520, Jessica 325, Samantha 480, Elizabeth 307, Jessica 425, Alexis 371, Hannah 181, Abigail 341, Lauren 459, Kayla 235, Olivia 134, Lauren 93</t>
-        </is>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>Samantha 20, Kayla 497, Ashley 481, Abigail 231, Madison 455, Sarah 501, Olivia 138, Alexis 355, Grace 431, Madison 243</t>
-        </is>
-      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1537,16 +1249,8 @@
           <t>Inimene ja ühiskond 3. periood</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>Jessica 423, Olivia 137, Abigail 338, Taylor 121, Madison 126, Samantha 487, Jessica 383, Elizabeth 391, Taylor 192, Taylor 94, Samantha 488, Emma 64, Emily 91, Ashley 81, Ashley 392, Emily 65, Kayla 272, Jessica 163, Grace 159, Lauren 258, Kayla 495, Grace 320, Jessica 265, Kayla 369, Jessica 230, Ashley 389, Ashley 117, Brianna 299, Emma 77, Abigail 82, Emma 72, Lauren 56, Grace 463, Ashley 198, Sarah 277, Olivia 270</t>
-        </is>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>Kayla 466, Ashley 481, Alyssa 491, Lauren 11, Madison 444, Samantha 211, Samantha 402, Madison 196, Sarah 482, Olivia 237</t>
-        </is>
-      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1556,14 +1260,10 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Madison 24, Emma 25, Taylor 222, Lauren 12, Elizabeth 289, Isabella 95, Kayla 379, Madison 417, Jessica 189, Jessica 32, Alyssa 491, Isabella 161, Isabella 275, Madison 444, Madison 415, Emma 257, Alexis 355, Lauren 494, Elizabeth 313, Brianna 197, Hannah 281, Elizabeth 227, Olivia 21, Kayla 51, Emma 76, Grace 411, Sarah 424, Grace 111, Hannah 393, Alyssa 440, Alexis 69, Grace 253, Olivia 237, Emily 349, Hannah 194, Ashley 441</t>
-        </is>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>Emily 390, Olivia 38, Sarah 377, Alyssa 493, Elizabeth 364, Jessica 325, Lauren 372, Emily 146, Abigail 209, Jessica 163</t>
-        </is>
-      </c>
+          <t>Lauren 12</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1573,14 +1273,10 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Jessica 278, Abigail 269, Kayla 407, Lauren 90, Alyssa 359, Samantha 276, Hannah 317, Lauren 136, Abigail 125, Madison 162, Alyssa 245, Sarah 442, Madison 225, Olivia 38, Isabella 3, Olivia 239, Sarah 482, Lauren 29, Abigail 450, Olivia 40, Taylor 394, Grace 122, Alyssa 128, Isabella 242, Brianna 251, Lauren 358, Sarah 57, Brianna 200, Grace 515, Kayla 469</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>Brianna 419, Brianna 438, Alexis 80, Sarah 107, Alyssa 304, Ashley 140, Grace 213, Lauren 85, Taylor 226, Olivia 234</t>
-        </is>
-      </c>
+          <t>Isabella 3</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1590,14 +1286,10 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Sarah 400, Kayla 15, Samantha 27, Brianna 221, Abigail 338, Isabella 395, Elizabeth 476, Jessica 506, Taylor 254, Abigail 413, Lauren 457, Brianna 153, Sarah 31, Jessica 46, Alexis 316, Elizabeth 391, Lauren 12, Jessica 437, Alexis 378, Kayla 252, Isabella 426, Lauren 475, Alexis 261, Emily 507, Emma 300, Brianna 148, Lauren 207, Emily 91, Brianna 361, Emily 65</t>
-        </is>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>Grace 267, Sarah 315, Emily 34, Hannah 357, Abigail 291, Brianna 179, Madison 225, Grace 321, Isabella 474, Emily 439</t>
-        </is>
-      </c>
+          <t>Lauren 12, Kayla 15, Elizabeth 10, Lauren 11</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1605,16 +1297,8 @@
           <t>Turundus</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Hannah 59, Lauren 232, Brianna 221, Olivia 259, Alyssa 39, Jessica 461, Ashley 240, Brianna 88, Lauren 52, Lauren 33, Ashley 348, Abigail 503, Taylor 130, Emily 390, Lauren 346, Alyssa 421, Emma 305, Madison 155, Elizabeth 141, Ashley 84, Alyssa 432, Emily 97, Abigail 71, Elizabeth 262, Taylor 158, Ashley 168</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>Samantha 398, Alexis 470, Kayla 75, Madison 301, Grace 411, Emma 76, Madison 415, Kayla 369, Alyssa 304, Hannah 317</t>
-        </is>
-      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1624,14 +1308,10 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Lauren 85, Grace 396, Elizabeth 476, Sarah 518, Sarah 74, Olivia 274, Elizabeth 449, Sarah 331, Kayla 13, Lauren 489, Abigail 517, Taylor 17, Hannah 332, Grace 120, Abigail 109, Elizabeth 284, Alexis 45, Emily 439, Madison 184, Samantha 250, Olivia 167, Samantha 68, Samantha 73, Lauren 356</t>
-        </is>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Brianna 362, Alexis 468, Madison 322, Samantha 298, Grace 428, Emma 257, Emily 333, Hannah 281, Taylor 500, Madison 519</t>
-        </is>
-      </c>
+          <t>Kayla 13, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1641,14 +1321,10 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Kayla 15, Elizabeth 486, Hannah 202, Lauren 85, Grace 100, Isabella 395, Alyssa 508, Emma 25, Taylor 222, Grace 199, Abigail 408, Lauren 12, Jessica 437, Emma 118, Lauren 248, Abigail 108, Taylor 226, Elizabeth 449, Isabella 426, Emily 336</t>
-        </is>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Jessica 325, Alexis 343, Grace 267, Alexis 443, Samantha 276, Jessica 293, Jessica 44, Olivia 239, Lauren 11, Elizabeth 166</t>
-        </is>
-      </c>
+          <t>Lauren 12, Kayla 15, Elizabeth 10, Lauren 11, Isabella 3</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1656,16 +1332,8 @@
           <t>Kujutav geomeetria</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Sarah 400, Hannah 59, Taylor 509, Emma 98, Ashley 453, Madison 173, Isabella 354, Kayla 252, Alyssa 273, Ashley 478, Taylor 288, Elizabeth 289, Emma 300, Isabella 329, Ashley 81, Grace 30, Emily 34, Lauren 136, Abigail 125, Jessica 446, Olivia 502, Madison 162</t>
-        </is>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Hannah 332, Hannah 181, Kayla 235, Madison 464, Elizabeth 328, Jessica 374, Isabella 95, Lauren 372, Grace 247, Lauren 101</t>
-        </is>
-      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1673,11 +1341,7 @@
           <t>Loominguline joonistamine 2</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Alexis 381, Samantha 302</t>
-        </is>
-      </c>
+      <c r="E83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
@@ -1688,14 +1352,10 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Taylor 115, Jessica 206, Madison 24, Sarah 210, Hannah 323, Jessica 66, Lauren 309, Emily 229, Grace 285, Kayla 13, Ashley 348, Kayla 409, Taylor 94, Grace 83, Taylor 523, Hannah 317, Lauren 249, Abigail 291, Brianna 180, Alexis 36, Elizabeth 284, Olivia 127, Olivia 169, Isabella 260, Grace 159, Hannah 287, Grace 511, Sarah 57, Brianna 200, Isabella 161, Samantha 73, Abigail 231, Emily 403, Isabella 353, Madison 322</t>
-        </is>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Emma 72, Lauren 56, Ashley 458, Abigail 279, Ashley 78, Ashley 392, Alyssa 304, Taylor 222, Alyssa 432, Taylor 6</t>
-        </is>
-      </c>
+          <t>Kayla 13, Taylor 6, Madison 14</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1705,14 +1365,10 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Jessica 278, Taylor 115, Alexis 370, Jessica 423, Ashley 123, Sarah 210, Grace 396, Grace 99, Lauren 96, Lauren 457, Lauren 60, Hannah 397, Elizabeth 391, Emma 28, Samantha 429, Alyssa 359, Kayla 13, Alyssa 273, Samantha 480, Grace 89, Brianna 361, Elizabeth 164, Olivia 234, Alyssa 245, Hannah 181, Ashley 297, Lauren 459, Elizabeth 284, Alyssa 380, Lauren 11, Lauren 372, Emma 217, Samantha 462, Olivia 477, Sarah 86, Samantha 224</t>
-        </is>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Jessica 265, Samantha 73, Emily 403, Isabella 353, Kayla 7, Madison 455, Sarah 501, Elizabeth 79, Grace 515, Abigail 71</t>
-        </is>
-      </c>
+          <t>Kayla 13, Kayla 7, Lauren 11</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1722,14 +1378,10 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Alyssa 435, Lauren 232, Brianna 221, Hannah 194, Elizabeth 476, Samantha 487, Abigail 408, Lauren 90, Emma 401, Lauren 8, Emily 334, Isabella 295, Emma 454, Jessica 520, Samantha 488</t>
-        </is>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>Kayla 410, Taylor 523, Taylor 17, Ashley 195, Sarah 156, Lauren 136, Sarah 114, Grace 321, Olivia 38, Olivia 239</t>
-        </is>
-      </c>
+          <t>Lauren 8, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1739,14 +1391,10 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Sarah 2, Brianna 433, Abigail 269, Olivia 137, Abigail 338, Samantha 143, Brianna 153, Samantha 402, Emily 445, Abigail 212, Isabella 160, Taylor 94, Abigail 517, Madison 14, Emma 387, Ashley 412, Emily 34, Hannah 317, Jessica 446, Brianna 42, Sarah 482, Abigail 109, Emily 439, Taylor 130</t>
-        </is>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>Grace 122, Alyssa 128, Isabella 260, Lauren 310, Samantha 484, Brianna 251, Ashley 246, Brianna 513, Alyssa 421, Jessica 219</t>
-        </is>
-      </c>
+          <t>Sarah 2, Madison 14</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1756,14 +1404,10 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Emily 146, Alyssa 493, Hannah 218, Olivia 103, Ashley 50, Taylor 226, Samantha 327, Emma 448, Ashley 392, Emily 152, Emily 65, Hannah 467, Abigail 255, Hannah 357, Elizabeth 473, Isabella 474, Emma 290, Ashley 414, Olivia 169, Lauren 101, Samantha 150, Lauren 346, Kayla 495, Samantha 386, Emily 349, Hannah 287, Grace 282, Kayla 5, Emma 305, Elizabeth 10, Kayla 469, Ashley 117, Alexis 340, Ashley 168, Olivia 186, Hannah 119, Ashley 458, Emma 185, Taylor 500, Grace 463, Lauren 310, Brianna 92, Emma 216, Kayla 272, Elizabeth 262, Olivia 138, Emily 135, Brianna 205, Kayla 497, Emily 479, Isabella 347, Sarah 114, Emma 72, Abigail 82, Grace 159, Taylor 176, Sarah 420, Jessica 265, Madison 225, Brianna 419, Brianna 492, Olivia 264, Hannah 266, Brianna 172, Brianna 47, Sarah 518, Alexis 294, Elizabeth 116, Brianna 299, Olivia 154, Elizabeth 385, Samantha 298, Elizabeth 157, Abigail 108, Brianna 513, Madison 455, Samantha 398, Hannah 332, Isabella 375, Kayla 75</t>
-        </is>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>Emily 65, Lauren 337, Jessica 325, Elizabeth 166, Emma 28, Isabella 426, Olivia 376, Ashley 460, Grace 282, Lauren 494</t>
-        </is>
-      </c>
+          <t>Kayla 5</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1771,11 +1415,7 @@
           <t>Riigikaitse 2</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Hannah 218, Taylor 226, Olivia 169, Samantha 150, Samantha 386, Ashley 392, Hannah 119, Ashley 414, Emma 185, Brianna 47, Alexis 294, Lauren 346, Elizabeth 10, Elizabeth 157, Olivia 138, Sarah 420, Elizabeth 262, Elizabeth 116, Emily 135, Emily 349, Hannah 266, Hannah 467, Kayla 272, Emily 152, Ashley 458</t>
-        </is>
-      </c>
+      <c r="E89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
@@ -1786,14 +1426,10 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Hannah 59, Isabella 183, Alyssa 308, Kayla 407, Alyssa 306, Taylor 121, Taylor 106, Abigail 413, Alexis 498, Olivia 274, Emily 229, Jessica 46, Olivia 345, Madison 173, Brianna 88, Lauren 52, Lauren 33, Kayla 409, Ashley 286, Lauren 207, Emily 91, Brianna 456, Jessica 425, Lauren 249, Taylor 145</t>
-        </is>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>Madison 225, Grace 120, Isabella 3, Samantha 483, Alexis 294, Kayla 272, Abigail 450, Olivia 496, Brianna 492, Ashley 326</t>
-        </is>
-      </c>
+          <t>Hannah 16, Isabella 3</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1801,16 +1437,8 @@
           <t>Ajakirjanduse praktika</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Emily 330, Jessica 23, Ashley 460, Emily 229, Isabella 375, Taylor 523, Abigail 255, Hannah 317, Jessica 70, Alexis 36, Brianna 190, Grace 511, Samantha 73, Lauren 309, Hannah 165, Alexis 371, Emily 334, Isabella 161, Brianna 200, Brianna 492, Jessica 189, Elizabeth 284, Samantha 143, Emily 403, Kayla 13, Lauren 223, Lauren 136, Olivia 345, Isabella 353, Alyssa 128</t>
-        </is>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>Brianna 88, Lauren 207, Elizabeth 141, Emily 144, Kayla 409, Jessica 461, Emily 479, Emma 499, Ashley 414, Elizabeth 307</t>
-        </is>
-      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1820,14 +1448,10 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Jessica 278, Alexis 370, Elizabeth 436, Madison 54, Isabella 342, Hannah 323, Taylor 6, Alexis 35, Samantha 487, Hannah 397, Taylor 222, Grace 199, Brianna 201, Lauren 90, Elizabeth 67, Elizabeth 174, Jessica 461, Hannah 522, Alyssa 359, Isabella 241, Abigail 490, Taylor 288, Emily 336, Olivia 318, Olivia 53, Grace 48, Jessica 147, Grace 89, Ashley 195, Olivia 384</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>Isabella 485, Lauren 249, Taylor 145, Alyssa 245, Hannah 181, Ashley 297, Lauren 459, Grace 463, Grace 263, Hannah 165</t>
-        </is>
-      </c>
+          <t>Taylor 6, Kayla 13</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1837,14 +1461,10 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Sarah 2, Alexis 104, Elizabeth 486, Madison 24, Abigail 269, Hannah 202, Olivia 103, Sarah 210, Alyssa 308, Kayla 407, Taylor 121, Sarah 74, Madison 126, Emma 98, Lauren 60, Kayla 139, Alyssa 39, Jessica 191</t>
-        </is>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>Alyssa 19, Samantha 429, Grace 285, Brianna 88, Alexis 171, Ashley 348, Taylor 192, Alexis 471, Lauren 8, Emily 334</t>
-        </is>
-      </c>
+          <t>Sarah 2, Lauren 8</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1854,14 +1474,10 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Alyssa 132, Taylor 115, Ashley 123, Alyssa 435, Alyssa 493, Olivia 416, Grace 100, Emily 228, Grace 99, Taylor 509, Samantha 402, Jessica 383, Alyssa 366, Emma 499, Emma 118, Ashley 78</t>
-        </is>
-      </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>Olivia 345, Olivia 1, Samantha 271, Emily 87, Kayla 409, Samantha 327, Lauren 337, Taylor 94, Jessica 303, Grace 83</t>
-        </is>
-      </c>
+          <t>Olivia 1, Hannah 16, Emma 9, Kayla 7</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1871,14 +1487,10 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Lauren 363, Olivia 504, Alyssa 493, Emily 330, Madison 24, Brianna 221, Kayla 407, Emma 216, Taylor 6, Abigail 413, Sarah 31, Sarah 377, Elizabeth 174, Hannah 522, Taylor 226, Grace 285, Isabella 241, Lauren 52, Elizabeth 422, Abigail 490</t>
-        </is>
-      </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>Ashley 478, Lauren 8, Taylor 94, Jessica 520, Jessica 303, Elizabeth 399, Taylor 523, Emily 91, Madison 14, Taylor 17</t>
-        </is>
-      </c>
+          <t>Taylor 6, Lauren 8, Samantha 18, Madison 14, Taylor 17</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1888,14 +1500,10 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Emily 146, Lauren 49, Taylor 151, Taylor 121, Sarah 518, Ashley 460, Alexis 35, Lauren 309, Abigail 131, Sarah 377, Hannah 522, Olivia 1, Emily 87, Isabella 426, Lauren 430, Ashley 286</t>
-        </is>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>Emma 448, Grace 89, Grace 30, Brianna 179, Taylor 145, Hannah 181, Lauren 29, Grace 122, Samantha 462, Samantha 18</t>
-        </is>
-      </c>
+          <t>Olivia 1, Samantha 18, Kayla 7</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1903,16 +1511,8 @@
           <t>Tänavakunst</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Alyssa 132, Alexis 104, Elizabeth 486, Brianna 433, Samantha 211, Isabella 342, Alyssa 306, Jessica 23, Grace 99, Lauren 96, Alexis 498, Taylor 509, Lauren 309, Emily 229, Hannah 397, Abigail 408, Emma 499, Lauren 90, Jessica 191, Ashley 240</t>
-        </is>
-      </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>Kayla 252, Sarah 331, Emily 144, Emily 336, Olivia 318, Samantha 488, Jessica 325, Ashley 81, Brianna 456, Grace 292</t>
-        </is>
-      </c>
+      <c r="E97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
paari kommentaari lisamine ja muud parandused
</commit_message>
<xml_diff>
--- a/õpetajateFail.xlsx
+++ b/õpetajateFail.xlsx
@@ -378,10 +378,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lauren 8, Alyssa 4, Kayla 5, Madison 14</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
+          <t>Kayla 252, Alexis 370, Jessica 278, Lauren 96, Olivia 137, Lauren 8, Abigail 269, Madison 204, Alyssa 4, Jessica 46, Abigail 490, Isabella 427, Madison 324, Lauren 60, Emily 144, Emily 405, Kayla 5, Madison 14, Grace 320, Olivia 186, Brianna 47, Emily 505, Isabella 485, Abigail 109, Olivia 270, Isabella 275, Emma 76</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Emily 135, Samantha 488, Kayla 497, Madison 464, Brianna 197, Olivia 318, Alexis 443, Grace 280, Isabella 187, Isabella 95</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -391,10 +395,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lauren 12, Lauren 11</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr"/>
+          <t>Alyssa 435, Lauren 12, Taylor 222, Isabella 426, Elizabeth 449, Elizabeth 476, Olivia 259, Jessica 423, Sarah 210, Ashley 50, Ashley 453, Alyssa 306, Emily 229, Emily 91, Lauren 494, Sarah 315, Hannah 314, Madison 519, Olivia 234, Jessica 32, Abigail 125, Madison 184, Emily 439, Taylor 215, Abigail 255, Samantha 327, Samantha 150</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Jessica 44, Taylor 176, Grace 351, Olivia 264, Olivia 53, Madison 417, Lauren 11, Olivia 477, Emily 390, Ashley 117</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -404,7 +412,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Lauren 8, Alyssa 4</t>
+          <t>Jessica 278, Lauren 8, Jessica 46, Samantha 150, Olivia 270, Alyssa 4</t>
         </is>
       </c>
       <c r="O4" t="inlineStr"/>
@@ -417,10 +425,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emma 9, Elizabeth 10</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr"/>
+          <t>Lauren 363, Isabella 244, Elizabeth 516, Madison 204, Jessica 206, Alexis 365, Emma 118, Lauren 367, Madison 352, Elizabeth 486, Elizabeth 472, Jessica 23, Alexis 104, Emily 144, Ashley 458, Taylor 500, Abigail 291, Jessica 374, Jessica 293, Olivia 451, Brianna 373, Taylor 158, Emily 349, Madison 149, Grace 256, Abigail 406, Brianna 200, Samantha 484, Madison 455, Elizabeth 262</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Emma 9, Alyssa 421, Isabella 329, Brianna 513, Alexis 261, Ashley 220, Elizabeth 166, Ashley 195, Ashley 283, Abigail 344</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -430,7 +442,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Emma 9, Elizabeth 10</t>
+          <t>Lauren 363, Isabella 244, Elizabeth 516, Madison 204, Jessica 206, Alexis 365, Emma 118, Lauren 367, Madison 352, Elizabeth 486, Elizabeth 472, Jessica 23, Alexis 104, Emily 144, Ashley 458, Taylor 500, Abigail 291, Jessica 374, Jessica 293, Olivia 451, Brianna 373, Taylor 158, Emily 349, Madison 149, Grace 256, Abigail 406, Brianna 200, Samantha 484, Madison 455, Elizabeth 262</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
@@ -443,7 +455,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Emma 9, Elizabeth 10</t>
+          <t>Lauren 363, Isabella 244, Elizabeth 516, Madison 204, Jessica 206, Alexis 365, Emma 118, Lauren 367, Madison 352, Elizabeth 486, Elizabeth 472, Jessica 23, Alexis 104, Emily 144, Ashley 458, Taylor 500, Abigail 291, Jessica 374, Jessica 293, Olivia 451, Brianna 373, Taylor 158, Emily 349, Madison 149, Grace 256, Abigail 406, Brianna 200, Samantha 484, Madison 455, Elizabeth 262</t>
         </is>
       </c>
       <c r="O7" t="inlineStr"/>
@@ -454,8 +466,16 @@
           <t>Planimeetria alused</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Taylor 288, Olivia 274, Isabella 244, Alyssa 233, Madison 352, Alyssa 493, Jessica 383, Abigail 212, Lauren 56, Lauren 494, Grace 263, Hannah 314, Grace 321, Sarah 501, Abigail 71, Alexis 468, Grace 120, Brianna 362, Emma 185, Taylor 215, Alexis 470, Elizabeth 399, Brianna 513, Samantha 398, Grace 159, Elizabeth 284, Hannah 165, Ashley 195, Madison 162, Alyssa 304</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Madison 243, Abigail 514, Hannah 323, Hannah 317, Jessica 423, Lauren 101, Alexis 355, Alexis 443, Emma 300, Sarah 442</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -463,7 +483,11 @@
           <t>3D-modelleerimine 3. periood</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Elizabeth 174, Hannah 218, Lauren 346, Olivia 53, Ashley 140, Emma 58, Olivia 451, Isabella 63, Grace 253</t>
+        </is>
+      </c>
       <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -472,7 +496,11 @@
           <t>3D-modelleerimine 5. periood</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Grace 122, Elizabeth 157, Jessica 147, Grace 253, Abigail 71, Samantha 20, Samantha 27, Taylor 176, Madison 519, Grace 463, Sarah 501</t>
+        </is>
+      </c>
       <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -483,10 +511,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Alyssa 4, Kayla 5, Madison 14</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr"/>
+          <t>Taylor 151, Emma 98, Emma 238, Kayla 252, Alyssa 508, Alyssa 4, Emma 216, Alyssa 493, Alyssa 19, Ashley 123, Abigail 108, Lauren 60, Elizabeth 328, Kayla 5, Sarah 315, Jessica 70, Madison 14, Alexis 343, Emma 217, Hannah 393, Samantha 224, Ashley 326, Lauren 249, Abigail 177</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Alexis 294, Jessica 32, Emily 152, Grace 256, Taylor 110, Emily 135, Lauren 170, Brianna 418, Samantha 382, Madison 415</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -496,10 +528,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr"/>
+          <t>Kayla 188, Isabella 183, Hannah 218, Hannah 266, Emily 91, Alexis 340, Olivia 124, Samantha 20, Grace 320, Hannah 393, Brianna 373, Alexis 294, Emily 349, Emily 507, Emma 76, Emily 333, Kayla 268, Brianna 251, Alyssa 128, Brianna 42, Sarah 86, Alyssa 421, Brianna 492, Grace 89</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Alexis 112, Taylor 145, Samantha 18, Taylor 176, Grace 213, Sarah 482, Madison 196, Ashley 412, Sarah 107, Elizabeth 227</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -509,10 +545,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr"/>
+          <t>Olivia 1, Alyssa 435, Taylor 254, Isabella 426, Olivia 416, Alexis 381, Olivia 137, Alexis 365, Madison 173, Lauren 90, Emma 216, Emma 28, Alyssa 19, Sarah 74, Madison 324, Ashley 348, Brianna 92, Ashley 286, Ashley 481, Alyssa 432, Emma 217, Grace 321, Brianna 47, Grace 83</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Sarah 501, Grace 267, Ashley 246, Jessica 230, Grace 111, Alyssa 440, Grace 431, Madison 455, Jessica 325, Lauren 356</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -522,10 +562,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Isabella 3, Kayla 5, Madison 14, Taylor 17, Alyssa 4, Samantha 18</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr"/>
+          <t>Lauren 232, Isabella 160, Emma 208, Abigail 131, Lauren 452, Samantha 211, Alexis 335, Isabella 244, Elizabeth 385, Ashley 193, Kayla 188, Jessica 206, Madison 368, Emma 28</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Lauren 49, Ashley 50, Alexis 498, Lauren 360, Lauren 93, Emily 405, Emma 257, Emma 290, Kayla 5, Madison 14</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -535,10 +579,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Sarah 2, Kayla 15, Lauren 12</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr"/>
+          <t>Sarah 2, Olivia 103, Ashley 193, Kayla 15, Sarah 210, Madison 368, Kayla 139, Samantha 302, Alexis 498, Elizabeth 67, Brianna 172, Alyssa 306, Abigail 296, Jessica 175, Sarah 156, Olivia 124, Ashley 441, Alyssa 491, Lauren 310, Olivia 496, Grace 267</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Emma 300, Emily 34, Isabella 474, Olivia 502, Olivia 127, Emma 58, Jessica 521, Brianna 513, Samantha 18, Brianna 361</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -548,10 +596,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Alyssa 4</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr"/>
+          <t>Taylor 288, Elizabeth 422, Isabella 241, Emma 238, Isabella 426, Alyssa 4, Madison 368, Taylor 192, Kayla 139, Sarah 74, Emily 228, Madison 324, Lauren 85, Abigail 514, Ashley 140, Sarah 315</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Lauren 337, Ashley 481, Alexis 343, Grace 320, Alexis 80, Olivia 451, Brianna 47, Abigail 231, Abigail 341, Sarah 312</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -561,10 +613,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Lauren 8, Kayla 15</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr"/>
+          <t>Isabella 160, Madison 24, Brianna 88, Kayla 252, Alyssa 508, Grace 465, Hannah 202, Samantha 211, Alexis 335, Lauren 8, Ashley 478, Alyssa 308, Jessica 46, Emily 146, Abigail 212, Ashley 198, Grace 463, Elizabeth 328, Isabella 353, Samantha 73, Lauren 372, Taylor 26, Madison 519, Olivia 234, Samantha 20, Alexis 80, Ashley 326, Abigail 231, Samantha 276, Sarah 57, Emma 55, Jessica 147, Taylor 110, Isabella 275, Elizabeth 262, Samantha 447</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Grace 411, Lauren 207, Brianna 492, Olivia 154, Hannah 182, Grace 159, Olivia 134, Emma 454, Elizabeth 166, Brianna 388</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -574,10 +630,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Isabella 3</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr"/>
+          <t>Isabella 241, Emma 208, Grace 465, Brianna 433, Elizabeth 449, Alexis 365, Grace 285, Ashley 50, Taylor 106, Taylor 115, Jessica 175, Lauren 223, Olivia 237, Grace 48, Abigail 113, Jessica 70, Abigail 105, Lauren 372, Sarah 420, Samantha 224</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Alyssa 491, Olivia 496, Alyssa 133, Madison 184, Kayla 469, Lauren 356, Samantha 447, Elizabeth 164, Lauren 136, Alyssa 421</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -587,10 +647,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Lauren 8, Lauren 11</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr"/>
+          <t>Grace 99, Taylor 509, Samantha 211, Olivia 416, Lauren 8, Emily 146, Isabella 354, Hannah 397, Abigail 408, Samantha 429, Hannah 467, Abigail 514, Emily 403, Brianna 47, Kayla 409, Olivia 169, Samantha 386, Isabella 260, Ashley 414, Kayla 268</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Isabella 329, Samantha 483, Sarah 114, Hannah 182, Madison 196, Brianna 388, Lauren 101, Ashley 510, Lauren 11, Emma 448</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -598,8 +662,16 @@
           <t>Labortöid füüsikas 10. ja 11. klassile</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Elizabeth 422, Lauren 232, Grace 99, Madison 24, Abigail 131, Kayla 252, Lauren 33, Brianna 433, Olivia 274, Alexis 171, Emma 28, Alyssa 39</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Taylor 121, Hannah 59, Taylor 106, Kayla 139, Sarah 74, Elizabeth 116, Hannah 467, Emma 64, Emily 405, Taylor 523</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -609,10 +681,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Kayla 13</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr"/>
+          <t>Madison 126, Alyssa 359, Isabella 342, Elizabeth 174, Madison 368, Kayla 13, Samantha 429, Hannah 218, Elizabeth 67, Hannah 266, Ashley 389, Samantha 73, Taylor 523, Alexis 69, Jessica 293, Olivia 234, Samantha 20, Alyssa 432, Olivia 21, Olivia 451, Ashley 246, Lauren 459, Elizabeth 157, Ashley 392, Jessica 147, Taylor 110, Brianna 419, Brianna 251, Sarah 86, Taylor 130, Jessica 44, Emma 454, Samantha 178, Sarah 512, Grace 253, Olivia 167, Grace 247, Brianna 388, Elizabeth 227, Madison 464, Sarah 424, Olivia 376, Olivia 53, Ashley 458, Taylor 176</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Lauren 236, Elizabeth 486, Brianna 221, Olivia 154, Madison 352, Emma 76, Hannah 165, Elizabeth 473, Emma 25, Grace 159</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -620,8 +696,16 @@
           <t>Joonestamine 4. periood</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Grace 99, Emma 142, Alyssa 132, Alyssa 366, Emma 216, Elizabeth 174, Elizabeth 472, Isabella 63, Samantha 27, Hannah 467, Olivia 237, Grace 463, Ashley 140, Madison 519, Isabella 375, Lauren 430, Ashley 326, Alyssa 491, Grace 122, Olivia 496, Abigail 71, Kayla 272, Jessica 147, Grace 431, Emily 439, Lauren 170, Emma 77, Jessica 189, Emma 58, Alexis 470, Kayla 7, Emma 387, Samantha 178, Brianna 388, Brianna 438, Olivia 53, Samantha 462, Lauren 346, Sarah 424, Alyssa 304, Jessica 425, Alexis 335, Brianna 88, Ashley 84, Sarah 501</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Taylor 226, Elizabeth 262, Jessica 278, Madison 464, Jessica 383, Lauren 459, Emily 97, Alyssa 132, Brianna 197, Taylor 130</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -631,10 +715,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Hannah 16</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr"/>
+          <t>Elizabeth 422, Isabella 241, Lauren 457, Alyssa 435, Emma 142, Brianna 433, Alexis 335, Alexis 171, Samantha 402, Isabella 183, Emma 28, Taylor 106, Abigail 212, Hannah 218, Samantha 27, Elizabeth 116, Lauren 494, Hannah 129, Grace 282, Hannah 16, Isabella 295, Isabella 375, Jessica 219, Sarah 277</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Grace 111, Isabella 275, Taylor 215, Olivia 477, Alexis 112, Grace 253, Emily 336, Kayla 51, Ashley 412, Elizabeth 364</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -644,10 +732,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Kayla 7, Kayla 13</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr"/>
+          <t>Abigail 131, Jessica 278, Lauren 33, Elizabeth 476, Alyssa 233, Olivia 259, Samantha 271, Emily 146, Hannah 194, Sarah 74, Samantha 487, Brianna 153, Olivia 237, Hannah 266, Abigail 105, Lauren 489, Emma 217, Lauren 249, Grace 83, Grace 511, Grace 256, Samantha 484, Kayla 235, Alexis 468</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Emily 439, Hannah 357, Emily 135, Ashley 414, Samantha 382, Kayla 7, Brianna 42, Alyssa 421, Brianna 197, Taylor 130</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -657,10 +749,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Kayla 15</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr"/>
+          <t>Kayla 252, Jessica 506, Emma 142, Samantha 211, Alexis 381, Kayla 15, Emily 37, Alexis 316, Lauren 49, Jessica 383, Samantha 302, Ashley 198, Lauren 360, Elizabeth 67, Jessica 191, Abigail 296, Olivia 237, Grace 30, Grace 463, Hannah 266, Ashley 389, Jessica 70, Alexis 45, Lauren 489, Samantha 20</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Lauren 430, Elizabeth 307, Alexis 524, Jessica 163, Emily 505, Samantha 276, Grace 267, Isabella 485, Elizabeth 157, Sarah 442</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -670,10 +766,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Kayla 7</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr"/>
+          <t>Isabella 426, Alexis 381, Elizabeth 436, Isabella 342, Emily 37, Isabella 427, Ashley 50, Jessica 191, Ashley 453, Samantha 143, Olivia 237, Grace 30, Emma 290, Sarah 420, Olivia 234, Alexis 524, Brianna 190, Grace 83, Grace 511, Brianna 456, Alyssa 133, Ashley 246</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Isabella 485, Elizabeth 157, Emily 507, Olivia 270, Hannah 357, Abigail 255, Kayla 7, Samantha 327, Brianna 492, Olivia 318</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -683,10 +783,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Emma 9</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr"/>
+          <t>Isabella 241, Emma 208, Olivia 102, Brianna 221, Olivia 103, Elizabeth 516, Alyssa 233, Alyssa 493, Taylor 121, Ashley 50, Ashley 123, Abigail 296, Elizabeth 116, Ashley 389, Jessica 70, Hannah 129, Grace 263, Ashley 286, Grace 321, Elizabeth 307, Olivia 451, Elizabeth 157, Jessica 230, Samantha 386, Madison 184, Emma 448, Lauren 356, Emily 390, Emma 9</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Lauren 207, Kayla 379, Samantha 382, Olivia 318, Samantha 250, Sarah 114, Grace 351, Madison 225, Abigail 517, Olivia 167</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -696,10 +800,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Kayla 15, Kayla 5</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr"/>
+          <t>Grace 199, Taylor 288, Olivia 345, Alexis 370, Isabella 244, Brianna 203, Jessica 206, Elizabeth 436, Kayla 15, Emma 118, Sarah 518, Alexis 316, Alexis 471, Emma 401, Madison 324, Alexis 62, Jessica 437, Elizabeth 328, Emily 403, Hannah 314, Ashley 481, Grace 320, Abigail 177, Brianna 47, Taylor 158, Abigail 125, Abigail 341, Emma 300, Lauren 258, Hannah 281, Elizabeth 262, Emma 77, Brianna 418, Jessica 189, Elizabeth 289, Alexis 470, Madison 415, Samantha 327, Olivia 477, Isabella 329, Brianna 513, Samantha 483, Samantha 250, Emma 454, Brianna 179, Elizabeth 284, Ashley 220, Olivia 214, Olivia 53, Olivia 376</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Olivia 477, Lauren 11, Sarah 512, Brianna 92, Madison 415, Olivia 103, Emily 439, Brianna 179, Abigail 341, Emma 55</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -709,10 +817,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Kayla 15, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr"/>
+          <t>Emily 445, Taylor 254, Alexis 378, Elizabeth 391, Elizabeth 436, Kayla 15, Lauren 367, Isabella 354, Alyssa 39, Abigail 408, Lauren 475, Alexis 104, Samantha 27, Samantha 487, Alyssa 306, Ashley 84, Emma 257, Isabella 353, Sarah 434, Isabella 295, Ashley 441, Elizabeth 307, Brianna 373, Taylor 158, Emily 152</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Samantha 276, Abigail 406, Emily 507, Hannah 281, Ashley 297, Madison 155, Brianna 418, Jessica 189, Grace 411, Brianna 205</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -722,10 +834,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Taylor 6, Elizabeth 10</t>
-        </is>
-      </c>
-      <c r="O30" t="inlineStr"/>
+          <t>Kayla 407, Lauren 248, Olivia 345, Abigail 413, Lauren 457, Jessica 423, Isabella 183, Emma 28, Taylor 6, Abigail 108, Jessica 191, Abigail 296, Emily 91, Alexis 340, Taylor 26, Emma 404, Jessica 374, Taylor 394, Isabella 375, Grace 83, Kayla 409, Sarah 277, Grace 267, Emily 34, Isabella 260, Brianna 492, Lauren 358, Ashley 117</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Elizabeth 166, Elizabeth 79, Sarah 424, Elizabeth 10, Lauren 101, Alexis 36, Hannah 317, Grace 396, Sarah 107, Samantha 462</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -735,10 +851,14 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hannah 16, Isabella 3</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr"/>
+          <t>Ashley 193, Alexis 381, Madison 204, Alyssa 359, Emily 37, Taylor 121, Ashley 50, Ashley 453, Taylor 115, Grace 100, Olivia 41, Elizabeth 116, Ashley 84, Hannah 181, Grace 48, Jessica 70, Lauren 372, Taylor 26, Olivia 124, Isabella 375, Alyssa 491, Grace 267, Isabella 485, Olivia 169, Samantha 386, Grace 431, Madison 155, Jessica 311, Samantha 68, Abigail 279, Olivia 127, Brianna 299, Hannah 332, Samantha 150, Samantha 398, Samantha 178, Sarah 424, Alyssa 304, Emily 97, Emily 507, Ashley 392, Olivia 21, Elizabeth 227, Lauren 337, Hannah 16, Taylor 110, Lauren 346, Grace 465, Abigail 406, Isabella 3</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Olivia 237, Lauren 8, Samantha 302, Abigail 131, Emily 333, Hannah 165, Grace 22, Taylor 115, Alyssa 39, Grace 463</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -746,8 +866,16 @@
           <t>Astronoomia</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Taylor 151, Ashley 240, Lauren 96, Alexis 381, Jessica 461, Alyssa 273, Emma 216, Alyssa 493, Abigail 408, Hannah 194, Samantha 429, Sarah 331, Abigail 108, Elizabeth 67, Brianna 172, Lauren 85, Lauren 60, Taylor 94, Alexis 524, Brianna 47, Alexis 294, Lauren 310, Brianna 180, Lauren 459, Sarah 57, Grace 431, Kayla 469, Emily 507, Samantha 447, Brianna 419</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Lauren 207, Kayla 379, Alexis 470, Alyssa 128, Alyssa 245, Brianna 197, Emma 387, Olivia 138, Grace 253, Alyssa 339</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -755,8 +883,16 @@
           <t>Astrofüüsika 2. periood</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Grace 99, Olivia 102, Emma 238, Hannah 202, Lauren 33, Brianna 201, Samantha 211, Elizabeth 385, Abigail 338, Samantha 402, Olivia 259, Emily 37, Alyssa 273, Madison 54, Emma 25, Ashley 123, Hannah 194, Emily 334, Alexis 471, Emma 401, Ashley 453, Brianna 153, Emma 64, Emma 290, Elizabeth 328, Kayla 466, Alexis 355, Taylor 94, Alexis 80, Jessica 219, Kayla 75, Brianna 190, Brianna 456, Abigail 231, Samantha 484</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Sarah 442, Emily 439, Ashley 81, Grace 213, Olivia 138, Brianna 388, Emily 479, Madison 417, Jessica 446, Ashley 348</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -766,10 +902,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Kayla 5, Emma 9</t>
-        </is>
-      </c>
-      <c r="O34" t="inlineStr"/>
+          <t>Kayla 407, Lauren 248, Alexis 35, Alyssa 132, Elizabeth 476, Lauren 49, Taylor 192, Hannah 397, Abigail 108, Alexis 104, Lauren 360, Abigail 296, Hannah 266, Kayla 5, Grace 320, Brianna 373, Alexis 294, Madison 149, Abigail 341, Abigail 503, Grace 22, Emma 9, Taylor 215, Sarah 86, Taylor 130, Samantha 483, Emma 72, Lauren 236, Ashley 220, Hannah 287, Elizabeth 43, Sarah 424, Alyssa 304, Lauren 29, Isabella 95</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Brianna 203, Lauren 309, Isabella 187, Hannah 323, Abigail 341, Hannah 16, Emma 55, Abigail 125, Jessica 278, Elizabeth 449</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -779,10 +919,14 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Alyssa 4, Lauren 11</t>
-        </is>
-      </c>
-      <c r="O35" t="inlineStr"/>
+          <t>Grace 199, Taylor 151, Alexis 370, Jessica 278, Emma 142, Elizabeth 385, Olivia 103, Elizabeth 449, Alyssa 233, Madison 204, Alyssa 359, Jessica 206, Elizabeth 436, Alyssa 4, Alyssa 273, Sarah 210, Isabella 183, Taylor 121, Abigail 408, Samantha 27</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Elizabeth 67, Jessica 191, Brianna 153, Ashley 140, Lauren 494, Ashley 458, Kayla 466, Olivia 124, Olivia 21, Elizabeth 307</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -790,8 +934,16 @@
           <t>Loogika 2. periood</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="O36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Taylor 509, Emma 98, Ashley 240, Alexis 335, Brianna 221, Jessica 206, Ashley 78, Sarah 210, Hannah 397, Isabella 63, Ashley 198, Lauren 360, Hannah 323, Emily 229, Brianna 92, Hannah 129, Olivia 239, Jessica 265, Jessica 163, Emily 349, Brianna 200, Jessica 230, Kayla 379, Kayla 268, Samantha 327, Olivia 264, Sarah 482, Ashley 168, Olivia 214, Abigail 517, Abigail 450</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Olivia 40, Samantha 480, Isabella 63, Emily 445, Samantha 483, Isabella 260, Brianna 92, Alexis 381, Lauren 337, Grace 282</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -801,10 +953,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sarah 2</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr"/>
+          <t>Lauren 33, Alexis 378, Sarah 2, Samantha 402, Madison 204, Jessica 423, Abigail 490, Hannah 194, Lauren 475, Sarah 331, Brianna 153, Elizabeth 141, Emma 404, Hannah 314, Lauren 337, Alexis 355, Alexis 80, Alyssa 133, Ashley 246, Lauren 459, Emma 55, Alyssa 440, Grace 120, Elizabeth 262, Ashley 414, Alexis 261, Isabella 187, Abigail 344, Samantha 480, Sarah 107, Madison 415</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Lauren 232, Emily 144, Olivia 504, Abigail 82, Olivia 137, Hannah 194, Hannah 467, Elizabeth 43, Kayla 407, Alyssa 421</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -812,7 +968,11 @@
           <t>Programmeerimine keeles Java 1</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Sarah 315, Hannah 314, Emily 405, Isabella 485</t>
+        </is>
+      </c>
       <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
@@ -832,10 +992,14 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Kayla 5</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr"/>
+          <t>Elizabeth 422, Grace 396, Lauren 457, Lauren 96, Isabella 244, Olivia 416, Brianna 203, Alexis 365, Lauren 52, Taylor 106, Sarah 74, Jessica 23, Brianna 172, Olivia 504, Emily 405, Lauren 494, Kayla 5, Grace 282, Jessica 32, Emily 505, Sarah 277, Samantha 484, Abigail 109, Kayla 469, Abigail 255, Samantha 327, Elizabeth 473, Samantha 398, Olivia 134, Madison 301</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Lauren 236, Sarah 512, Olivia 214, Brianna 361, Olivia 384, Ashley 510, Samantha 462, Grace 280, Sarah 114, Alexis 62</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -845,10 +1009,14 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Elizabeth 10, Alyssa 4</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr"/>
+          <t>Taylor 151, Brianna 88, Olivia 102, Emma 238, Lauren 457, Emma 142, Elizabeth 391, Olivia 103, Alexis 171, Alyssa 366, Alexis 365, Madison 368, Isabella 427, Alyssa 39, Lauren 49, Alyssa 19, Hannah 59, Isabella 63, Abigail 108, Abigail 291, Sarah 420, Alexis 80, Lauren 430, Elizabeth 307, Olivia 186, Kayla 75, Alexis 294, Brianna 180, Ashley 246, Olivia 270, Kayla 369, Isabella 474, Olivia 502, Emma 185, Emily 390, Madison 322, Taylor 215, Emma 350, Grace 428, Elizabeth 473, Sarah 512, Madison 225, Alexis 443, Ashley 195, Emma 305, Kayla 51, Jessica 425, Ashley 510, Brianna 388, Sarah 312</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Alyssa 366, Abigail 279, Hannah 181, Lauren 90, Emma 9, Alyssa 491, Samantha 484, Alexis 381, Alexis 355, Grace 30</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -858,10 +1026,14 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Lauren 12, Emma 9, Lauren 11, Sarah 2, Olivia 1</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr"/>
+          <t>Isabella 160, Madison 126, Grace 396, Alyssa 508, Lauren 452, Alyssa 435, Lauren 12, Elizabeth 385, Abigail 338, Emily 87, Madison 173, Alyssa 308, Isabella 183, Elizabeth 472, Samantha 429, Hannah 218, Elizabeth 67, Samantha 143, Jessica 175, Hannah 467, Emily 405, Ashley 458, Isabella 353, Sarah 315, Alexis 340, Grace 282, Ashley 286, Taylor 394, Jessica 293, Alexis 343, Alyssa 432, Jessica 163, Kayla 409, Lauren 459, Jessica 230, Kayla 272, Emma 9, Abigail 255, Madison 301, Emma 387, Elizabeth 166, Alyssa 339, Olivia 167, Ashley 283, Sarah 107, Abigail 82, Samantha 480, Madison 243, Lauren 11, Samantha 382</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Jessica 265, Grace 263, Emma 387, Alexis 335, Sarah 482, Olivia 1, Taylor 394, Isabella 161, Abigail 209, Abigail 82</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -869,8 +1041,16 @@
           <t>Arvutite riistvara ja lisaseadmed</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="O43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Taylor 288, Abigail 131, Alexis 370, Madison 173, Alyssa 273, Alexis 316, Emily 334, Emma 401, Emily 229, Grace 463, Brianna 92, Lauren 372, Taylor 26, Alexis 69, Brianna 180, Isabella 161</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Emma 55, Emma 448, Alyssa 380, Ashley 297, Jessica 189, Hannah 119, Brianna 205, Madison 464, Brianna 42, Grace 89</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -878,8 +1058,16 @@
           <t>Loodusteadused, tehnoloogia ja ühiskond</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Isabella 160, Sarah 377, Emily 445, Emma 238, Lauren 452, Taylor 254, Samantha 211, Elizabeth 385, Olivia 137, Elizabeth 476, Emily 87, Elizabeth 436, Lauren 90, Emily 146, Emily 228, Lauren 60, Emily 144, Emma 217, Emily 152, Grace 515, Sarah 312, Jessica 311, Brianna 419, Brianna 205, Taylor 215</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Jessica 521, Hannah 165, Samantha 298, Elizabeth 79, Grace 280, Emma 305, Brianna 172, Madison 54, Ashley 412, Hannah 129</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -889,10 +1077,14 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Hannah 16, Olivia 1</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr"/>
+          <t>Madison 126, Alexis 35, Ashley 193, Alyssa 308, Lauren 49, Emily 334, Samantha 429, Brianna 61, Alexis 471, Abigail 514, Emma 290, Sarah 156, Hannah 16, Alexis 69, Taylor 394, Olivia 234, Alyssa 432, Olivia 21, Jessica 219, Abigail 177, Taylor 158, Isabella 485, Ashley 392, Alexis 468, Taylor 110, Isabella 275, Madison 155</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Alyssa 245, Taylor 130, Samantha 483, Ashley 283, Isabella 347, Elizabeth 364, Madison 243, Isabella 187, Emily 65, Olivia 186</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -902,10 +1094,14 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr"/>
+          <t>Lauren 248, Sarah 400, Lauren 452, Emily 330, Brianna 201, Alyssa 233, Kayla 188, Ashley 460, Ashley 78, Abigail 490, Emma 499, Jessica 66, Taylor 6, Brianna 61, Grace 100, Olivia 41, Lauren 93, Abigail 113</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Hannah 129, Alexis 69, Sarah 277, Alyssa 133, Abigail 71, Elizabeth 157, Samantha 386, Abigail 503, Taylor 110, Isabella 474</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -915,7 +1111,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
+          <t>Lauren 248, Sarah 400, Lauren 452, Emily 330, Brianna 201, Alyssa 233, Kayla 188, Ashley 460, Ashley 78, Abigail 490, Emma 499, Jessica 66, Taylor 6, Brianna 61, Grace 100, Olivia 41, Lauren 93, Abigail 113</t>
         </is>
       </c>
       <c r="O47" t="inlineStr"/>
@@ -928,7 +1124,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Taylor 6</t>
+          <t>Lauren 248, Sarah 400, Lauren 452, Emily 330, Brianna 201, Alyssa 233, Kayla 188, Ashley 460, Ashley 78, Abigail 490, Emma 499, Jessica 66, Taylor 6, Brianna 61, Grace 100, Olivia 41, Lauren 93, Abigail 113</t>
         </is>
       </c>
       <c r="O48" t="inlineStr"/>
@@ -939,8 +1135,16 @@
           <t>Kirjandus ja film</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Sarah 400, Emily 330, Olivia 416, Alexis 171, Elizabeth 516, Kayla 188, Alyssa 308, Lauren 90, Alexis 316, Elizabeth 472, Alyssa 19, Sarah 331, Alexis 62, Grace 100, Samantha 143, Olivia 41, Sarah 156, Abigail 291, Grace 282, Emily 403, Madison 519, Kayla 495, Madison 149, Olivia 38, Isabella 161, Olivia 169, Samantha 386, Kayla 272, Grace 431, Kayla 235, Kayla 369, Hannah 357, Lauren 170, Emma 77</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Emily 390, Madison 415, Abigail 255, Emma 350, Alyssa 245, Hannah 332, Sarah 114, Emma 387, Sarah 107, Abigail 82</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -950,10 +1154,14 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Emma 9</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr"/>
+          <t>Isabella 395, Lauren 363, Jessica 506, Emma 142, Alexis 381, Brianna 203, Elizabeth 476, Samantha 271, Elizabeth 486, Hannah 59, Samantha 302, Brianna 61, Jessica 23, Olivia 504, Ashley 348, Elizabeth 141, Emma 217, Alexis 524, Lauren 249, Abigail 125, Grace 511, Sarah 57, Olivia 502</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Elizabeth 313, Emma 9, Elizabeth 289, Madison 322, Jessica 521, Olivia 53, Lauren 346, Emma 305, Ashley 412, Isabella 347</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -963,10 +1171,14 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Sarah 2, Lauren 12, Hannah 16</t>
-        </is>
-      </c>
-      <c r="O51" t="inlineStr"/>
+          <t>Elizabeth 422, Lauren 232, Madison 24, Sarah 31, Lauren 452, Lauren 12, Sarah 2, Alyssa 366, Emma 118, Taylor 226, Taylor 192, Sarah 74, Alexis 498, Madison 319, Lauren 85, Ashley 140, Hannah 16, Olivia 124, Lauren 337, Alexis 343</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Hannah 393, Ashley 326, Lauren 310, Jessica 32, Abigail 341, Sarah 312, Jessica 325, Grace 22, Alyssa 380, Elizabeth 262</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -976,10 +1188,14 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Lauren 11</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr"/>
+          <t>Grace 199, Isabella 160, Brianna 88, Alyssa 435, Taylor 222, Olivia 103, Emma 499, Kayla 139, Brianna 172, Jessica 437, Hannah 467, Lauren 93, Grace 463, Sarah 315, Alexis 45, Ashley 481, Alexis 294, Brianna 180, Grace 256, Grace 515</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Abigail 503, Emma 300, Madison 455, Lauren 258, Isabella 474, Hannah 119, Emma 58, Samantha 382, Alexis 112, Alexis 261</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -989,10 +1205,14 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Kayla 13, Lauren 8, Isabella 3, Kayla 7</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr"/>
+          <t>Emma 98, Emma 142, Elizabeth 385, Lauren 8, Sarah 518, Alyssa 308, Jessica 46, Isabella 183, Alyssa 19, Kayla 13, Abigail 212, Emma 401, Samantha 27, Grace 30, Taylor 26, Olivia 124</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Ashley 441, Taylor 394, Samantha 20, Olivia 186, Olivia 169, Emily 390, Madison 415, Kayla 7, Olivia 154, Samantha 250</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1011,10 +1231,14 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Madison 14, Taylor 17, Kayla 5</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr"/>
+          <t>Taylor 509, Grace 396, Jessica 278, Abigail 269, Abigail 338, Isabella 342, Emily 37, Madison 173, Emma 25, Taylor 192, Alexis 498, Lauren 360, Brianna 92, Madison 14, Sarah 420, Ashley 286</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Hannah 393, Brianna 456, Olivia 496, Kayla 495, Grace 267, Sarah 442, Ashley 81, Alyssa 380, Emma 77, Abigail 279</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1031,8 +1255,16 @@
           <t>Lähis-Ida 20. sajandi teisest poolest tänapäevani</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Olivia 345, Brianna 88, Emma 238, Lauren 457, Brianna 221, Alyssa 359, Lauren 90, Lauren 49, Lauren 52, Samantha 302, Emily 228, Madison 324, Alexis 45, Alyssa 432, Alexis 355, Emma 217, Grace 321, Jessica 219, Grace 515, Jessica 230, Emma 55, Kayla 235, Alexis 468, Brianna 362, Hannah 357, Olivia 127, Grace 428, Brianna 42, Taylor 145, Grace 213, Emma 72, Madison 225, Olivia 214, Grace 280, Lauren 346, Alexis 371</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Brianna 172, Sarah 312, Emma 448, Samantha 483, Ashley 392, Abigail 177, Lauren 475, Samantha 382, Samantha 480, Brianna 492</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1042,10 +1274,14 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sarah 2</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr"/>
+          <t>Isabella 241, Madison 126, Alexis 35, Sarah 2, Olivia 416, Olivia 103, Madison 54, Madison 368, Jessica 383, Hannah 397, Emily 334, Hannah 218, Samantha 143, Abigail 296, Olivia 237, Abigail 514, Emma 257, Jessica 70, Sarah 156, Jessica 520, Emily 403, Ashley 481, Isabella 375, Grace 320, Lauren 249, Grace 83, Sarah 501, Isabella 485, Kayla 272, Emma 76, Grace 22, Emma 185</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Lauren 356, Emily 65, Hannah 119, Elizabeth 289, Grace 411, Emily 333, Kayla 268, Elizabeth 164, Brianna 492, Samantha 298</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1055,10 +1291,14 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr"/>
+          <t>Grace 199, Sarah 377, Isabella 395, Olivia 102, Olivia 1, Grace 465, Hannah 202, Alexis 378, Brianna 203, Alyssa 366, Grace 285, Lauren 309, Elizabeth 141, Emma 404, Sarah 434, Grace 263, Elizabeth 307, Kayla 75, Jessica 303, Emma 300</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Jessica 147, Lauren 258, Grace 120, Isabella 275, Kayla 369, Elizabeth 313, Lauren 170, Jessica 311, Elizabeth 399, Grace 89</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1068,7 +1308,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
+          <t>Grace 199, Sarah 377, Isabella 395, Olivia 102, Olivia 1, Grace 465, Hannah 202, Alexis 378, Brianna 203, Alyssa 366, Grace 285, Lauren 309, Elizabeth 141, Emma 404, Sarah 434, Grace 263, Elizabeth 307, Kayla 75, Jessica 303, Emma 300</t>
         </is>
       </c>
       <c r="O60" t="inlineStr"/>
@@ -1081,7 +1321,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Olivia 1</t>
+          <t>Grace 199, Sarah 377, Isabella 395, Olivia 102, Olivia 1, Grace 465, Hannah 202, Alexis 378, Brianna 203, Alyssa 366, Grace 285, Lauren 309, Elizabeth 141, Emma 404, Sarah 434, Grace 263, Elizabeth 307, Kayla 75, Jessica 303, Emma 300</t>
         </is>
       </c>
       <c r="O61" t="inlineStr"/>
@@ -1094,10 +1334,14 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr"/>
+          <t>Emma 208, Sarah 31, Taylor 254, Alyssa 132, Ashley 478, Emily 87, Samantha 271, Elizabeth 174, Hannah 522, Isabella 63, Alexis 471, Hannah 323, Madison 319, Alexis 62, Olivia 504, Jessica 437, Lauren 223, Ashley 84, Grace 48, Kayla 466, Isabella 353, Abigail 105, Lauren 337, Olivia 21, Lauren 430</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Jessica 265, Samantha 224, Abigail 177, Alyssa 491, Grace 511, Abigail 231, Emily 505, Olivia 502, Madison 155, Samantha 68</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1107,7 +1351,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
+          <t>Emma 208, Sarah 31, Taylor 254, Alyssa 132, Ashley 478, Emily 87, Samantha 271, Elizabeth 174, Hannah 522, Isabella 63, Alexis 471, Hannah 323, Madison 319, Alexis 62, Olivia 504, Jessica 437, Lauren 223, Ashley 84, Grace 48, Kayla 466, Isabella 353, Abigail 105, Lauren 337, Olivia 21, Lauren 430</t>
         </is>
       </c>
       <c r="O63" t="inlineStr"/>
@@ -1120,7 +1364,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Samantha 18</t>
+          <t>Emma 208, Sarah 31, Taylor 254, Alyssa 132, Ashley 478, Emily 87, Samantha 271, Elizabeth 174, Hannah 522, Isabella 63, Alexis 471, Hannah 323, Madison 319, Alexis 62, Olivia 504, Jessica 437, Lauren 223, Ashley 84, Grace 48, Kayla 466, Isabella 353, Abigail 105, Lauren 337, Olivia 21, Lauren 430</t>
         </is>
       </c>
       <c r="O64" t="inlineStr"/>
@@ -1133,10 +1377,14 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Kayla 15, Alyssa 4, Hannah 16</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr"/>
+          <t>Abigail 413, Alyssa 508, Alexis 370, Jessica 506, Alexis 335, Elizabeth 391, Ashley 193, Kayla 15, Alyssa 4, Emily 146, Isabella 354, Ashley 123, Lauren 475, Ashley 198, Jessica 191, Samantha 487, Jessica 175, Hannah 266</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Ashley 140, Ashley 389, Emma 290, Elizabeth 328, Samantha 73, Grace 282, Ashley 326, Brianna 190, Grace 122, Abigail 341</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1144,8 +1392,16 @@
           <t>Ajakirjanduse alused</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
-      <c r="O66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Elizabeth 422, Olivia 345, Abigail 131, Emily 330, Ashley 193, Kayla 188, Ashley 460, Elizabeth 472, Kayla 139, Jessica 23, Sarah 331, Jessica 175, Lauren 223, Jessica 293, Olivia 239, Lauren 430, Brianna 190, Taylor 158, Olivia 496, Alyssa 133, Olivia 38, Isabella 161, Lauren 459, Samantha 386, Kayla 469, Isabella 260, Madison 155, Jessica 189, Madison 322, Madison 415, Abigail 255</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Alyssa 128, Lauren 136, Kayla 410, Jessica 44, Alexis 261, Madison 301, Madison 444, Samantha 178, Elizabeth 284, Hannah 165</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1155,10 +1411,14 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Hannah 16, Samantha 18</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr"/>
+          <t>Taylor 288, Sarah 377, Emma 208, Emily 445, Lauren 457, Ashley 240, Abigail 338, Emily 87, Emma 118, Jessica 423, Ashley 78, Grace 285, Taylor 106, Samantha 302, Olivia 504, Ashley 453, Taylor 115, Emily 229, Elizabeth 116, Lauren 93, Ashley 84, Taylor 500, Jessica 70, Hannah 16, Lauren 489, Taylor 394, Lauren 310, Kayla 495, Emily 505, Abigail 406</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>Emma 300, Sarah 312, Lauren 258, Emily 507, Ashley 81, Hannah 281, Emily 390, Emma 58, Isabella 242, Madison 464</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1166,7 +1426,11 @@
           <t>Filosoofia 2</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Emma 208, Emily 445, Taylor 106, Lauren 93, Kayla 495, Lauren 310</t>
+        </is>
+      </c>
       <c r="O68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -1177,10 +1441,14 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Kayla 7, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O69" t="inlineStr"/>
+          <t>Lauren 363, Jessica 506, Brianna 433, Samantha 271, Sarah 518, Madison 368, Alyssa 39, Jessica 383, Emma 401, Madison 319, Samantha 143, Grace 30, Jessica 520, Sarah 434, Isabella 295, Ashley 441, Jessica 303, Grace 511</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Abigail 71, Emma 185, Elizabeth 313, Brianna 419, Brianna 205, Alexis 470, Samantha 488, Kayla 7, Brianna 251, Taylor 17</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1190,7 +1458,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Kayla 7, Taylor 17</t>
+          <t>Lauren 363, Jessica 506, Brianna 433, Samantha 271, Sarah 518, Madison 368, Alyssa 39, Jessica 383, Emma 401, Madison 319, Samantha 143, Grace 30, Jessica 520, Sarah 434, Isabella 295, Ashley 441, Jessica 303, Grace 511</t>
         </is>
       </c>
       <c r="O70" t="inlineStr"/>
@@ -1203,10 +1471,14 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Lauren 12, Taylor 6</t>
-        </is>
-      </c>
-      <c r="O71" t="inlineStr"/>
+          <t>Taylor 509, Emma 98, Sarah 400, Lauren 33, Lauren 12, Lauren 96, Isabella 244, Lauren 367, Alyssa 493, Isabella 354, Ashley 50, Ashley 123, Lauren 475, Hannah 467, Emma 257, Alexis 340, Jessica 374, Lauren 337, Alexis 524, Olivia 186, Lauren 249, Kayla 409, Jessica 32, Brianna 180, Kayla 272, Emily 439</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Olivia 270, Brianna 362, Isabella 474, Hannah 357, Ashley 414, Hannah 119, Abigail 279, Kayla 379, Samantha 382, Lauren 358</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1216,10 +1488,14 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Sarah 2, Isabella 3, Madison 14, Elizabeth 10</t>
-        </is>
-      </c>
-      <c r="O72" t="inlineStr"/>
+          <t>Isabella 395, Madison 126, Brianna 201, Sarah 2, Abigail 269, Abigail 490, Isabella 427, Hannah 522, Lauren 52, Hannah 194, Samantha 429, Brianna 61, Hannah 323, Alexis 62, Samantha 487, Alyssa 306, Lauren 60, Olivia 41</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>Abigail 514, Elizabeth 141, Abigail 113, Hannah 129, Madison 14, Grace 282, Emily 403, Grace 263, Alyssa 491, Sarah 277</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1229,10 +1505,14 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Kayla 13</t>
-        </is>
-      </c>
-      <c r="O73" t="inlineStr"/>
+          <t>Isabella 241, Abigail 413, Sarah 31, Alexis 378, Olivia 274, Brianna 221, Elizabeth 391, Elizabeth 516, Jessica 461, Madison 352, Emma 499, Kayla 13, Emily 334, Alexis 498, Alexis 471, Brianna 172</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Lauren 309, Emily 144, Jessica 437, Taylor 523, Hannah 393, Emily 349, Emily 152, Grace 515, Elizabeth 157, Lauren 170</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1240,8 +1520,16 @@
           <t>Fotograafia 1</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
-      <c r="O74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Isabella 160, Emily 445, Alexis 35, Abigail 413, Jessica 506, Lauren 96, Alyssa 308, Taylor 226, Lauren 49, Lauren 475, Brianna 153, Hannah 181, Jessica 520, Hannah 314, Ashley 481, Samantha 20, Alexis 355, Sarah 501, Abigail 231, Abigail 341, Lauren 459, Grace 431, Kayla 235, Jessica 325</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>Grace 22, Emma 185, Emma 9, Kayla 497, Olivia 134, Olivia 138, Elizabeth 227, Samantha 480, Alexis 371, Jessica 425</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1249,8 +1537,16 @@
           <t>Inimene ja ühiskond 3. periood</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
-      <c r="O75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Madison 126, Elizabeth 391, Olivia 137, Abigail 338, Jessica 423, Jessica 383, Taylor 192, Taylor 121, Samantha 487, Emma 64, Lauren 56, Ashley 389, Emily 91, Grace 320, Taylor 94, Jessica 265, Jessica 163, Kayla 495, Emily 505, Jessica 230, Ashley 392, Kayla 272, Lauren 258, Ashley 81, Kayla 369, Emily 65, Emma 77, Samantha 488, Brianna 299, Grace 159, Emma 72, Alexis 261, Ashley 117, Ashley 283, Abigail 82, Grace 89</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Alyssa 366, Lauren 11, Lauren 49, Sarah 512, Alyssa 491, Madison 417, Alexis 524, Sarah 482, Lauren 337, Olivia 270</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1260,10 +1556,14 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Lauren 12</t>
-        </is>
-      </c>
-      <c r="O76" t="inlineStr"/>
+          <t>Madison 24, Lauren 12, Taylor 222, Emma 25, Jessica 32, Taylor 110, Emily 507, Isabella 275, Olivia 502, Elizabeth 313, Jessica 189, Emma 9, Elizabeth 289, Kayla 379, Madison 415, Brianna 197, Isabella 329, Madison 444, Brianna 179, Madison 196, Olivia 53, Grace 280, Madison 417, Elizabeth 227, Isabella 95, Alexis 371, Samantha 462, Samantha 382, Alyssa 440, Abigail 209, Hannah 194, Sarah 424, Kayla 51, Emily 34, Olivia 318, Lauren 236</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Alyssa 493, Emily 146, Alexis 343, Emma 76, Elizabeth 307, Ashley 198, Elizabeth 364, Brianna 456, Madison 155, Alexis 498</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1273,10 +1573,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Isabella 3</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr"/>
+          <t>Kayla 407, Jessica 278, Abigail 269, Alyssa 359, Lauren 90, Ashley 140, Taylor 394, Olivia 239, Alexis 80, Grace 122, Abigail 125, Samantha 276, Olivia 38, Grace 515, Sarah 442, Sarah 57, Kayla 469, Brianna 419, Isabella 242, Brianna 251, Alyssa 128, Alyssa 245, Lauren 136, Kayla 410, Grace 213, Sarah 482, Lauren 358, Madison 225, Brianna 438, Madison 162</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Sarah 107, Abigail 450, Olivia 40, Isabella 3, Alyssa 304, Lauren 29, Hannah 317, Emily 390, Sarah 312, Alexis 470</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1286,10 +1590,14 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Lauren 12, Kayla 15, Elizabeth 10, Lauren 11</t>
-        </is>
-      </c>
-      <c r="O78" t="inlineStr"/>
+          <t>Isabella 395, Sarah 400, Abigail 413, Sarah 31, Kayla 252, Lauren 457, Lauren 12, Taylor 254, Jessica 506, Alexis 378, Isabella 426, Brianna 221, Elizabeth 391, Elizabeth 476, Abigail 338, Kayla 15, Jessica 46, Alexis 316, Lauren 475, Samantha 27, Brianna 153, Jessica 437, Lauren 223, Hannah 266, Emily 91, Ashley 458, Taylor 500, Sarah 315, Abigail 291, Emma 404</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Madison 519, Grace 321, Kayla 75, Lauren 310, Abigail 231, Sarah 277, Grace 267, Sarah 57, Emma 55, Emma 300</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1297,8 +1605,16 @@
           <t>Turundus</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
-      <c r="O79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Lauren 232, Brianna 88, Ashley 240, Lauren 33, Brianna 221, Olivia 259, Jessica 461, Alyssa 39, Hannah 59, Lauren 52, Ashley 348, Alyssa 432, Abigail 71, Abigail 503, Emma 76, Madison 155, Emily 390, Jessica 311, Grace 411, Alexis 470, Alyssa 421, Taylor 130, Samantha 398, Madison 301, Ashley 220, Ashley 168</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Lauren 346, Emma 305, Emily 97, Elizabeth 227, Hannah 317, Samantha 484, Madison 415, Alexis 355, Abigail 341, Abigail 125</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1308,10 +1624,14 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Kayla 13, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O80" t="inlineStr"/>
+          <t>Grace 396, Olivia 274, Elizabeth 449, Elizabeth 476, Sarah 518, Kayla 13, Sarah 74, Sarah 331, Lauren 85, Emma 257, Alexis 45, Samantha 73, Lauren 489, Madison 519, Abigail 109, Madison 184, Jessica 147, Alexis 468, Grace 120, Emily 439, Brianna 362, Hannah 281, Lauren 356, Samantha 68</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Madison 322, Elizabeth 399, Emily 333, Grace 428, Hannah 332, Taylor 17, Samantha 250, Elizabeth 284, Samantha 298, Abigail 517</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1321,10 +1641,14 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Lauren 12, Kayla 15, Elizabeth 10, Lauren 11, Isabella 3</t>
-        </is>
-      </c>
-      <c r="O81" t="inlineStr"/>
+          <t>Grace 199, Lauren 248, Isabella 395, Alyssa 508, Hannah 202, Lauren 12, Taylor 222, Isabella 426, Elizabeth 449, Kayla 15, Emma 118, Taylor 226, Elizabeth 486, Emma 25, Abigail 408, Abigail 108, Lauren 85, Grace 100, Jessica 437, Jessica 293</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Alexis 343, Olivia 239, Lauren 310, Sarah 501, Kayla 495, Samantha 276, Grace 267, Madison 455, Jessica 325, Brianna 362</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1332,8 +1656,16 @@
           <t>Kujutav geomeetria</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="O82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Taylor 288, Taylor 509, Emma 98, Sarah 400, Kayla 252, Ashley 478, Madison 173, Alyssa 273, Isabella 354, Hannah 59, Ashley 453, Hannah 181, Emma 257, Elizabeth 328, Abigail 113, Lauren 372, Jessica 374, Olivia 186, Kayla 75, Brianna 190, Jessica 163, Abigail 125</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Abigail 406, Emma 300, Emily 34, Kayla 235, Olivia 270, Ashley 81, Abigail 209, Olivia 502, Samantha 447, Elizabeth 289</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1341,7 +1673,11 @@
           <t>Loominguline joonistamine 2</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Alexis 381, Samantha 302</t>
+        </is>
+      </c>
       <c r="O83" t="inlineStr"/>
     </row>
     <row r="84">
@@ -1352,10 +1688,14 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Kayla 13, Taylor 6, Madison 14</t>
-        </is>
-      </c>
-      <c r="O84" t="inlineStr"/>
+          <t>Madison 24, Jessica 206, Grace 285, Sarah 210, Jessica 66, Kayla 13, Hannah 323, Ashley 348, Taylor 115, Lauren 309, Emily 229, Lauren 56, Ashley 458, Isabella 353, Abigail 291, Samantha 73, Taylor 523, Emily 403, Taylor 94, Lauren 249, Grace 83, Kayla 409, Abigail 231, Brianna 180, Isabella 161, Brianna 200, Olivia 169, Sarah 57, Isabella 260, Madison 322, Abigail 279, Olivia 127, Samantha 488, Grace 159, Emma 72</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Elizabeth 284, Hannah 287, Alexis 36, Hannah 317, Ashley 392, Sarah 512, Emma 9, Alyssa 491, Ashley 50, Brianna 92</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1365,10 +1705,14 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Kayla 13, Kayla 7, Lauren 11</t>
-        </is>
-      </c>
-      <c r="O85" t="inlineStr"/>
+          <t>Grace 99, Grace 396, Alexis 370, Lauren 457, Jessica 278, Lauren 96, Elizabeth 391, Alyssa 359, Jessica 423, Alyssa 273, Sarah 210, Emma 28, Hannah 397, Kayla 13, Ashley 123, Samantha 429, Taylor 115, Lauren 60, Hannah 181, Samantha 73, Lauren 372, Emily 403, Hannah 314, Olivia 234, Emma 217, Jessica 265, Samantha 224, Abigail 177, Sarah 501, Lauren 459, Abigail 71, Grace 515, Alyssa 440, Alyssa 380, Ashley 297, Abigail 279</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Alexis 470, Kayla 7, Brianna 299, Elizabeth 164, Alyssa 245, Olivia 477, Sarah 86, Grace 89, Alexis 261, Elizabeth 284</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1378,10 +1722,14 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Lauren 8, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O86" t="inlineStr"/>
+          <t>Lauren 232, Alyssa 435, Brianna 221, Lauren 8, Elizabeth 476, Lauren 90, Abigail 408, Hannah 194, Emily 334, Emma 401, Samantha 487, Emily 405, Elizabeth 328, Sarah 156, Jessica 520</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Taylor 523, Olivia 124, Isabella 295, Olivia 239, Grace 321, Brianna 190, Jessica 303, Taylor 158, Sarah 277, Grace 256</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1391,10 +1739,14 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Sarah 2, Madison 14</t>
-        </is>
-      </c>
-      <c r="O87" t="inlineStr"/>
+          <t>Isabella 160, Emily 445, Brianna 433, Sarah 2, Olivia 137, Abigail 269, Abigail 338, Samantha 402, Abigail 212, Brianna 153, Samantha 143, Madison 14, Madison 519, Taylor 94, Jessica 219, Grace 122, Lauren 310, Ashley 246, Abigail 109, Emily 34, Isabella 260, Emily 439, Jessica 311, Brianna 251</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Alyssa 128, Brianna 42, Alyssa 421, Taylor 130, Brianna 513, Sarah 482, Madison 301, Emma 387, Abigail 517, Alyssa 339</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1404,10 +1756,14 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Kayla 5</t>
-        </is>
-      </c>
-      <c r="O88" t="inlineStr"/>
+          <t>Olivia 103, Alyssa 493, Emily 146, Taylor 226, Ashley 50, Hannah 218, Hannah 467, Emma 290, Kayla 5, Hannah 129, Alexis 340, Grace 282, Olivia 186, Emily 152, Kayla 495, Ashley 392, Olivia 169, Samantha 386, Emma 448, Kayla 469, Isabella 474, Hannah 357, Emma 185, Emily 65, Ashley 414, Hannah 119, Abigail 255, Samantha 327, Samantha 150, Elizabeth 473, Ashley 117, Ashley 168, Hannah 287, Lauren 346, Emma 305, Elizabeth 10, Lauren 101, Elizabeth 364, Brianna 172, Samantha 480, Hannah 317, Brianna 492, Sarah 114, Brianna 205, Brianna 47, Isabella 161, Olivia 138, Kayla 497, Abigail 82, Brianna 299, Elizabeth 164, Kayla 409, Emily 479, Sarah 86, Samantha 18, Sarah 518, Alexis 294, Emily 135, Lauren 207, Olivia 264, Taylor 176, Emma 216, Kayla 272, Emma 72, Abigail 344, Alyssa 245, Madison 225, Grace 159, Isabella 347, Kayla 410, Elizabeth 116, Emily 336, Brianna 419, Sarah 420, Jessica 325, Hannah 332, Abigail 517, Alyssa 39, Samantha 298, Brianna 513</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Kayla 13, Lauren 367, Emma 217, Olivia 169, Abigail 413, Emily 405, Olivia 137, Grace 511, Alexis 36, Elizabeth 284</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1415,7 +1771,11 @@
           <t>Riigikaitse 2</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Taylor 226, Hannah 218, Olivia 169, Samantha 386, Samantha 150, Elizabeth 364, Ashley 392, Brianna 47, Ashley 414, Emma 185, Lauren 346, Alexis 294, Hannah 119, Emily 152, Elizabeth 10, Olivia 138, Sarah 420, Ashley 50, Emily 135, Elizabeth 116, Abigail 344, Hannah 467, Kayla 272</t>
+        </is>
+      </c>
       <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
@@ -1426,10 +1786,14 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Hannah 16, Isabella 3</t>
-        </is>
-      </c>
-      <c r="O90" t="inlineStr"/>
+          <t>Kayla 407, Olivia 345, Brianna 88, Abigail 413, Lauren 33, Olivia 274, Madison 173, Alyssa 308, Jessica 46, Isabella 183, Taylor 121, Hannah 59, Lauren 52, Taylor 106, Alexis 498, Alyssa 306, Emily 229, Jessica 175, Emily 91, Brianna 92, Taylor 26, Hannah 16, Ashley 286, Alexis 69, Ashley 441</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Taylor 394, Alyssa 432, Hannah 393, Ashley 326, Lauren 249, Alexis 294, Kayla 409, Brianna 456, Olivia 496, Brianna 200</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1437,7 +1801,11 @@
           <t>Ajakirjanduse praktika</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Emily 330, Ashley 460, Jessica 23, Emily 229, Jessica 70, Samantha 73, Taylor 523, Isabella 375, Brianna 190, Sarah 501, Abigail 255, Lauren 309, Isabella 161, Jessica 189, Samantha 488, Emma 76, Emily 334, Brianna 200, Jessica 175, Emma 257, Samantha 143, Kayla 13, Emily 403, Kayla 409</t>
+        </is>
+      </c>
       <c r="O91" t="inlineStr"/>
     </row>
     <row r="92">
@@ -1448,10 +1816,14 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Taylor 6, Kayla 13</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr"/>
+          <t>Grace 199, Taylor 288, Isabella 241, Alexis 35, Alexis 370, Jessica 278, Brianna 201, Taylor 222, Alyssa 359, Elizabeth 436, Jessica 461, Isabella 342, Abigail 490, Lauren 90, Madison 54, Elizabeth 174, Hannah 397, Taylor 6, Hannah 522, Elizabeth 67, Hannah 323, Samantha 487, Olivia 41, Grace 463, Lauren 56, Ashley 140, Ashley 389, Hannah 181, Grace 48, Isabella 353</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Alexis 340, Taylor 26, Olivia 124, Grace 263, Alexis 80, Lauren 249, Taylor 158, Madison 149, Grace 256, Isabella 161</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1461,10 +1833,14 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Sarah 2, Lauren 8</t>
-        </is>
-      </c>
-      <c r="O93" t="inlineStr"/>
+          <t>Emma 98, Kayla 407, Madison 126, Madison 24, Brianna 88, Hannah 202, Sarah 2, Olivia 103, Lauren 8, Alexis 171, Abigail 269, Alyssa 308, Grace 285, Sarah 210, Elizabeth 486, Alyssa 39, Alyssa 19, Taylor 192</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Taylor 121, Kayla 139, Emily 334, Samantha 429, Sarah 74, Alexis 471, Alexis 104, Jessica 191, Ashley 348, Lauren 60</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1474,10 +1850,14 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Olivia 1, Hannah 16, Emma 9, Kayla 7</t>
-        </is>
-      </c>
-      <c r="O94" t="inlineStr"/>
+          <t>Grace 99, Taylor 509, Olivia 345, Olivia 1, Alyssa 435, Olivia 416, Alyssa 132, Samantha 402, Emily 87, Alyssa 366, Samantha 271, Emma 118, Ashley 78, Alyssa 493, Emma 499, Jessica 383</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Ashley 123, Emily 228, Taylor 115, Grace 100, Abigail 296, Hannah 467, Brianna 92, Hannah 16, Lauren 337, Olivia 234</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1487,10 +1867,14 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Taylor 6, Lauren 8, Samantha 18, Madison 14, Taylor 17</t>
-        </is>
-      </c>
-      <c r="O95" t="inlineStr"/>
+          <t>Elizabeth 422, Sarah 377, Kayla 407, Isabella 241, Madison 24, Abigail 413, Sarah 31, Lauren 363, Emily 330, Brianna 221, Lauren 8, Ashley 478, Grace 285, Abigail 490, Emma 216, Alyssa 493, Taylor 226, Elizabeth 174, Taylor 6, Hannah 522</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Lauren 52, Olivia 504, Abigail 296, Grace 30, Ashley 140, Emily 91, Kayla 466, Jessica 520, Madison 14, Taylor 523</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1500,10 +1884,14 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Olivia 1, Samantha 18, Kayla 7</t>
-        </is>
-      </c>
-      <c r="O96" t="inlineStr"/>
+          <t>Taylor 151, Sarah 377, Alexis 35, Abigail 131, Olivia 1, Isabella 426, Emily 87, Ashley 460, Sarah 518, Emily 146, Lauren 49, Taylor 121, Hannah 522, Lauren 309, Elizabeth 116, Grace 30</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Hannah 181, Ashley 458, Taylor 500, Ashley 286, Lauren 430, Abigail 177, Grace 122, Grace 111, Alyssa 440, Emma 448</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1511,8 +1899,16 @@
           <t>Tänavakunst</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
-      <c r="O97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Grace 99, Taylor 509, Kayla 252, Ashley 240, Brianna 433, Samantha 211, Lauren 96, Alyssa 132, Isabella 342, Lauren 90, Emma 499, Elizabeth 486, Hannah 397, Abigail 408, Jessica 23, Sarah 331, Alexis 498, Alexis 104, Jessica 191, Lauren 309</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>Alyssa 306, Emily 229, Emily 144, Grace 463, Ashley 389, Emma 257, Grace 263, Olivia 239, Brianna 373, Jessica 32</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
praks registreerimine faili kirjutamine
</commit_message>
<xml_diff>
--- a/õpetajateFail.xlsx
+++ b/õpetajateFail.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,7 +635,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Jessica 2, Brianna 1</t>
+          <t>Brianna 1, Jessica 2</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Hannah 3, Brianna 1</t>
+          <t>Brianna 1, Hannah 3</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
@@ -1449,10 +1449,132 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Jessica 2, Hannah 3</t>
+          <t>Hannah 3, Jessica 2</t>
         </is>
       </c>
       <c r="O97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>PRAKTIKUMID:</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Geograafia</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Kirjandus</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Inglise keel</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Ökoloogia</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Koorilaul</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Brianna 1, Hannah 3, Lauren 4, Emma 5</t>
+        </is>
+      </c>
+      <c r="O103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Rahvatants</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Jessica 2, Emma 5, Lauren 4, Hannah 3</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Akvaristika</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Lauren 4, Emma 5</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Näitering</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Emma 5</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Mehhatroonika ja robootika</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Digitehnoloogiaga sõbraks</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Keskkonnaseire ja digilahendused</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>